<commit_message>
funciona correctamente las columnas de fechas
</commit_message>
<xml_diff>
--- a/importaciones_unificadas.xlsx
+++ b/importaciones_unificadas.xlsx
@@ -605,7 +605,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H2" t="inlineStr"/>
@@ -688,7 +688,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H3" t="inlineStr"/>
@@ -771,7 +771,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H4" t="inlineStr"/>
@@ -854,7 +854,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H5" t="inlineStr"/>
@@ -937,7 +937,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H6" t="inlineStr"/>
@@ -1020,7 +1020,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H7" t="inlineStr"/>
@@ -1099,11 +1099,11 @@
         <v>2025</v>
       </c>
       <c r="F8" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.02</t>
         </is>
       </c>
       <c r="H8" t="inlineStr"/>
@@ -1182,11 +1182,11 @@
         <v>2025</v>
       </c>
       <c r="F9" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.03</t>
         </is>
       </c>
       <c r="H9" t="inlineStr"/>
@@ -1265,11 +1265,11 @@
         <v>2025</v>
       </c>
       <c r="F10" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.03</t>
         </is>
       </c>
       <c r="H10" t="inlineStr"/>
@@ -1348,11 +1348,11 @@
         <v>2025</v>
       </c>
       <c r="F11" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.03</t>
         </is>
       </c>
       <c r="H11" t="inlineStr"/>
@@ -1431,11 +1431,11 @@
         <v>2025</v>
       </c>
       <c r="F12" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.03</t>
         </is>
       </c>
       <c r="H12" t="inlineStr"/>
@@ -1514,11 +1514,11 @@
         <v>2025</v>
       </c>
       <c r="F13" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.03</t>
         </is>
       </c>
       <c r="H13" t="inlineStr"/>
@@ -1597,11 +1597,11 @@
         <v>2025</v>
       </c>
       <c r="F14" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.03</t>
         </is>
       </c>
       <c r="H14" t="inlineStr"/>
@@ -1680,11 +1680,11 @@
         <v>2025</v>
       </c>
       <c r="F15" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H15" t="inlineStr"/>
@@ -1763,11 +1763,11 @@
         <v>2025</v>
       </c>
       <c r="F16" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H16" t="inlineStr"/>
@@ -1846,11 +1846,11 @@
         <v>2025</v>
       </c>
       <c r="F17" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H17" t="inlineStr"/>
@@ -1929,11 +1929,11 @@
         <v>2025</v>
       </c>
       <c r="F18" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H18" t="inlineStr"/>
@@ -2012,11 +2012,11 @@
         <v>2025</v>
       </c>
       <c r="F19" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H19" t="inlineStr"/>
@@ -2095,11 +2095,11 @@
         <v>2025</v>
       </c>
       <c r="F20" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H20" t="inlineStr"/>
@@ -2178,11 +2178,11 @@
         <v>2025</v>
       </c>
       <c r="F21" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H21" t="inlineStr"/>
@@ -2261,11 +2261,11 @@
         <v>2025</v>
       </c>
       <c r="F22" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H22" t="inlineStr"/>
@@ -2344,11 +2344,11 @@
         <v>2025</v>
       </c>
       <c r="F23" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H23" t="inlineStr"/>
@@ -2427,11 +2427,11 @@
         <v>2025</v>
       </c>
       <c r="F24" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H24" t="inlineStr"/>
@@ -2510,11 +2510,11 @@
         <v>2025</v>
       </c>
       <c r="F25" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H25" t="inlineStr"/>
@@ -2593,11 +2593,11 @@
         <v>2025</v>
       </c>
       <c r="F26" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.06</t>
         </is>
       </c>
       <c r="H26" t="inlineStr"/>
@@ -2680,7 +2680,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H27" t="inlineStr"/>
@@ -2763,7 +2763,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H28" t="inlineStr"/>
@@ -2846,7 +2846,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H29" t="inlineStr"/>
@@ -2925,11 +2925,11 @@
         <v>2025</v>
       </c>
       <c r="F30" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.03</t>
         </is>
       </c>
       <c r="H30" t="inlineStr"/>
@@ -3008,11 +3008,11 @@
         <v>2025</v>
       </c>
       <c r="F31" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.03</t>
         </is>
       </c>
       <c r="H31" t="inlineStr"/>
@@ -3091,11 +3091,11 @@
         <v>2025</v>
       </c>
       <c r="F32" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H32" t="inlineStr"/>
@@ -3174,11 +3174,11 @@
         <v>2025</v>
       </c>
       <c r="F33" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.06</t>
         </is>
       </c>
       <c r="H33" t="inlineStr"/>
@@ -3257,11 +3257,11 @@
         <v>2025</v>
       </c>
       <c r="F34" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H34" t="inlineStr"/>
@@ -3344,7 +3344,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H35" t="inlineStr"/>
@@ -3427,7 +3427,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H36" t="inlineStr"/>
@@ -3510,7 +3510,7 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H37" t="inlineStr"/>
@@ -3589,11 +3589,11 @@
         <v>2025</v>
       </c>
       <c r="F38" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.03</t>
         </is>
       </c>
       <c r="H38" t="inlineStr"/>
@@ -3672,11 +3672,11 @@
         <v>2025</v>
       </c>
       <c r="F39" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H39" t="inlineStr"/>
@@ -3755,11 +3755,11 @@
         <v>2025</v>
       </c>
       <c r="F40" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H40" t="inlineStr"/>
@@ -3842,7 +3842,7 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H41" t="inlineStr"/>
@@ -3921,11 +3921,11 @@
         <v>2025</v>
       </c>
       <c r="F42" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.02</t>
         </is>
       </c>
       <c r="H42" t="inlineStr"/>
@@ -4004,11 +4004,11 @@
         <v>2025</v>
       </c>
       <c r="F43" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.02</t>
         </is>
       </c>
       <c r="H43" t="inlineStr"/>
@@ -4087,11 +4087,11 @@
         <v>2025</v>
       </c>
       <c r="F44" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.03</t>
         </is>
       </c>
       <c r="H44" t="inlineStr"/>
@@ -4170,11 +4170,11 @@
         <v>2025</v>
       </c>
       <c r="F45" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H45" t="inlineStr"/>
@@ -4253,11 +4253,11 @@
         <v>2025</v>
       </c>
       <c r="F46" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.06</t>
         </is>
       </c>
       <c r="H46" t="inlineStr"/>
@@ -4336,11 +4336,11 @@
         <v>2025</v>
       </c>
       <c r="F47" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H47" t="inlineStr"/>
@@ -4419,11 +4419,11 @@
         <v>2025</v>
       </c>
       <c r="F48" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G48" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.02</t>
         </is>
       </c>
       <c r="H48" t="inlineStr"/>
@@ -4502,11 +4502,11 @@
         <v>2025</v>
       </c>
       <c r="F49" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G49" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H49" t="inlineStr"/>
@@ -4585,11 +4585,11 @@
         <v>2025</v>
       </c>
       <c r="F50" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G50" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H50" t="inlineStr"/>
@@ -4668,11 +4668,11 @@
         <v>2025</v>
       </c>
       <c r="F51" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G51" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H51" t="inlineStr"/>
@@ -4751,11 +4751,11 @@
         <v>2025</v>
       </c>
       <c r="F52" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G52" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H52" t="inlineStr"/>
@@ -4834,11 +4834,11 @@
         <v>2025</v>
       </c>
       <c r="F53" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G53" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H53" t="inlineStr"/>
@@ -4917,11 +4917,11 @@
         <v>2025</v>
       </c>
       <c r="F54" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G54" t="inlineStr">
         <is>
-          <t>2025.0.2.0</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H54" t="inlineStr"/>
@@ -5002,11 +5002,11 @@
         <v>2025</v>
       </c>
       <c r="F55" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G55" t="inlineStr">
         <is>
-          <t>2025.0.7.0</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H55" t="inlineStr"/>
@@ -5087,11 +5087,11 @@
         <v>2025</v>
       </c>
       <c r="F56" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G56" t="inlineStr">
         <is>
-          <t>2025.0.8.0</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H56" t="inlineStr"/>
@@ -5172,11 +5172,11 @@
         <v>2025</v>
       </c>
       <c r="F57" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="G57" t="inlineStr">
         <is>
-          <t>2025.0.10.0</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H57" t="inlineStr"/>
@@ -5253,11 +5253,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E58" t="inlineStr"/>
-      <c r="F58" t="inlineStr"/>
+      <c r="E58" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F58" t="n">
+        <v>1</v>
+      </c>
       <c r="G58" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H58" t="inlineStr"/>
@@ -5334,11 +5338,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E59" t="inlineStr"/>
-      <c r="F59" t="inlineStr"/>
+      <c r="E59" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F59" t="n">
+        <v>1</v>
+      </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H59" t="inlineStr"/>
@@ -5415,11 +5423,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E60" t="inlineStr"/>
-      <c r="F60" t="inlineStr"/>
+      <c r="E60" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F60" t="n">
+        <v>1</v>
+      </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H60" t="inlineStr"/>
@@ -5496,11 +5508,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E61" t="inlineStr"/>
-      <c r="F61" t="inlineStr"/>
+      <c r="E61" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F61" t="n">
+        <v>1</v>
+      </c>
       <c r="G61" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H61" t="inlineStr"/>
@@ -5577,11 +5593,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E62" t="inlineStr"/>
-      <c r="F62" t="inlineStr"/>
+      <c r="E62" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F62" t="n">
+        <v>1</v>
+      </c>
       <c r="G62" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H62" t="inlineStr"/>
@@ -5658,11 +5678,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E63" t="inlineStr"/>
-      <c r="F63" t="inlineStr"/>
+      <c r="E63" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F63" t="n">
+        <v>1</v>
+      </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H63" t="inlineStr"/>
@@ -5739,11 +5763,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E64" t="inlineStr"/>
-      <c r="F64" t="inlineStr"/>
+      <c r="E64" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F64" t="n">
+        <v>1</v>
+      </c>
       <c r="G64" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H64" t="inlineStr"/>
@@ -5824,11 +5852,11 @@
         <v>2025</v>
       </c>
       <c r="F65" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G65" t="inlineStr">
         <is>
-          <t>2025.0.6.0</t>
+          <t>2025.02</t>
         </is>
       </c>
       <c r="H65" t="inlineStr"/>
@@ -5909,11 +5937,11 @@
         <v>2025</v>
       </c>
       <c r="F66" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G66" t="inlineStr">
         <is>
-          <t>2025.0.6.0</t>
+          <t>2025.02</t>
         </is>
       </c>
       <c r="H66" t="inlineStr"/>
@@ -5990,11 +6018,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E67" t="inlineStr"/>
-      <c r="F67" t="inlineStr"/>
+      <c r="E67" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F67" t="n">
+        <v>2</v>
+      </c>
       <c r="G67" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.02</t>
         </is>
       </c>
       <c r="H67" t="inlineStr"/>
@@ -6071,11 +6103,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E68" t="inlineStr"/>
-      <c r="F68" t="inlineStr"/>
+      <c r="E68" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F68" t="n">
+        <v>2</v>
+      </c>
       <c r="G68" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.02</t>
         </is>
       </c>
       <c r="H68" t="inlineStr"/>
@@ -6152,11 +6188,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E69" t="inlineStr"/>
-      <c r="F69" t="inlineStr"/>
+      <c r="E69" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F69" t="n">
+        <v>3</v>
+      </c>
       <c r="G69" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.03</t>
         </is>
       </c>
       <c r="H69" t="inlineStr"/>
@@ -6237,11 +6277,11 @@
         <v>2025</v>
       </c>
       <c r="F70" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G70" t="inlineStr">
         <is>
-          <t>2025.0.2.0</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H70" t="inlineStr"/>
@@ -6326,7 +6366,7 @@
       </c>
       <c r="G71" t="inlineStr">
         <is>
-          <t>2025.0.4.0</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H71" t="inlineStr"/>
@@ -6407,11 +6447,11 @@
         <v>2025</v>
       </c>
       <c r="F72" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G72" t="inlineStr">
         <is>
-          <t>2025.0.7.0</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H72" t="inlineStr"/>
@@ -6488,11 +6528,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E73" t="inlineStr"/>
-      <c r="F73" t="inlineStr"/>
+      <c r="E73" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F73" t="n">
+        <v>4</v>
+      </c>
       <c r="G73" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H73" t="inlineStr"/>
@@ -6569,11 +6613,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E74" t="inlineStr"/>
-      <c r="F74" t="inlineStr"/>
+      <c r="E74" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F74" t="n">
+        <v>4</v>
+      </c>
       <c r="G74" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H74" t="inlineStr"/>
@@ -6650,11 +6698,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E75" t="inlineStr"/>
-      <c r="F75" t="inlineStr"/>
+      <c r="E75" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F75" t="n">
+        <v>4</v>
+      </c>
       <c r="G75" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H75" t="inlineStr"/>
@@ -6731,11 +6783,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E76" t="inlineStr"/>
-      <c r="F76" t="inlineStr"/>
+      <c r="E76" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F76" t="n">
+        <v>4</v>
+      </c>
       <c r="G76" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H76" t="inlineStr"/>
@@ -6812,11 +6868,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E77" t="inlineStr"/>
-      <c r="F77" t="inlineStr"/>
+      <c r="E77" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F77" t="n">
+        <v>4</v>
+      </c>
       <c r="G77" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H77" t="inlineStr"/>
@@ -6893,11 +6953,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E78" t="inlineStr"/>
-      <c r="F78" t="inlineStr"/>
+      <c r="E78" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F78" t="n">
+        <v>4</v>
+      </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H78" t="inlineStr"/>
@@ -6974,11 +7038,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E79" t="inlineStr"/>
-      <c r="F79" t="inlineStr"/>
+      <c r="E79" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F79" t="n">
+        <v>4</v>
+      </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H79" t="inlineStr"/>
@@ -7055,11 +7123,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E80" t="inlineStr"/>
-      <c r="F80" t="inlineStr"/>
+      <c r="E80" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F80" t="n">
+        <v>4</v>
+      </c>
       <c r="G80" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H80" t="inlineStr"/>
@@ -7136,11 +7208,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E81" t="inlineStr"/>
-      <c r="F81" t="inlineStr"/>
+      <c r="E81" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F81" t="n">
+        <v>4</v>
+      </c>
       <c r="G81" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H81" t="inlineStr"/>
@@ -7217,11 +7293,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E82" t="inlineStr"/>
-      <c r="F82" t="inlineStr"/>
+      <c r="E82" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F82" t="n">
+        <v>4</v>
+      </c>
       <c r="G82" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H82" t="inlineStr"/>
@@ -7302,11 +7382,11 @@
         <v>2025</v>
       </c>
       <c r="F83" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G83" t="inlineStr">
         <is>
-          <t>2025.0.7.0</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H83" t="inlineStr"/>
@@ -7387,11 +7467,11 @@
         <v>2025</v>
       </c>
       <c r="F84" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G84" t="inlineStr">
         <is>
-          <t>2025.0.7.0</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H84" t="inlineStr"/>
@@ -7472,11 +7552,11 @@
         <v>2025</v>
       </c>
       <c r="F85" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G85" t="inlineStr">
         <is>
-          <t>2025.0.9.0</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H85" t="inlineStr"/>
@@ -7557,11 +7637,11 @@
         <v>2025</v>
       </c>
       <c r="F86" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G86" t="inlineStr">
         <is>
-          <t>2025.0.9.0</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H86" t="inlineStr"/>
@@ -7642,11 +7722,11 @@
         <v>2025</v>
       </c>
       <c r="F87" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="G87" t="inlineStr">
         <is>
-          <t>2025.0.9.0</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H87" t="inlineStr"/>
@@ -7723,11 +7803,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E88" t="inlineStr"/>
-      <c r="F88" t="inlineStr"/>
+      <c r="E88" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F88" t="n">
+        <v>5</v>
+      </c>
       <c r="G88" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H88" t="inlineStr"/>
@@ -7804,11 +7888,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E89" t="inlineStr"/>
-      <c r="F89" t="inlineStr"/>
+      <c r="E89" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F89" t="n">
+        <v>5</v>
+      </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H89" t="inlineStr"/>
@@ -7885,11 +7973,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E90" t="inlineStr"/>
-      <c r="F90" t="inlineStr"/>
+      <c r="E90" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F90" t="n">
+        <v>5</v>
+      </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H90" t="inlineStr"/>
@@ -7966,11 +8058,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E91" t="inlineStr"/>
-      <c r="F91" t="inlineStr"/>
+      <c r="E91" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F91" t="n">
+        <v>5</v>
+      </c>
       <c r="G91" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H91" t="inlineStr"/>
@@ -8047,11 +8143,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E92" t="inlineStr"/>
-      <c r="F92" t="inlineStr"/>
+      <c r="E92" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F92" t="n">
+        <v>5</v>
+      </c>
       <c r="G92" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H92" t="inlineStr"/>
@@ -8132,11 +8232,11 @@
         <v>2025</v>
       </c>
       <c r="F93" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G93" t="inlineStr">
         <is>
-          <t>2025.0.2.0</t>
+          <t>2025.06</t>
         </is>
       </c>
       <c r="H93" t="inlineStr"/>
@@ -8217,11 +8317,11 @@
         <v>2025</v>
       </c>
       <c r="F94" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="G94" t="inlineStr">
         <is>
-          <t>2025.0.9.0</t>
+          <t>2025.06</t>
         </is>
       </c>
       <c r="H94" t="inlineStr"/>
@@ -8298,11 +8398,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E95" t="inlineStr"/>
-      <c r="F95" t="inlineStr"/>
+      <c r="E95" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F95" t="n">
+        <v>6</v>
+      </c>
       <c r="G95" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.06</t>
         </is>
       </c>
       <c r="H95" t="inlineStr"/>
@@ -8379,11 +8483,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E96" t="inlineStr"/>
-      <c r="F96" t="inlineStr"/>
+      <c r="E96" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F96" t="n">
+        <v>6</v>
+      </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.06</t>
         </is>
       </c>
       <c r="H96" t="inlineStr"/>
@@ -8460,11 +8568,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E97" t="inlineStr"/>
-      <c r="F97" t="inlineStr"/>
+      <c r="E97" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F97" t="n">
+        <v>6</v>
+      </c>
       <c r="G97" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.06</t>
         </is>
       </c>
       <c r="H97" t="inlineStr"/>
@@ -8541,11 +8653,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E98" t="inlineStr"/>
-      <c r="F98" t="inlineStr"/>
+      <c r="E98" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F98" t="n">
+        <v>6</v>
+      </c>
       <c r="G98" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.06</t>
         </is>
       </c>
       <c r="H98" t="inlineStr"/>
@@ -8622,11 +8738,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E99" t="inlineStr"/>
-      <c r="F99" t="inlineStr"/>
+      <c r="E99" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F99" t="n">
+        <v>6</v>
+      </c>
       <c r="G99" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.06</t>
         </is>
       </c>
       <c r="H99" t="inlineStr"/>
@@ -8711,7 +8831,7 @@
       </c>
       <c r="G100" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H100" t="inlineStr"/>
@@ -8796,7 +8916,7 @@
       </c>
       <c r="G101" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H101" t="inlineStr"/>
@@ -8881,7 +9001,7 @@
       </c>
       <c r="G102" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H102" t="inlineStr"/>
@@ -8966,7 +9086,7 @@
       </c>
       <c r="G103" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H103" t="inlineStr"/>
@@ -9051,7 +9171,7 @@
       </c>
       <c r="G104" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H104" t="inlineStr"/>
@@ -9136,7 +9256,7 @@
       </c>
       <c r="G105" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H105" t="inlineStr"/>
@@ -9217,11 +9337,11 @@
         <v>2025</v>
       </c>
       <c r="F106" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G106" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.02</t>
         </is>
       </c>
       <c r="H106" t="inlineStr"/>
@@ -9302,11 +9422,11 @@
         <v>2025</v>
       </c>
       <c r="F107" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G107" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.02</t>
         </is>
       </c>
       <c r="H107" t="inlineStr"/>
@@ -9387,11 +9507,11 @@
         <v>2025</v>
       </c>
       <c r="F108" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G108" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.02</t>
         </is>
       </c>
       <c r="H108" t="inlineStr"/>
@@ -9472,11 +9592,11 @@
         <v>2025</v>
       </c>
       <c r="F109" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G109" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.02</t>
         </is>
       </c>
       <c r="H109" t="inlineStr"/>
@@ -9557,11 +9677,11 @@
         <v>2025</v>
       </c>
       <c r="F110" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G110" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.02</t>
         </is>
       </c>
       <c r="H110" t="inlineStr"/>
@@ -9642,11 +9762,11 @@
         <v>2025</v>
       </c>
       <c r="F111" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G111" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.02</t>
         </is>
       </c>
       <c r="H111" t="inlineStr"/>
@@ -9727,11 +9847,11 @@
         <v>2025</v>
       </c>
       <c r="F112" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G112" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.02</t>
         </is>
       </c>
       <c r="H112" t="inlineStr"/>
@@ -9812,11 +9932,11 @@
         <v>2025</v>
       </c>
       <c r="F113" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G113" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.03</t>
         </is>
       </c>
       <c r="H113" t="inlineStr"/>
@@ -9897,11 +10017,11 @@
         <v>2025</v>
       </c>
       <c r="F114" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G114" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.03</t>
         </is>
       </c>
       <c r="H114" t="inlineStr"/>
@@ -9982,11 +10102,11 @@
         <v>2025</v>
       </c>
       <c r="F115" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G115" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.03</t>
         </is>
       </c>
       <c r="H115" t="inlineStr"/>
@@ -10067,11 +10187,11 @@
         <v>2025</v>
       </c>
       <c r="F116" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G116" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.03</t>
         </is>
       </c>
       <c r="H116" t="inlineStr"/>
@@ -10152,11 +10272,11 @@
         <v>2025</v>
       </c>
       <c r="F117" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G117" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.03</t>
         </is>
       </c>
       <c r="H117" t="inlineStr"/>
@@ -10237,11 +10357,11 @@
         <v>2025</v>
       </c>
       <c r="F118" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G118" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H118" t="inlineStr"/>
@@ -10322,11 +10442,11 @@
         <v>2025</v>
       </c>
       <c r="F119" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G119" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H119" t="inlineStr"/>
@@ -10407,11 +10527,11 @@
         <v>2025</v>
       </c>
       <c r="F120" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G120" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H120" t="inlineStr"/>
@@ -10492,11 +10612,11 @@
         <v>2025</v>
       </c>
       <c r="F121" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G121" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H121" t="inlineStr"/>
@@ -10577,11 +10697,11 @@
         <v>2025</v>
       </c>
       <c r="F122" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G122" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H122" t="inlineStr"/>
@@ -10662,11 +10782,11 @@
         <v>2025</v>
       </c>
       <c r="F123" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G123" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H123" t="inlineStr"/>
@@ -10747,11 +10867,11 @@
         <v>2025</v>
       </c>
       <c r="F124" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G124" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H124" t="inlineStr"/>
@@ -10832,11 +10952,11 @@
         <v>2025</v>
       </c>
       <c r="F125" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G125" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H125" t="inlineStr"/>
@@ -10917,11 +11037,11 @@
         <v>2025</v>
       </c>
       <c r="F126" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G126" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H126" t="inlineStr"/>
@@ -11002,11 +11122,11 @@
         <v>2025</v>
       </c>
       <c r="F127" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G127" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H127" t="inlineStr"/>
@@ -11087,11 +11207,11 @@
         <v>2025</v>
       </c>
       <c r="F128" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G128" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H128" t="inlineStr"/>
@@ -11172,11 +11292,11 @@
         <v>2025</v>
       </c>
       <c r="F129" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G129" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H129" t="inlineStr"/>
@@ -11257,11 +11377,11 @@
         <v>2025</v>
       </c>
       <c r="F130" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G130" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H130" t="inlineStr"/>
@@ -11342,11 +11462,11 @@
         <v>2025</v>
       </c>
       <c r="F131" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G131" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H131" t="inlineStr"/>
@@ -11427,11 +11547,11 @@
         <v>2025</v>
       </c>
       <c r="F132" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G132" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.06</t>
         </is>
       </c>
       <c r="H132" t="inlineStr"/>
@@ -11512,11 +11632,11 @@
         <v>2025</v>
       </c>
       <c r="F133" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G133" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.06</t>
         </is>
       </c>
       <c r="H133" t="inlineStr"/>
@@ -11597,11 +11717,11 @@
         <v>2025</v>
       </c>
       <c r="F134" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G134" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.06</t>
         </is>
       </c>
       <c r="H134" t="inlineStr"/>
@@ -11682,11 +11802,11 @@
         <v>2025</v>
       </c>
       <c r="F135" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G135" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.06</t>
         </is>
       </c>
       <c r="H135" t="inlineStr"/>
@@ -11767,11 +11887,11 @@
         <v>2025</v>
       </c>
       <c r="F136" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G136" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.06</t>
         </is>
       </c>
       <c r="H136" t="inlineStr"/>
@@ -11852,11 +11972,11 @@
         <v>2025</v>
       </c>
       <c r="F137" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G137" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.06</t>
         </is>
       </c>
       <c r="H137" t="inlineStr"/>
@@ -11937,11 +12057,11 @@
         <v>2025</v>
       </c>
       <c r="F138" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="G138" t="inlineStr">
         <is>
-          <t>2025.0.9.0</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H138" t="n">
@@ -12038,11 +12158,11 @@
         <v>2025</v>
       </c>
       <c r="F139" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="G139" t="inlineStr">
         <is>
-          <t>2025.0.9.0</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H139" t="n">
@@ -12135,11 +12255,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E140" t="inlineStr"/>
-      <c r="F140" t="inlineStr"/>
+      <c r="E140" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F140" t="n">
+        <v>1</v>
+      </c>
       <c r="G140" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H140" t="n">
@@ -12232,11 +12356,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E141" t="inlineStr"/>
-      <c r="F141" t="inlineStr"/>
+      <c r="E141" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F141" t="n">
+        <v>1</v>
+      </c>
       <c r="G141" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H141" t="n">
@@ -12329,11 +12457,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E142" t="inlineStr"/>
-      <c r="F142" t="inlineStr"/>
+      <c r="E142" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F142" t="n">
+        <v>1</v>
+      </c>
       <c r="G142" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H142" t="n">
@@ -12430,11 +12562,11 @@
         <v>2025</v>
       </c>
       <c r="F143" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G143" t="inlineStr">
         <is>
-          <t>2025.0.7.0</t>
+          <t>2025.02</t>
         </is>
       </c>
       <c r="H143" t="n">
@@ -12531,11 +12663,11 @@
         <v>2025</v>
       </c>
       <c r="F144" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G144" t="inlineStr">
         <is>
-          <t>2025.0.8.0</t>
+          <t>2025.02</t>
         </is>
       </c>
       <c r="H144" t="n">
@@ -12632,11 +12764,11 @@
         <v>2025</v>
       </c>
       <c r="F145" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="G145" t="inlineStr">
         <is>
-          <t>2025.0.12.0</t>
+          <t>2025.02</t>
         </is>
       </c>
       <c r="H145" t="n">
@@ -12733,11 +12865,11 @@
         <v>2025</v>
       </c>
       <c r="F146" t="n">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G146" t="inlineStr">
         <is>
-          <t>2025.0.7.0</t>
+          <t>2025.03</t>
         </is>
       </c>
       <c r="H146" t="n">
@@ -12830,11 +12962,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E147" t="inlineStr"/>
-      <c r="F147" t="inlineStr"/>
+      <c r="E147" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F147" t="n">
+        <v>3</v>
+      </c>
       <c r="G147" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.03</t>
         </is>
       </c>
       <c r="H147" t="n">
@@ -12927,11 +13063,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E148" t="inlineStr"/>
-      <c r="F148" t="inlineStr"/>
+      <c r="E148" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F148" t="n">
+        <v>3</v>
+      </c>
       <c r="G148" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.03</t>
         </is>
       </c>
       <c r="H148" t="n">
@@ -13024,11 +13164,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E149" t="inlineStr"/>
-      <c r="F149" t="inlineStr"/>
+      <c r="E149" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F149" t="n">
+        <v>3</v>
+      </c>
       <c r="G149" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.03</t>
         </is>
       </c>
       <c r="H149" t="n">
@@ -13125,11 +13269,11 @@
         <v>2025</v>
       </c>
       <c r="F150" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G150" t="inlineStr">
         <is>
-          <t>2025.0.1.0</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H150" t="n">
@@ -13226,11 +13370,11 @@
         <v>2025</v>
       </c>
       <c r="F151" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G151" t="inlineStr">
         <is>
-          <t>2025.0.8.0</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H151" t="n">
@@ -13327,11 +13471,11 @@
         <v>2025</v>
       </c>
       <c r="F152" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="G152" t="inlineStr">
         <is>
-          <t>2025.0.11.0</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H152" t="n">
@@ -13424,11 +13568,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E153" t="inlineStr"/>
-      <c r="F153" t="inlineStr"/>
+      <c r="E153" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F153" t="n">
+        <v>4</v>
+      </c>
       <c r="G153" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H153" t="n">
@@ -13521,11 +13669,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E154" t="inlineStr"/>
-      <c r="F154" t="inlineStr"/>
+      <c r="E154" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F154" t="n">
+        <v>4</v>
+      </c>
       <c r="G154" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H154" t="n">
@@ -13618,11 +13770,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E155" t="inlineStr"/>
-      <c r="F155" t="inlineStr"/>
+      <c r="E155" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F155" t="n">
+        <v>4</v>
+      </c>
       <c r="G155" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H155" t="n">
@@ -13715,11 +13871,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E156" t="inlineStr"/>
-      <c r="F156" t="inlineStr"/>
+      <c r="E156" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F156" t="n">
+        <v>4</v>
+      </c>
       <c r="G156" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H156" t="n">
@@ -13812,11 +13972,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E157" t="inlineStr"/>
-      <c r="F157" t="inlineStr"/>
+      <c r="E157" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F157" t="n">
+        <v>4</v>
+      </c>
       <c r="G157" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H157" t="n">
@@ -13913,11 +14077,11 @@
         <v>2025</v>
       </c>
       <c r="F158" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G158" t="inlineStr">
         <is>
-          <t>2025.0.3.0</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H158" t="inlineStr"/>
@@ -14008,11 +14172,11 @@
         <v>2025</v>
       </c>
       <c r="F159" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G159" t="inlineStr">
         <is>
-          <t>2025.0.7.0</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H159" t="inlineStr"/>
@@ -14099,11 +14263,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E160" t="inlineStr"/>
-      <c r="F160" t="inlineStr"/>
+      <c r="E160" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F160" t="n">
+        <v>1</v>
+      </c>
       <c r="G160" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H160" t="inlineStr"/>
@@ -14190,11 +14358,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E161" t="inlineStr"/>
-      <c r="F161" t="inlineStr"/>
+      <c r="E161" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F161" t="n">
+        <v>1</v>
+      </c>
       <c r="G161" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H161" t="inlineStr"/>
@@ -14281,11 +14453,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E162" t="inlineStr"/>
-      <c r="F162" t="inlineStr"/>
+      <c r="E162" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F162" t="n">
+        <v>1</v>
+      </c>
       <c r="G162" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H162" t="inlineStr"/>
@@ -14372,11 +14548,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E163" t="inlineStr"/>
-      <c r="F163" t="inlineStr"/>
+      <c r="E163" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F163" t="n">
+        <v>1</v>
+      </c>
       <c r="G163" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H163" t="inlineStr"/>
@@ -14463,11 +14643,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E164" t="inlineStr"/>
-      <c r="F164" t="inlineStr"/>
+      <c r="E164" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F164" t="n">
+        <v>1</v>
+      </c>
       <c r="G164" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H164" t="inlineStr"/>
@@ -14558,11 +14742,11 @@
         <v>2025</v>
       </c>
       <c r="F165" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G165" t="inlineStr">
         <is>
-          <t>2025.0.6.0</t>
+          <t>2025.03</t>
         </is>
       </c>
       <c r="H165" t="inlineStr"/>
@@ -14649,11 +14833,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E166" t="inlineStr"/>
-      <c r="F166" t="inlineStr"/>
+      <c r="E166" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F166" t="n">
+        <v>3</v>
+      </c>
       <c r="G166" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.03</t>
         </is>
       </c>
       <c r="H166" t="inlineStr"/>
@@ -14740,11 +14928,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E167" t="inlineStr"/>
-      <c r="F167" t="inlineStr"/>
+      <c r="E167" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F167" t="n">
+        <v>3</v>
+      </c>
       <c r="G167" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.03</t>
         </is>
       </c>
       <c r="H167" t="inlineStr"/>
@@ -14831,11 +15023,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E168" t="inlineStr"/>
-      <c r="F168" t="inlineStr"/>
+      <c r="E168" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F168" t="n">
+        <v>3</v>
+      </c>
       <c r="G168" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.03</t>
         </is>
       </c>
       <c r="H168" t="inlineStr"/>
@@ -14922,11 +15118,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E169" t="inlineStr"/>
-      <c r="F169" t="inlineStr"/>
+      <c r="E169" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F169" t="n">
+        <v>3</v>
+      </c>
       <c r="G169" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.03</t>
         </is>
       </c>
       <c r="H169" t="inlineStr"/>
@@ -15017,11 +15217,11 @@
         <v>2025</v>
       </c>
       <c r="F170" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G170" t="inlineStr">
         <is>
-          <t>2025.0.6.0</t>
+          <t>2025.02</t>
         </is>
       </c>
       <c r="H170" t="inlineStr"/>
@@ -15112,11 +15312,11 @@
         <v>2025</v>
       </c>
       <c r="F171" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G171" t="inlineStr">
         <is>
-          <t>2025.0.5.0</t>
+          <t>2025.03</t>
         </is>
       </c>
       <c r="H171" t="inlineStr"/>
@@ -15203,11 +15403,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E172" t="inlineStr"/>
-      <c r="F172" t="inlineStr"/>
+      <c r="E172" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F172" t="n">
+        <v>3</v>
+      </c>
       <c r="G172" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.03</t>
         </is>
       </c>
       <c r="H172" t="inlineStr"/>
@@ -15294,11 +15498,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E173" t="inlineStr"/>
-      <c r="F173" t="inlineStr"/>
+      <c r="E173" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F173" t="n">
+        <v>3</v>
+      </c>
       <c r="G173" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.03</t>
         </is>
       </c>
       <c r="H173" t="inlineStr"/>
@@ -15393,7 +15601,7 @@
       </c>
       <c r="G174" t="inlineStr">
         <is>
-          <t>2025.0.4.0</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H174" t="inlineStr"/>
@@ -15480,11 +15688,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E175" t="inlineStr"/>
-      <c r="F175" t="inlineStr"/>
+      <c r="E175" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F175" t="n">
+        <v>4</v>
+      </c>
       <c r="G175" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H175" t="inlineStr"/>
@@ -15571,11 +15783,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E176" t="inlineStr"/>
-      <c r="F176" t="inlineStr"/>
+      <c r="E176" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F176" t="n">
+        <v>4</v>
+      </c>
       <c r="G176" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H176" t="inlineStr"/>
@@ -15662,11 +15878,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E177" t="inlineStr"/>
-      <c r="F177" t="inlineStr"/>
+      <c r="E177" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F177" t="n">
+        <v>4</v>
+      </c>
       <c r="G177" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H177" t="inlineStr"/>
@@ -15753,11 +15973,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E178" t="inlineStr"/>
-      <c r="F178" t="inlineStr"/>
+      <c r="E178" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F178" t="n">
+        <v>5</v>
+      </c>
       <c r="G178" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H178" t="inlineStr"/>
@@ -15844,11 +16068,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E179" t="inlineStr"/>
-      <c r="F179" t="inlineStr"/>
+      <c r="E179" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F179" t="n">
+        <v>5</v>
+      </c>
       <c r="G179" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H179" t="inlineStr"/>
@@ -15935,11 +16163,15 @@
           <t>Silicato de Sodio</t>
         </is>
       </c>
-      <c r="E180" t="inlineStr"/>
-      <c r="F180" t="inlineStr"/>
+      <c r="E180" t="n">
+        <v>2025</v>
+      </c>
+      <c r="F180" t="n">
+        <v>5</v>
+      </c>
       <c r="G180" t="inlineStr">
         <is>
-          <t>nan.nan</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H180" t="inlineStr"/>
@@ -16034,7 +16266,7 @@
       </c>
       <c r="G181" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H181" t="inlineStr">
@@ -16139,7 +16371,7 @@
       </c>
       <c r="G182" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H182" t="inlineStr">
@@ -16244,7 +16476,7 @@
       </c>
       <c r="G183" t="inlineStr">
         <is>
-          <t>2025.2</t>
+          <t>2025.02</t>
         </is>
       </c>
       <c r="H183" t="inlineStr">
@@ -16349,7 +16581,7 @@
       </c>
       <c r="G184" t="inlineStr">
         <is>
-          <t>2025.2</t>
+          <t>2025.02</t>
         </is>
       </c>
       <c r="H184" t="inlineStr">
@@ -16454,7 +16686,7 @@
       </c>
       <c r="G185" t="inlineStr">
         <is>
-          <t>2025.2</t>
+          <t>2025.02</t>
         </is>
       </c>
       <c r="H185" t="inlineStr">
@@ -16559,7 +16791,7 @@
       </c>
       <c r="G186" t="inlineStr">
         <is>
-          <t>2025.3</t>
+          <t>2025.03</t>
         </is>
       </c>
       <c r="H186" t="inlineStr">
@@ -16664,7 +16896,7 @@
       </c>
       <c r="G187" t="inlineStr">
         <is>
-          <t>2025.3</t>
+          <t>2025.03</t>
         </is>
       </c>
       <c r="H187" t="inlineStr">
@@ -16769,7 +17001,7 @@
       </c>
       <c r="G188" t="inlineStr">
         <is>
-          <t>2025.3</t>
+          <t>2025.03</t>
         </is>
       </c>
       <c r="H188" t="inlineStr">
@@ -16874,7 +17106,7 @@
       </c>
       <c r="G189" t="inlineStr">
         <is>
-          <t>2025.3</t>
+          <t>2025.03</t>
         </is>
       </c>
       <c r="H189" t="inlineStr">
@@ -16979,7 +17211,7 @@
       </c>
       <c r="G190" t="inlineStr">
         <is>
-          <t>2025.3</t>
+          <t>2025.03</t>
         </is>
       </c>
       <c r="H190" t="inlineStr">
@@ -17084,7 +17316,7 @@
       </c>
       <c r="G191" t="inlineStr">
         <is>
-          <t>2025.3</t>
+          <t>2025.03</t>
         </is>
       </c>
       <c r="H191" t="inlineStr">
@@ -17189,7 +17421,7 @@
       </c>
       <c r="G192" t="inlineStr">
         <is>
-          <t>2025.3</t>
+          <t>2025.03</t>
         </is>
       </c>
       <c r="H192" t="inlineStr">
@@ -17294,7 +17526,7 @@
       </c>
       <c r="G193" t="inlineStr">
         <is>
-          <t>2025.4</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H193" t="inlineStr">
@@ -17399,7 +17631,7 @@
       </c>
       <c r="G194" t="inlineStr">
         <is>
-          <t>2025.4</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H194" t="inlineStr">
@@ -17504,7 +17736,7 @@
       </c>
       <c r="G195" t="inlineStr">
         <is>
-          <t>2025.4</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H195" t="inlineStr">
@@ -17609,7 +17841,7 @@
       </c>
       <c r="G196" t="inlineStr">
         <is>
-          <t>2025.4</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H196" t="inlineStr">
@@ -17714,7 +17946,7 @@
       </c>
       <c r="G197" t="inlineStr">
         <is>
-          <t>2025.4</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H197" t="inlineStr">
@@ -17819,7 +18051,7 @@
       </c>
       <c r="G198" t="inlineStr">
         <is>
-          <t>2025.4</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H198" t="inlineStr">
@@ -17924,7 +18156,7 @@
       </c>
       <c r="G199" t="inlineStr">
         <is>
-          <t>2025.5</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H199" t="inlineStr">
@@ -18029,7 +18261,7 @@
       </c>
       <c r="G200" t="inlineStr">
         <is>
-          <t>2025.5</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H200" t="inlineStr">
@@ -18134,7 +18366,7 @@
       </c>
       <c r="G201" t="inlineStr">
         <is>
-          <t>2025.5</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H201" t="inlineStr">
@@ -18239,7 +18471,7 @@
       </c>
       <c r="G202" t="inlineStr">
         <is>
-          <t>2025.5</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H202" t="inlineStr">
@@ -18344,7 +18576,7 @@
       </c>
       <c r="G203" t="inlineStr">
         <is>
-          <t>2025.5</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H203" t="inlineStr">
@@ -18449,7 +18681,7 @@
       </c>
       <c r="G204" t="inlineStr">
         <is>
-          <t>2025.5</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H204" t="inlineStr">
@@ -18554,7 +18786,7 @@
       </c>
       <c r="G205" t="inlineStr">
         <is>
-          <t>2025.5</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H205" t="inlineStr">
@@ -18659,7 +18891,7 @@
       </c>
       <c r="G206" t="inlineStr">
         <is>
-          <t>2025.5</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H206" t="inlineStr">
@@ -18764,7 +18996,7 @@
       </c>
       <c r="G207" t="inlineStr">
         <is>
-          <t>2025.6</t>
+          <t>2025.06</t>
         </is>
       </c>
       <c r="H207" t="inlineStr">
@@ -18869,7 +19101,7 @@
       </c>
       <c r="G208" t="inlineStr">
         <is>
-          <t>2025.6</t>
+          <t>2025.06</t>
         </is>
       </c>
       <c r="H208" t="inlineStr">
@@ -18974,7 +19206,7 @@
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>2025.6</t>
+          <t>2025.06</t>
         </is>
       </c>
       <c r="H209" t="inlineStr">
@@ -19079,7 +19311,7 @@
       </c>
       <c r="G210" t="inlineStr">
         <is>
-          <t>2025.6</t>
+          <t>2025.06</t>
         </is>
       </c>
       <c r="H210" t="inlineStr">
@@ -19184,7 +19416,7 @@
       </c>
       <c r="G211" t="inlineStr">
         <is>
-          <t>2025.6</t>
+          <t>2025.06</t>
         </is>
       </c>
       <c r="H211" t="inlineStr">
@@ -19289,7 +19521,7 @@
       </c>
       <c r="G212" t="inlineStr">
         <is>
-          <t>2025.6</t>
+          <t>2025.06</t>
         </is>
       </c>
       <c r="H212" t="inlineStr">
@@ -19394,7 +19626,7 @@
       </c>
       <c r="G213" t="inlineStr">
         <is>
-          <t>2025.6</t>
+          <t>2025.06</t>
         </is>
       </c>
       <c r="H213" t="inlineStr">
@@ -19499,7 +19731,7 @@
       </c>
       <c r="G214" t="inlineStr">
         <is>
-          <t>2025.6</t>
+          <t>2025.06</t>
         </is>
       </c>
       <c r="H214" t="inlineStr">
@@ -19604,7 +19836,7 @@
       </c>
       <c r="G215" t="inlineStr">
         <is>
-          <t>2025.6</t>
+          <t>2025.06</t>
         </is>
       </c>
       <c r="H215" t="inlineStr">
@@ -19709,7 +19941,7 @@
       </c>
       <c r="G216" t="inlineStr">
         <is>
-          <t>2025.6</t>
+          <t>2025.06</t>
         </is>
       </c>
       <c r="H216" t="inlineStr">
@@ -19814,7 +20046,7 @@
       </c>
       <c r="G217" t="inlineStr">
         <is>
-          <t>2025.6</t>
+          <t>2025.06</t>
         </is>
       </c>
       <c r="H217" t="inlineStr">
@@ -19919,7 +20151,7 @@
       </c>
       <c r="G218" t="inlineStr">
         <is>
-          <t>2025.6</t>
+          <t>2025.06</t>
         </is>
       </c>
       <c r="H218" t="inlineStr">
@@ -20024,7 +20256,7 @@
       </c>
       <c r="G219" t="inlineStr">
         <is>
-          <t>2025.6</t>
+          <t>2025.06</t>
         </is>
       </c>
       <c r="H219" t="inlineStr">
@@ -20129,7 +20361,7 @@
       </c>
       <c r="G220" t="inlineStr">
         <is>
-          <t>2025.6</t>
+          <t>2025.06</t>
         </is>
       </c>
       <c r="H220" t="inlineStr">
@@ -20234,7 +20466,7 @@
       </c>
       <c r="G221" t="inlineStr">
         <is>
-          <t>2025.6</t>
+          <t>2025.06</t>
         </is>
       </c>
       <c r="H221" t="inlineStr">
@@ -20339,7 +20571,7 @@
       </c>
       <c r="G222" t="inlineStr">
         <is>
-          <t>2025.6</t>
+          <t>2025.06</t>
         </is>
       </c>
       <c r="H222" t="inlineStr">
@@ -20444,7 +20676,7 @@
       </c>
       <c r="G223" t="inlineStr">
         <is>
-          <t>2025.6</t>
+          <t>2025.06</t>
         </is>
       </c>
       <c r="H223" t="inlineStr">
@@ -20549,7 +20781,7 @@
       </c>
       <c r="G224" t="inlineStr">
         <is>
-          <t>2025.7</t>
+          <t>2025.07</t>
         </is>
       </c>
       <c r="H224" t="inlineStr">
@@ -20654,7 +20886,7 @@
       </c>
       <c r="G225" t="inlineStr">
         <is>
-          <t>2025.7</t>
+          <t>2025.07</t>
         </is>
       </c>
       <c r="H225" t="inlineStr">
@@ -20759,7 +20991,7 @@
       </c>
       <c r="G226" t="inlineStr">
         <is>
-          <t>2025.7</t>
+          <t>2025.07</t>
         </is>
       </c>
       <c r="H226" t="inlineStr">
@@ -20864,7 +21096,7 @@
       </c>
       <c r="G227" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H227" t="inlineStr"/>
@@ -20949,7 +21181,7 @@
       </c>
       <c r="G228" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H228" t="inlineStr"/>
@@ -21034,7 +21266,7 @@
       </c>
       <c r="G229" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H229" t="inlineStr"/>
@@ -21119,7 +21351,7 @@
       </c>
       <c r="G230" t="inlineStr">
         <is>
-          <t>2025.2</t>
+          <t>2025.02</t>
         </is>
       </c>
       <c r="H230" t="inlineStr"/>
@@ -21204,7 +21436,7 @@
       </c>
       <c r="G231" t="inlineStr">
         <is>
-          <t>2025.2</t>
+          <t>2025.02</t>
         </is>
       </c>
       <c r="H231" t="inlineStr"/>
@@ -21289,7 +21521,7 @@
       </c>
       <c r="G232" t="inlineStr">
         <is>
-          <t>2025.2</t>
+          <t>2025.02</t>
         </is>
       </c>
       <c r="H232" t="inlineStr"/>
@@ -21374,7 +21606,7 @@
       </c>
       <c r="G233" t="inlineStr">
         <is>
-          <t>2025.2</t>
+          <t>2025.02</t>
         </is>
       </c>
       <c r="H233" t="inlineStr"/>
@@ -21459,7 +21691,7 @@
       </c>
       <c r="G234" t="inlineStr">
         <is>
-          <t>2025.3</t>
+          <t>2025.03</t>
         </is>
       </c>
       <c r="H234" t="inlineStr"/>
@@ -21544,7 +21776,7 @@
       </c>
       <c r="G235" t="inlineStr">
         <is>
-          <t>2025.4</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H235" t="inlineStr"/>
@@ -21629,7 +21861,7 @@
       </c>
       <c r="G236" t="inlineStr">
         <is>
-          <t>2025.4</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H236" t="inlineStr"/>
@@ -21714,7 +21946,7 @@
       </c>
       <c r="G237" t="inlineStr">
         <is>
-          <t>2025.4</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H237" t="inlineStr"/>
@@ -21799,7 +22031,7 @@
       </c>
       <c r="G238" t="inlineStr">
         <is>
-          <t>2025.4</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H238" t="inlineStr"/>
@@ -21884,7 +22116,7 @@
       </c>
       <c r="G239" t="inlineStr">
         <is>
-          <t>2025.5</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H239" t="inlineStr"/>
@@ -21969,7 +22201,7 @@
       </c>
       <c r="G240" t="inlineStr">
         <is>
-          <t>2025.5</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H240" t="inlineStr"/>
@@ -22054,7 +22286,7 @@
       </c>
       <c r="G241" t="inlineStr">
         <is>
-          <t>2025.5</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H241" t="inlineStr"/>
@@ -22139,7 +22371,7 @@
       </c>
       <c r="G242" t="inlineStr">
         <is>
-          <t>2025.5</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H242" t="inlineStr"/>
@@ -22224,7 +22456,7 @@
       </c>
       <c r="G243" t="inlineStr">
         <is>
-          <t>2025.5</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H243" t="inlineStr"/>
@@ -22309,7 +22541,7 @@
       </c>
       <c r="G244" t="inlineStr">
         <is>
-          <t>2025.6</t>
+          <t>2025.06</t>
         </is>
       </c>
       <c r="H244" t="inlineStr"/>
@@ -22394,7 +22626,7 @@
       </c>
       <c r="G245" t="inlineStr">
         <is>
-          <t>2025.6</t>
+          <t>2025.06</t>
         </is>
       </c>
       <c r="H245" t="inlineStr"/>
@@ -22479,7 +22711,7 @@
       </c>
       <c r="G246" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H246" t="n">
@@ -22568,7 +22800,7 @@
       </c>
       <c r="G247" t="inlineStr">
         <is>
-          <t>2025.1</t>
+          <t>2025.01</t>
         </is>
       </c>
       <c r="H247" t="n">
@@ -22657,7 +22889,7 @@
       </c>
       <c r="G248" t="inlineStr">
         <is>
-          <t>2025.2</t>
+          <t>2025.02</t>
         </is>
       </c>
       <c r="H248" t="n">
@@ -22746,7 +22978,7 @@
       </c>
       <c r="G249" t="inlineStr">
         <is>
-          <t>2025.2</t>
+          <t>2025.02</t>
         </is>
       </c>
       <c r="H249" t="n">
@@ -22835,7 +23067,7 @@
       </c>
       <c r="G250" t="inlineStr">
         <is>
-          <t>2025.2</t>
+          <t>2025.02</t>
         </is>
       </c>
       <c r="H250" t="n">
@@ -22924,7 +23156,7 @@
       </c>
       <c r="G251" t="inlineStr">
         <is>
-          <t>2025.4</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H251" t="n">
@@ -23013,7 +23245,7 @@
       </c>
       <c r="G252" t="inlineStr">
         <is>
-          <t>2025.4</t>
+          <t>2025.04</t>
         </is>
       </c>
       <c r="H252" t="n">
@@ -23102,7 +23334,7 @@
       </c>
       <c r="G253" t="inlineStr">
         <is>
-          <t>2025.5</t>
+          <t>2025.05</t>
         </is>
       </c>
       <c r="H253" t="n">

</xml_diff>

<commit_message>
ok unidad de medida, toneladas finales
</commit_message>
<xml_diff>
--- a/importaciones_unificadas.xlsx
+++ b/importaciones_unificadas.xlsx
@@ -650,10 +650,12 @@
       </c>
       <c r="X2" t="inlineStr">
         <is>
-          <t>TONELADA</t>
-        </is>
-      </c>
-      <c r="Y2" t="inlineStr"/>
+          <t>TONELADAS</t>
+        </is>
+      </c>
+      <c r="Y2" t="n">
+        <v>26</v>
+      </c>
       <c r="Z2" t="inlineStr">
         <is>
           <t>P S Q ARGENTINA SOCIEDAD ANONI</t>
@@ -733,10 +735,12 @@
       </c>
       <c r="X3" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y3" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y3" t="n">
+        <v>6.5</v>
+      </c>
       <c r="Z3" t="inlineStr">
         <is>
           <t>WORLD MARKET S R L</t>
@@ -899,10 +903,12 @@
       </c>
       <c r="X5" t="inlineStr">
         <is>
-          <t>TONELADA</t>
-        </is>
-      </c>
-      <c r="Y5" t="inlineStr"/>
+          <t>TONELADAS</t>
+        </is>
+      </c>
+      <c r="Y5" t="n">
+        <v>9</v>
+      </c>
       <c r="Z5" t="inlineStr">
         <is>
           <t>TERNIUM ARGENTINA S A</t>
@@ -982,10 +988,12 @@
       </c>
       <c r="X6" t="inlineStr">
         <is>
-          <t>TONELADA</t>
-        </is>
-      </c>
-      <c r="Y6" t="inlineStr"/>
+          <t>TONELADAS</t>
+        </is>
+      </c>
+      <c r="Y6" t="n">
+        <v>28</v>
+      </c>
       <c r="Z6" t="inlineStr">
         <is>
           <t>LABORATORIO CUENCA S A</t>
@@ -1065,10 +1073,12 @@
       </c>
       <c r="X7" t="inlineStr">
         <is>
-          <t>TONELADA</t>
-        </is>
-      </c>
-      <c r="Y7" t="inlineStr"/>
+          <t>TONELADAS</t>
+        </is>
+      </c>
+      <c r="Y7" t="n">
+        <v>13</v>
+      </c>
       <c r="Z7" t="inlineStr">
         <is>
           <t>TERNIUM ARGENTINA S A</t>
@@ -1231,10 +1241,12 @@
       </c>
       <c r="X9" t="inlineStr">
         <is>
-          <t>TONELADA</t>
-        </is>
-      </c>
-      <c r="Y9" t="inlineStr"/>
+          <t>TONELADAS</t>
+        </is>
+      </c>
+      <c r="Y9" t="n">
+        <v>26</v>
+      </c>
       <c r="Z9" t="inlineStr">
         <is>
           <t>P S Q ARGENTINA SOCIEDAD ANONI</t>
@@ -1314,10 +1326,12 @@
       </c>
       <c r="X10" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y10" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y10" t="n">
+        <v>5.2</v>
+      </c>
       <c r="Z10" t="inlineStr">
         <is>
           <t>WORLD MARKET S R L</t>
@@ -1397,10 +1411,12 @@
       </c>
       <c r="X11" t="inlineStr">
         <is>
-          <t>TONELADA</t>
-        </is>
-      </c>
-      <c r="Y11" t="inlineStr"/>
+          <t>TONELADAS</t>
+        </is>
+      </c>
+      <c r="Y11" t="n">
+        <v>6</v>
+      </c>
       <c r="Z11" t="inlineStr">
         <is>
           <t>TERNIUM ARGENTINA S A</t>
@@ -1480,10 +1496,12 @@
       </c>
       <c r="X12" t="inlineStr">
         <is>
-          <t>TONELADA</t>
-        </is>
-      </c>
-      <c r="Y12" t="inlineStr"/>
+          <t>TONELADAS</t>
+        </is>
+      </c>
+      <c r="Y12" t="n">
+        <v>3</v>
+      </c>
       <c r="Z12" t="inlineStr">
         <is>
           <t>TERNIUM ARGENTINA S A</t>
@@ -1563,10 +1581,12 @@
       </c>
       <c r="X13" t="inlineStr">
         <is>
-          <t>TONELADA</t>
-        </is>
-      </c>
-      <c r="Y13" t="inlineStr"/>
+          <t>TONELADAS</t>
+        </is>
+      </c>
+      <c r="Y13" t="n">
+        <v>6</v>
+      </c>
       <c r="Z13" t="inlineStr">
         <is>
           <t>TERNIUM ARGENTINA S A</t>
@@ -1646,10 +1666,12 @@
       </c>
       <c r="X14" t="inlineStr">
         <is>
-          <t>TONELADA</t>
-        </is>
-      </c>
-      <c r="Y14" t="inlineStr"/>
+          <t>TONELADAS</t>
+        </is>
+      </c>
+      <c r="Y14" t="n">
+        <v>28</v>
+      </c>
       <c r="Z14" t="inlineStr">
         <is>
           <t>LABORATORIO CUENCA S A</t>
@@ -1729,10 +1751,12 @@
       </c>
       <c r="X15" t="inlineStr">
         <is>
-          <t>TONELADA</t>
-        </is>
-      </c>
-      <c r="Y15" t="inlineStr"/>
+          <t>TONELADAS</t>
+        </is>
+      </c>
+      <c r="Y15" t="n">
+        <v>27</v>
+      </c>
       <c r="Z15" t="inlineStr">
         <is>
           <t>LABORATORIO LANODERM SRL</t>
@@ -1812,10 +1836,12 @@
       </c>
       <c r="X16" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y16" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y16" t="n">
+        <v>3</v>
+      </c>
       <c r="Z16" t="inlineStr">
         <is>
           <t>GRUPO AYUDIN ARGENTINA S. A.</t>
@@ -1895,10 +1921,12 @@
       </c>
       <c r="X17" t="inlineStr">
         <is>
-          <t>TONELADA</t>
-        </is>
-      </c>
-      <c r="Y17" t="inlineStr"/>
+          <t>TONELADAS</t>
+        </is>
+      </c>
+      <c r="Y17" t="n">
+        <v>28</v>
+      </c>
       <c r="Z17" t="inlineStr">
         <is>
           <t>LABORATORIO CUENCA S A</t>
@@ -1978,10 +2006,12 @@
       </c>
       <c r="X18" t="inlineStr">
         <is>
-          <t>TONELADA</t>
-        </is>
-      </c>
-      <c r="Y18" t="inlineStr"/>
+          <t>TONELADAS</t>
+        </is>
+      </c>
+      <c r="Y18" t="n">
+        <v>26</v>
+      </c>
       <c r="Z18" t="inlineStr">
         <is>
           <t>P S Q ARGENTINA SOCIEDAD ANONI</t>
@@ -2061,10 +2091,12 @@
       </c>
       <c r="X19" t="inlineStr">
         <is>
-          <t>TONELADA</t>
-        </is>
-      </c>
-      <c r="Y19" t="inlineStr"/>
+          <t>TONELADAS</t>
+        </is>
+      </c>
+      <c r="Y19" t="n">
+        <v>4</v>
+      </c>
       <c r="Z19" t="inlineStr">
         <is>
           <t>TERNIUM ARGENTINA S A</t>
@@ -2144,10 +2176,12 @@
       </c>
       <c r="X20" t="inlineStr">
         <is>
-          <t>TONELADA</t>
-        </is>
-      </c>
-      <c r="Y20" t="inlineStr"/>
+          <t>TONELADAS</t>
+        </is>
+      </c>
+      <c r="Y20" t="n">
+        <v>4</v>
+      </c>
       <c r="Z20" t="inlineStr">
         <is>
           <t>TERNIUM ARGENTINA S A</t>
@@ -2227,10 +2261,12 @@
       </c>
       <c r="X21" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y21" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y21" t="n">
+        <v>5.2</v>
+      </c>
       <c r="Z21" t="inlineStr">
         <is>
           <t>WORLD MARKET S R L</t>
@@ -2310,10 +2346,12 @@
       </c>
       <c r="X22" t="inlineStr">
         <is>
-          <t>TONELADA</t>
-        </is>
-      </c>
-      <c r="Y22" t="inlineStr"/>
+          <t>TONELADAS</t>
+        </is>
+      </c>
+      <c r="Y22" t="n">
+        <v>10</v>
+      </c>
       <c r="Z22" t="inlineStr">
         <is>
           <t>ACINDAR INDUSTRIA ARGENTINA DE</t>
@@ -2393,10 +2431,12 @@
       </c>
       <c r="X23" t="inlineStr">
         <is>
-          <t>TONELADA</t>
-        </is>
-      </c>
-      <c r="Y23" t="inlineStr"/>
+          <t>TONELADAS</t>
+        </is>
+      </c>
+      <c r="Y23" t="n">
+        <v>26</v>
+      </c>
       <c r="Z23" t="inlineStr">
         <is>
           <t>P S Q ARGENTINA SOCIEDAD ANONI</t>
@@ -2559,10 +2599,12 @@
       </c>
       <c r="X25" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y25" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y25" t="n">
+        <v>9.1</v>
+      </c>
       <c r="Z25" t="inlineStr">
         <is>
           <t>WORLD MARKET S R L</t>
@@ -2642,10 +2684,12 @@
       </c>
       <c r="X26" t="inlineStr">
         <is>
-          <t>TONELADA</t>
-        </is>
-      </c>
-      <c r="Y26" t="inlineStr"/>
+          <t>TONELADAS</t>
+        </is>
+      </c>
+      <c r="Y26" t="n">
+        <v>28</v>
+      </c>
       <c r="Z26" t="inlineStr">
         <is>
           <t>LABORATORIO CUENCA S A</t>
@@ -2725,10 +2769,12 @@
       </c>
       <c r="X27" t="inlineStr">
         <is>
-          <t>TONELADA</t>
-        </is>
-      </c>
-      <c r="Y27" t="inlineStr"/>
+          <t>TONELADAS</t>
+        </is>
+      </c>
+      <c r="Y27" t="n">
+        <v>6</v>
+      </c>
       <c r="Z27" t="inlineStr">
         <is>
           <t>SIDERCA S A I C</t>
@@ -2808,10 +2854,12 @@
       </c>
       <c r="X28" t="inlineStr">
         <is>
-          <t>TONELADA</t>
-        </is>
-      </c>
-      <c r="Y28" t="inlineStr"/>
+          <t>TONELADAS</t>
+        </is>
+      </c>
+      <c r="Y28" t="n">
+        <v>6</v>
+      </c>
       <c r="Z28" t="inlineStr">
         <is>
           <t>SIDERCA S A I C</t>
@@ -2891,10 +2939,12 @@
       </c>
       <c r="X29" t="inlineStr">
         <is>
-          <t>TONELADA</t>
-        </is>
-      </c>
-      <c r="Y29" t="inlineStr"/>
+          <t>TONELADAS</t>
+        </is>
+      </c>
+      <c r="Y29" t="n">
+        <v>6</v>
+      </c>
       <c r="Z29" t="inlineStr">
         <is>
           <t>SIDERCA S A I C</t>
@@ -2974,10 +3024,12 @@
       </c>
       <c r="X30" t="inlineStr">
         <is>
-          <t>TONELADA</t>
-        </is>
-      </c>
-      <c r="Y30" t="inlineStr"/>
+          <t>TONELADAS</t>
+        </is>
+      </c>
+      <c r="Y30" t="n">
+        <v>6</v>
+      </c>
       <c r="Z30" t="inlineStr">
         <is>
           <t>SIDERCA S A I C</t>
@@ -3057,10 +3109,12 @@
       </c>
       <c r="X31" t="inlineStr">
         <is>
-          <t>TONELADA</t>
-        </is>
-      </c>
-      <c r="Y31" t="inlineStr"/>
+          <t>TONELADAS</t>
+        </is>
+      </c>
+      <c r="Y31" t="n">
+        <v>6</v>
+      </c>
       <c r="Z31" t="inlineStr">
         <is>
           <t>SIDERCA S A I C</t>
@@ -3140,10 +3194,12 @@
       </c>
       <c r="X32" t="inlineStr">
         <is>
-          <t>TONELADA</t>
-        </is>
-      </c>
-      <c r="Y32" t="inlineStr"/>
+          <t>TONELADAS</t>
+        </is>
+      </c>
+      <c r="Y32" t="n">
+        <v>6</v>
+      </c>
       <c r="Z32" t="inlineStr">
         <is>
           <t>SIDERCA S A I C</t>
@@ -3223,10 +3279,12 @@
       </c>
       <c r="X33" t="inlineStr">
         <is>
-          <t>TONELADA</t>
-        </is>
-      </c>
-      <c r="Y33" t="inlineStr"/>
+          <t>TONELADAS</t>
+        </is>
+      </c>
+      <c r="Y33" t="n">
+        <v>6</v>
+      </c>
       <c r="Z33" t="inlineStr">
         <is>
           <t>SIDERCA S A I C</t>
@@ -3306,10 +3364,12 @@
       </c>
       <c r="X34" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y34" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y34" t="n">
+        <v>0.2</v>
+      </c>
       <c r="Z34" t="inlineStr">
         <is>
           <t>CASTELARI LUCAS NICOLAS</t>
@@ -3389,10 +3449,12 @@
       </c>
       <c r="X35" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y35" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y35" t="n">
+        <v>51</v>
+      </c>
       <c r="Z35" t="inlineStr">
         <is>
           <t>POLYKIM  S. R. L.</t>
@@ -3472,10 +3534,12 @@
       </c>
       <c r="X36" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y36" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y36" t="n">
+        <v>51</v>
+      </c>
       <c r="Z36" t="inlineStr">
         <is>
           <t>POLYKIM  S. R. L.</t>
@@ -3555,10 +3619,12 @@
       </c>
       <c r="X37" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y37" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y37" t="n">
+        <v>54</v>
+      </c>
       <c r="Z37" t="inlineStr">
         <is>
           <t>QUIMICERA ESPECIALIDADES  S.A.</t>
@@ -3638,10 +3704,12 @@
       </c>
       <c r="X38" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y38" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y38" t="n">
+        <v>51</v>
+      </c>
       <c r="Z38" t="inlineStr">
         <is>
           <t>POLYKIM  S. R. L.</t>
@@ -3721,10 +3789,12 @@
       </c>
       <c r="X39" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y39" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y39" t="n">
+        <v>51</v>
+      </c>
       <c r="Z39" t="inlineStr">
         <is>
           <t>POLYKIM  S. R. L.</t>
@@ -3804,10 +3874,12 @@
       </c>
       <c r="X40" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y40" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y40" t="n">
+        <v>50.4</v>
+      </c>
       <c r="Z40" t="inlineStr">
         <is>
           <t>ABA COLOR SRL</t>
@@ -3887,10 +3959,12 @@
       </c>
       <c r="X41" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y41" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y41" t="n">
+        <v>0.2</v>
+      </c>
       <c r="Z41" t="inlineStr">
         <is>
           <t>INDUSTRIAS CERAMICAS LOURDES S</t>
@@ -3970,10 +4044,12 @@
       </c>
       <c r="X42" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y42" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y42" t="n">
+        <v>3.44</v>
+      </c>
       <c r="Z42" t="inlineStr">
         <is>
           <t>UNILEVER DE ARGENTINA S A</t>
@@ -4053,10 +4129,12 @@
       </c>
       <c r="X43" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y43" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y43" t="n">
+        <v>25.2</v>
+      </c>
       <c r="Z43" t="inlineStr">
         <is>
           <t>ABA COLOR SRL</t>
@@ -4136,10 +4214,12 @@
       </c>
       <c r="X44" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y44" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y44" t="n">
+        <v>0.2</v>
+      </c>
       <c r="Z44" t="inlineStr">
         <is>
           <t>INDUSTRIAS CERAMICAS LOURDES S</t>
@@ -4219,10 +4299,12 @@
       </c>
       <c r="X45" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y45" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y45" t="n">
+        <v>0.08</v>
+      </c>
       <c r="Z45" t="inlineStr">
         <is>
           <t>CERAMICA ALBERDI S A</t>
@@ -4302,10 +4384,12 @@
       </c>
       <c r="X46" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y46" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y46" t="n">
+        <v>3.84</v>
+      </c>
       <c r="Z46" t="inlineStr">
         <is>
           <t>UNILEVER DE ARGENTINA S A</t>
@@ -4385,10 +4469,12 @@
       </c>
       <c r="X47" t="inlineStr">
         <is>
-          <t>TONELADA</t>
-        </is>
-      </c>
-      <c r="Y47" t="inlineStr"/>
+          <t>TONELADAS</t>
+        </is>
+      </c>
+      <c r="Y47" t="n">
+        <v>4</v>
+      </c>
       <c r="Z47" t="inlineStr">
         <is>
           <t>ACINDAR INDUSTRIA ARGENTINA DE</t>
@@ -4551,10 +4637,12 @@
       </c>
       <c r="X49" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y49" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y49" t="n">
+        <v>0.001</v>
+      </c>
       <c r="Z49" t="inlineStr">
         <is>
           <t>UNITS SUDAMERICANA S A</t>
@@ -4634,10 +4722,12 @@
       </c>
       <c r="X50" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y50" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y50" t="n">
+        <v>0.001</v>
+      </c>
       <c r="Z50" t="inlineStr">
         <is>
           <t>CLOROX SERVICIOS CORPORATIVOS</t>
@@ -4800,10 +4890,12 @@
       </c>
       <c r="X52" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y52" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y52" t="n">
+        <v>0</v>
+      </c>
       <c r="Z52" t="inlineStr">
         <is>
           <t>CLOROX SERVICIOS CORPORATIVOS</t>
@@ -4883,10 +4975,12 @@
       </c>
       <c r="X53" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y53" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y53" t="n">
+        <v>0.54</v>
+      </c>
       <c r="Z53" t="inlineStr">
         <is>
           <t>COLGATE PALMOLIVE ARGENTINA S.</t>
@@ -12116,10 +12210,12 @@
       </c>
       <c r="X138" t="inlineStr">
         <is>
-          <t>KILOS NETOS</t>
-        </is>
-      </c>
-      <c r="Y138" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y138" t="n">
+        <v>0.00675</v>
+      </c>
       <c r="Z138" t="inlineStr">
         <is>
           <t>MERCK S A</t>
@@ -12217,10 +12313,12 @@
       </c>
       <c r="X139" t="inlineStr">
         <is>
-          <t>KILOS NETOS</t>
-        </is>
-      </c>
-      <c r="Y139" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y139" t="n">
+        <v>10.72</v>
+      </c>
       <c r="Z139" t="inlineStr">
         <is>
           <t>MINOVA MINING SERVICES S.A.</t>
@@ -12318,10 +12416,12 @@
       </c>
       <c r="X140" t="inlineStr">
         <is>
-          <t>KILOS NETOS</t>
-        </is>
-      </c>
-      <c r="Y140" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y140" t="n">
+        <v>1.47654</v>
+      </c>
       <c r="Z140" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -12419,10 +12519,12 @@
       </c>
       <c r="X141" t="inlineStr">
         <is>
-          <t>KILOS NETOS</t>
-        </is>
-      </c>
-      <c r="Y141" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y141" t="n">
+        <v>10.4</v>
+      </c>
       <c r="Z141" t="inlineStr">
         <is>
           <t>COMEX S.A.</t>
@@ -12520,10 +12622,12 @@
       </c>
       <c r="X142" t="inlineStr">
         <is>
-          <t>KILOS NETOS</t>
-        </is>
-      </c>
-      <c r="Y142" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y142" t="n">
+        <v>2.70341</v>
+      </c>
       <c r="Z142" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -12621,10 +12725,12 @@
       </c>
       <c r="X143" t="inlineStr">
         <is>
-          <t>KILOS NETOS</t>
-        </is>
-      </c>
-      <c r="Y143" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y143" t="n">
+        <v>0.9979199999999999</v>
+      </c>
       <c r="Z143" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -12722,10 +12828,12 @@
       </c>
       <c r="X144" t="inlineStr">
         <is>
-          <t>KILOS NETOS</t>
-        </is>
-      </c>
-      <c r="Y144" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y144" t="n">
+        <v>112</v>
+      </c>
       <c r="Z144" t="inlineStr">
         <is>
           <t>CASAS DEL VALLE BARROS HNOS.LT</t>
@@ -12823,10 +12931,12 @@
       </c>
       <c r="X145" t="inlineStr">
         <is>
-          <t>KILOS NETOS</t>
-        </is>
-      </c>
-      <c r="Y145" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y145" t="n">
+        <v>0.005990000000000001</v>
+      </c>
       <c r="Z145" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -12924,10 +13034,12 @@
       </c>
       <c r="X146" t="inlineStr">
         <is>
-          <t>KILOS NETOS</t>
-        </is>
-      </c>
-      <c r="Y146" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y146" t="n">
+        <v>24</v>
+      </c>
       <c r="Z146" t="inlineStr">
         <is>
           <t>PRODUCTOS CAVE S A</t>
@@ -13025,10 +13137,12 @@
       </c>
       <c r="X147" t="inlineStr">
         <is>
-          <t>KILOS NETOS</t>
-        </is>
-      </c>
-      <c r="Y147" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y147" t="n">
+        <v>1.5</v>
+      </c>
       <c r="Z147" t="inlineStr">
         <is>
           <t>NALCO INDUSTRIAL SERVICES CHIL</t>
@@ -13126,10 +13240,12 @@
       </c>
       <c r="X148" t="inlineStr">
         <is>
-          <t>KILOS NETOS</t>
-        </is>
-      </c>
-      <c r="Y148" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y148" t="n">
+        <v>50</v>
+      </c>
       <c r="Z148" t="inlineStr">
         <is>
           <t>CASAS DEL VALLE BARROS HNOS.LT</t>
@@ -13227,10 +13343,12 @@
       </c>
       <c r="X149" t="inlineStr">
         <is>
-          <t>KILOS NETOS</t>
-        </is>
-      </c>
-      <c r="Y149" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y149" t="n">
+        <v>24</v>
+      </c>
       <c r="Z149" t="inlineStr">
         <is>
           <t>PRODUCTOS CAVE S A</t>
@@ -13328,10 +13446,12 @@
       </c>
       <c r="X150" t="inlineStr">
         <is>
-          <t>KILOS NETOS</t>
-        </is>
-      </c>
-      <c r="Y150" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y150" t="n">
+        <v>56</v>
+      </c>
       <c r="Z150" t="inlineStr">
         <is>
           <t>CASAS DEL VALLE BARROS HNOS.LT</t>
@@ -13429,10 +13549,12 @@
       </c>
       <c r="X151" t="inlineStr">
         <is>
-          <t>KILOS NETOS</t>
-        </is>
-      </c>
-      <c r="Y151" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y151" t="n">
+        <v>24</v>
+      </c>
       <c r="Z151" t="inlineStr">
         <is>
           <t>PRODUCTOS CAVE S A</t>
@@ -13530,10 +13652,12 @@
       </c>
       <c r="X152" t="inlineStr">
         <is>
-          <t>KILOS NETOS</t>
-        </is>
-      </c>
-      <c r="Y152" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y152" t="n">
+        <v>56</v>
+      </c>
       <c r="Z152" t="inlineStr">
         <is>
           <t>CASAS DEL VALLE BARROS HNOS.LT</t>
@@ -13631,10 +13755,12 @@
       </c>
       <c r="X153" t="inlineStr">
         <is>
-          <t>KILOS NETOS</t>
-        </is>
-      </c>
-      <c r="Y153" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y153" t="n">
+        <v>22.8</v>
+      </c>
       <c r="Z153" t="inlineStr">
         <is>
           <t>PRODUCTOS CAVE S A</t>
@@ -13732,10 +13858,12 @@
       </c>
       <c r="X154" t="inlineStr">
         <is>
-          <t>KILOS NETOS</t>
-        </is>
-      </c>
-      <c r="Y154" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y154" t="n">
+        <v>13.986</v>
+      </c>
       <c r="Z154" t="inlineStr">
         <is>
           <t>CIA.CHILENA DE FOSFOROS S.A.</t>
@@ -13833,10 +13961,12 @@
       </c>
       <c r="X155" t="inlineStr">
         <is>
-          <t>KILOS NETOS</t>
-        </is>
-      </c>
-      <c r="Y155" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y155" t="n">
+        <v>11.214</v>
+      </c>
       <c r="Z155" t="inlineStr">
         <is>
           <t>CIA.CHILENA DE FOSFOROS S.A.</t>
@@ -13934,10 +14064,12 @@
       </c>
       <c r="X156" t="inlineStr">
         <is>
-          <t>KILOS NETOS</t>
-        </is>
-      </c>
-      <c r="Y156" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y156" t="n">
+        <v>0.0135</v>
+      </c>
       <c r="Z156" t="inlineStr">
         <is>
           <t>MERCK S A</t>
@@ -14035,10 +14167,12 @@
       </c>
       <c r="X157" t="inlineStr">
         <is>
-          <t>KILOS NETOS</t>
-        </is>
-      </c>
-      <c r="Y157" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y157" t="n">
+        <v>10.89184</v>
+      </c>
       <c r="Z157" t="inlineStr">
         <is>
           <t>FUNDICION TALLERES LIMITADA</t>
@@ -14134,10 +14268,12 @@
       </c>
       <c r="X158" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y158" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y158" t="n">
+        <v>4.94</v>
+      </c>
       <c r="Z158" t="inlineStr">
         <is>
           <t>RECIEND SAS</t>
@@ -14229,10 +14365,12 @@
       </c>
       <c r="X159" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y159" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y159" t="n">
+        <v>1</v>
+      </c>
       <c r="Z159" t="inlineStr">
         <is>
           <t>SUDAMIN S A S</t>
@@ -14324,10 +14462,12 @@
       </c>
       <c r="X160" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y160" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y160" t="n">
+        <v>1.44</v>
+      </c>
       <c r="Z160" t="inlineStr">
         <is>
           <t>REPRESENTS COLON LTDA</t>
@@ -14419,10 +14559,12 @@
       </c>
       <c r="X161" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y161" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y161" t="n">
+        <v>0.13735</v>
+      </c>
       <c r="Z161" t="inlineStr">
         <is>
           <t>FLUIDRA COLOMBIA S A S</t>
@@ -14514,10 +14656,12 @@
       </c>
       <c r="X162" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y162" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y162" t="n">
+        <v>3.12</v>
+      </c>
       <c r="Z162" t="inlineStr">
         <is>
           <t>RECIEND SAS</t>
@@ -14609,10 +14753,12 @@
       </c>
       <c r="X163" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y163" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y163" t="n">
+        <v>0.0231</v>
+      </c>
       <c r="Z163" t="inlineStr">
         <is>
           <t>HENKEL COL S A S</t>
@@ -14704,10 +14850,12 @@
       </c>
       <c r="X164" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y164" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y164" t="n">
+        <v>0.0189</v>
+      </c>
       <c r="Z164" t="inlineStr">
         <is>
           <t>HENKEL COL S A S</t>
@@ -14799,10 +14947,12 @@
       </c>
       <c r="X165" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y165" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y165" t="n">
+        <v>3.12</v>
+      </c>
       <c r="Z165" t="inlineStr">
         <is>
           <t>RECIEND SAS</t>
@@ -14894,10 +15044,12 @@
       </c>
       <c r="X166" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y166" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y166" t="n">
+        <v>0.0189</v>
+      </c>
       <c r="Z166" t="inlineStr">
         <is>
           <t>HENKEL COL S A S</t>
@@ -14989,10 +15141,12 @@
       </c>
       <c r="X167" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y167" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y167" t="n">
+        <v>0.0231</v>
+      </c>
       <c r="Z167" t="inlineStr">
         <is>
           <t>HENKEL COL S A S</t>
@@ -15084,10 +15238,12 @@
       </c>
       <c r="X168" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y168" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y168" t="n">
+        <v>1.35</v>
+      </c>
       <c r="Z168" t="inlineStr">
         <is>
           <t>INNOVIAS CONSTRUCTORA SAS</t>
@@ -15179,10 +15335,12 @@
       </c>
       <c r="X169" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y169" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y169" t="n">
+        <v>8.4</v>
+      </c>
       <c r="Z169" t="inlineStr">
         <is>
           <t>SOLUCIONES ESPECIALIZADAS EN EQUIPOS Y MAQUINARIA DE COL SAS</t>
@@ -15270,10 +15428,12 @@
       </c>
       <c r="X170" t="inlineStr">
         <is>
-          <t>KILOGRAMO BRUTO</t>
-        </is>
-      </c>
-      <c r="Y170" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y170" t="n">
+        <v>20.878918</v>
+      </c>
       <c r="Z170" t="inlineStr">
         <is>
           <t>LINDE ECUADOR S.A.</t>
@@ -15365,10 +15525,12 @@
       </c>
       <c r="X171" t="inlineStr">
         <is>
-          <t>KILOGRAMO BRUTO</t>
-        </is>
-      </c>
-      <c r="Y171" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y171" t="n">
+        <v>25.8</v>
+      </c>
       <c r="Z171" t="inlineStr">
         <is>
           <t>TRANSMERQUIM DE ECUADOR S.A.</t>
@@ -15460,10 +15622,12 @@
       </c>
       <c r="X172" t="inlineStr">
         <is>
-          <t>KILOGRAMO BRUTO</t>
-        </is>
-      </c>
-      <c r="Y172" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y172" t="n">
+        <v>0.015</v>
+      </c>
       <c r="Z172" t="inlineStr">
         <is>
           <t>COMPAÑIA ANONIMA PRACTICASA</t>
@@ -15555,10 +15719,12 @@
       </c>
       <c r="X173" t="inlineStr">
         <is>
-          <t>KILOGRAMO BRUTO</t>
-        </is>
-      </c>
-      <c r="Y173" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y173" t="n">
+        <v>0.004</v>
+      </c>
       <c r="Z173" t="inlineStr">
         <is>
           <t>COMPAÑIA ANONIMA PRACTICASA</t>
@@ -15650,10 +15816,12 @@
       </c>
       <c r="X174" t="inlineStr">
         <is>
-          <t>KILOGRAMO BRUTO</t>
-        </is>
-      </c>
-      <c r="Y174" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y174" t="n">
+        <v>17.663749</v>
+      </c>
       <c r="Z174" t="inlineStr">
         <is>
           <t>LINDE ECUADOR S.A.</t>
@@ -15745,10 +15913,12 @@
       </c>
       <c r="X175" t="inlineStr">
         <is>
-          <t>KILOGRAMO BRUTO</t>
-        </is>
-      </c>
-      <c r="Y175" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y175" t="n">
+        <v>0.024</v>
+      </c>
       <c r="Z175" t="inlineStr">
         <is>
           <t>COMPAÑIA ANONIMA PRACTICASA</t>
@@ -15840,10 +16010,12 @@
       </c>
       <c r="X176" t="inlineStr">
         <is>
-          <t>KILOGRAMO BRUTO</t>
-        </is>
-      </c>
-      <c r="Y176" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y176" t="n">
+        <v>25.72</v>
+      </c>
       <c r="Z176" t="inlineStr">
         <is>
           <t>FIBESA FB-INC S.A.S.</t>
@@ -15935,10 +16107,12 @@
       </c>
       <c r="X177" t="inlineStr">
         <is>
-          <t>KILOGRAMO BRUTO</t>
-        </is>
-      </c>
-      <c r="Y177" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y177" t="n">
+        <v>0.001</v>
+      </c>
       <c r="Z177" t="inlineStr">
         <is>
           <t>LA FABRIL, S.A.</t>
@@ -16030,10 +16204,12 @@
       </c>
       <c r="X178" t="inlineStr">
         <is>
-          <t>KILOGRAMO BRUTO</t>
-        </is>
-      </c>
-      <c r="Y178" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y178" t="n">
+        <v>0.017232</v>
+      </c>
       <c r="Z178" t="inlineStr">
         <is>
           <t>APLIKA APLICADORES TECNICOS PARA LA CONSTRUCCION CIA. LTDA</t>
@@ -16125,10 +16301,12 @@
       </c>
       <c r="X179" t="inlineStr">
         <is>
-          <t>KILOGRAMO BRUTO</t>
-        </is>
-      </c>
-      <c r="Y179" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y179" t="n">
+        <v>0.362681</v>
+      </c>
       <c r="Z179" t="inlineStr">
         <is>
           <t>APLIKA APLICADORES TECNICOS PARA LA CONSTRUCCION CIA. LTDA</t>
@@ -16220,10 +16398,12 @@
       </c>
       <c r="X180" t="inlineStr">
         <is>
-          <t>KILOGRAMO BRUTO</t>
-        </is>
-      </c>
-      <c r="Y180" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y180" t="n">
+        <v>18.168656</v>
+      </c>
       <c r="Z180" t="inlineStr">
         <is>
           <t>LINDE ECUADOR S.A.</t>
@@ -16325,10 +16505,12 @@
       </c>
       <c r="X181" t="inlineStr">
         <is>
-          <t>KG</t>
-        </is>
-      </c>
-      <c r="Y181" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y181" t="n">
+        <v>20</v>
+      </c>
       <c r="Z181" t="inlineStr">
         <is>
           <t>CERAMICA LIMA S A</t>
@@ -16430,10 +16612,12 @@
       </c>
       <c r="X182" t="inlineStr">
         <is>
-          <t>KG</t>
-        </is>
-      </c>
-      <c r="Y182" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y182" t="n">
+        <v>1.4515</v>
+      </c>
       <c r="Z182" t="inlineStr">
         <is>
           <t>ECOLAB PERU HOLDINGS S.R.L.</t>
@@ -16535,10 +16719,12 @@
       </c>
       <c r="X183" t="inlineStr">
         <is>
-          <t>KG</t>
-        </is>
-      </c>
-      <c r="Y183" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y183" t="n">
+        <v>2.90299</v>
+      </c>
       <c r="Z183" t="inlineStr">
         <is>
           <t>ECOLAB PERU HOLDINGS S.R.L.</t>
@@ -16850,10 +17036,12 @@
       </c>
       <c r="X186" t="inlineStr">
         <is>
-          <t>KG</t>
-        </is>
-      </c>
-      <c r="Y186" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y186" t="n">
+        <v>15.6</v>
+      </c>
       <c r="Z186" t="inlineStr">
         <is>
           <t>UNITRADE S.A.C.</t>
@@ -17585,10 +17773,12 @@
       </c>
       <c r="X193" t="inlineStr">
         <is>
-          <t>KG</t>
-        </is>
-      </c>
-      <c r="Y193" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y193" t="n">
+        <v>3.75</v>
+      </c>
       <c r="Z193" t="inlineStr">
         <is>
           <t>CERAMICA LIMA S A</t>
@@ -17690,10 +17880,12 @@
       </c>
       <c r="X194" t="inlineStr">
         <is>
-          <t>KG</t>
-        </is>
-      </c>
-      <c r="Y194" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y194" t="n">
+        <v>1.25</v>
+      </c>
       <c r="Z194" t="inlineStr">
         <is>
           <t>CERAMICA LIMA S A</t>
@@ -18005,10 +18197,12 @@
       </c>
       <c r="X197" t="inlineStr">
         <is>
-          <t>KG</t>
-        </is>
-      </c>
-      <c r="Y197" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y197" t="n">
+        <v>0.8709</v>
+      </c>
       <c r="Z197" t="inlineStr">
         <is>
           <t>ECOLAB PERU HOLDINGS S.R.L.</t>
@@ -18110,10 +18304,12 @@
       </c>
       <c r="X198" t="inlineStr">
         <is>
-          <t>KG</t>
-        </is>
-      </c>
-      <c r="Y198" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y198" t="n">
+        <v>11.25</v>
+      </c>
       <c r="Z198" t="inlineStr">
         <is>
           <t>CERAMICA LIMA S A</t>
@@ -18320,10 +18516,12 @@
       </c>
       <c r="X200" t="inlineStr">
         <is>
-          <t>KG</t>
-        </is>
-      </c>
-      <c r="Y200" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y200" t="n">
+        <v>1.4515</v>
+      </c>
       <c r="Z200" t="inlineStr">
         <is>
           <t>ECOLAB PERU HOLDINGS S.R.L.</t>
@@ -18740,10 +18938,12 @@
       </c>
       <c r="X204" t="inlineStr">
         <is>
-          <t>KG</t>
-        </is>
-      </c>
-      <c r="Y204" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y204" t="n">
+        <v>7.5</v>
+      </c>
       <c r="Z204" t="inlineStr">
         <is>
           <t>CERAMICA LIMA S A</t>
@@ -18845,10 +19045,12 @@
       </c>
       <c r="X205" t="inlineStr">
         <is>
-          <t>KG</t>
-        </is>
-      </c>
-      <c r="Y205" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y205" t="n">
+        <v>3.75</v>
+      </c>
       <c r="Z205" t="inlineStr">
         <is>
           <t>CERAMICA LIMA S A</t>
@@ -18950,10 +19152,12 @@
       </c>
       <c r="X206" t="inlineStr">
         <is>
-          <t>KG</t>
-        </is>
-      </c>
-      <c r="Y206" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y206" t="n">
+        <v>11.44</v>
+      </c>
       <c r="Z206" t="inlineStr">
         <is>
           <t>UNITRADE S.A.C.</t>
@@ -20945,10 +21149,12 @@
       </c>
       <c r="X225" t="inlineStr">
         <is>
-          <t>KG</t>
-        </is>
-      </c>
-      <c r="Y225" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y225" t="n">
+        <v>1.4515</v>
+      </c>
       <c r="Z225" t="inlineStr">
         <is>
           <t>ECOLAB PERU HOLDINGS S.R.L.</t>
@@ -21147,10 +21353,12 @@
       </c>
       <c r="X227" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y227" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y227" t="n">
+        <v>3.3</v>
+      </c>
       <c r="Z227" t="inlineStr"/>
       <c r="AA227" t="inlineStr"/>
       <c r="AB227" t="inlineStr"/>
@@ -21232,10 +21440,12 @@
       </c>
       <c r="X228" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y228" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y228" t="n">
+        <v>25.2</v>
+      </c>
       <c r="Z228" t="inlineStr"/>
       <c r="AA228" t="inlineStr"/>
       <c r="AB228" t="inlineStr"/>
@@ -21317,10 +21527,12 @@
       </c>
       <c r="X229" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y229" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y229" t="n">
+        <v>25</v>
+      </c>
       <c r="Z229" t="inlineStr"/>
       <c r="AA229" t="inlineStr"/>
       <c r="AB229" t="inlineStr"/>
@@ -21402,10 +21614,12 @@
       </c>
       <c r="X230" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y230" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y230" t="n">
+        <v>2</v>
+      </c>
       <c r="Z230" t="inlineStr"/>
       <c r="AA230" t="inlineStr"/>
       <c r="AB230" t="inlineStr"/>
@@ -21487,10 +21701,12 @@
       </c>
       <c r="X231" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y231" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y231" t="n">
+        <v>112</v>
+      </c>
       <c r="Z231" t="inlineStr"/>
       <c r="AA231" t="inlineStr"/>
       <c r="AB231" t="inlineStr"/>
@@ -21572,10 +21788,12 @@
       </c>
       <c r="X232" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y232" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y232" t="n">
+        <v>0.065</v>
+      </c>
       <c r="Z232" t="inlineStr"/>
       <c r="AA232" t="inlineStr"/>
       <c r="AB232" t="inlineStr"/>
@@ -21657,10 +21875,12 @@
       </c>
       <c r="X233" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y233" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y233" t="n">
+        <v>1</v>
+      </c>
       <c r="Z233" t="inlineStr"/>
       <c r="AA233" t="inlineStr"/>
       <c r="AB233" t="inlineStr"/>
@@ -21742,10 +21962,12 @@
       </c>
       <c r="X234" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y234" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y234" t="n">
+        <v>0.516</v>
+      </c>
       <c r="Z234" t="inlineStr"/>
       <c r="AA234" t="inlineStr"/>
       <c r="AB234" t="inlineStr"/>
@@ -21827,10 +22049,12 @@
       </c>
       <c r="X235" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y235" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y235" t="n">
+        <v>2.2</v>
+      </c>
       <c r="Z235" t="inlineStr"/>
       <c r="AA235" t="inlineStr"/>
       <c r="AB235" t="inlineStr"/>
@@ -21912,10 +22136,12 @@
       </c>
       <c r="X236" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y236" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y236" t="n">
+        <v>0.8328</v>
+      </c>
       <c r="Z236" t="inlineStr"/>
       <c r="AA236" t="inlineStr"/>
       <c r="AB236" t="inlineStr"/>
@@ -21997,10 +22223,12 @@
       </c>
       <c r="X237" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y237" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y237" t="n">
+        <v>0.065</v>
+      </c>
       <c r="Z237" t="inlineStr"/>
       <c r="AA237" t="inlineStr"/>
       <c r="AB237" t="inlineStr"/>
@@ -22082,10 +22310,12 @@
       </c>
       <c r="X238" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y238" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y238" t="n">
+        <v>25.2</v>
+      </c>
       <c r="Z238" t="inlineStr"/>
       <c r="AA238" t="inlineStr"/>
       <c r="AB238" t="inlineStr"/>
@@ -22167,10 +22397,12 @@
       </c>
       <c r="X239" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y239" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y239" t="n">
+        <v>3.25</v>
+      </c>
       <c r="Z239" t="inlineStr"/>
       <c r="AA239" t="inlineStr"/>
       <c r="AB239" t="inlineStr"/>
@@ -22252,10 +22484,12 @@
       </c>
       <c r="X240" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y240" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y240" t="n">
+        <v>0.06</v>
+      </c>
       <c r="Z240" t="inlineStr"/>
       <c r="AA240" t="inlineStr"/>
       <c r="AB240" t="inlineStr"/>
@@ -22337,10 +22571,12 @@
       </c>
       <c r="X241" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y241" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y241" t="n">
+        <v>0.52</v>
+      </c>
       <c r="Z241" t="inlineStr"/>
       <c r="AA241" t="inlineStr"/>
       <c r="AB241" t="inlineStr"/>
@@ -22422,10 +22658,12 @@
       </c>
       <c r="X242" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y242" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y242" t="n">
+        <v>1.6</v>
+      </c>
       <c r="Z242" t="inlineStr"/>
       <c r="AA242" t="inlineStr"/>
       <c r="AB242" t="inlineStr"/>
@@ -22507,10 +22745,12 @@
       </c>
       <c r="X243" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y243" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y243" t="n">
+        <v>2</v>
+      </c>
       <c r="Z243" t="inlineStr"/>
       <c r="AA243" t="inlineStr"/>
       <c r="AB243" t="inlineStr"/>
@@ -22592,10 +22832,12 @@
       </c>
       <c r="X244" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y244" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y244" t="n">
+        <v>2.2</v>
+      </c>
       <c r="Z244" t="inlineStr"/>
       <c r="AA244" t="inlineStr"/>
       <c r="AB244" t="inlineStr"/>
@@ -22677,10 +22919,12 @@
       </c>
       <c r="X245" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y245" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y245" t="n">
+        <v>1.1</v>
+      </c>
       <c r="Z245" t="inlineStr"/>
       <c r="AA245" t="inlineStr"/>
       <c r="AB245" t="inlineStr"/>
@@ -23025,10 +23269,12 @@
       </c>
       <c r="X249" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y249" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y249" t="n">
+        <v>3.4</v>
+      </c>
       <c r="Z249" t="inlineStr">
         <is>
           <t>TECNIGOM LTDA.</t>
@@ -23292,10 +23538,12 @@
       </c>
       <c r="X252" t="inlineStr">
         <is>
-          <t>KILOGRAMO</t>
-        </is>
-      </c>
-      <c r="Y252" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y252" t="n">
+        <v>1.08</v>
+      </c>
       <c r="Z252" t="inlineStr">
         <is>
           <t>TECNIGOM LTDA.</t>

</xml_diff>

<commit_message>
Argentina completo y ok
</commit_message>
<xml_diff>
--- a/importaciones_unificadas.xlsx
+++ b/importaciones_unificadas.xlsx
@@ -629,7 +629,11 @@
           <t>China</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr"/>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>BS.AS.(CAPITAL)</t>
+        </is>
+      </c>
       <c r="N2" t="inlineStr"/>
       <c r="O2" t="inlineStr">
         <is>
@@ -641,7 +645,9 @@
         <v>14905</v>
       </c>
       <c r="R2" t="inlineStr"/>
-      <c r="S2" t="inlineStr"/>
+      <c r="S2" t="n">
+        <v>573.27</v>
+      </c>
       <c r="T2" t="inlineStr"/>
       <c r="U2" t="inlineStr"/>
       <c r="V2" t="inlineStr"/>
@@ -663,7 +669,11 @@
       </c>
       <c r="AA2" t="inlineStr"/>
       <c r="AB2" t="inlineStr"/>
-      <c r="AC2" t="inlineStr"/>
+      <c r="AC2" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr"/>
@@ -714,7 +724,11 @@
           <t>Brasil</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr"/>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>BS.AS.(CAPITAL)</t>
+        </is>
+      </c>
       <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr">
         <is>
@@ -726,7 +740,9 @@
         <v>6240</v>
       </c>
       <c r="R3" t="inlineStr"/>
-      <c r="S3" t="inlineStr"/>
+      <c r="S3" t="n">
+        <v>960</v>
+      </c>
       <c r="T3" t="inlineStr"/>
       <c r="U3" t="inlineStr"/>
       <c r="V3" t="inlineStr"/>
@@ -748,7 +764,11 @@
       </c>
       <c r="AA3" t="inlineStr"/>
       <c r="AB3" t="inlineStr"/>
-      <c r="AC3" t="inlineStr"/>
+      <c r="AC3" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr"/>
@@ -799,7 +819,11 @@
           <t>Estados Unidos</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr"/>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>BS.AS.(CAPITAL)</t>
+        </is>
+      </c>
       <c r="N4" t="inlineStr"/>
       <c r="O4" t="inlineStr">
         <is>
@@ -831,7 +855,11 @@
       </c>
       <c r="AA4" t="inlineStr"/>
       <c r="AB4" t="inlineStr"/>
-      <c r="AC4" t="inlineStr"/>
+      <c r="AC4" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr"/>
@@ -882,7 +910,11 @@
           <t>España</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr"/>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>BS.AS.(CAPITAL)</t>
+        </is>
+      </c>
       <c r="N5" t="inlineStr"/>
       <c r="O5" t="inlineStr">
         <is>
@@ -894,7 +926,9 @@
         <v>5141.83</v>
       </c>
       <c r="R5" t="inlineStr"/>
-      <c r="S5" t="inlineStr"/>
+      <c r="S5" t="n">
+        <v>571.3099999999999</v>
+      </c>
       <c r="T5" t="inlineStr"/>
       <c r="U5" t="inlineStr"/>
       <c r="V5" t="inlineStr"/>
@@ -916,7 +950,11 @@
       </c>
       <c r="AA5" t="inlineStr"/>
       <c r="AB5" t="inlineStr"/>
-      <c r="AC5" t="inlineStr"/>
+      <c r="AC5" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr"/>
@@ -967,7 +1005,11 @@
           <t>China</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr"/>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>BS.AS.(CAPITAL)</t>
+        </is>
+      </c>
       <c r="N6" t="inlineStr"/>
       <c r="O6" t="inlineStr">
         <is>
@@ -979,7 +1021,9 @@
         <v>23492</v>
       </c>
       <c r="R6" t="inlineStr"/>
-      <c r="S6" t="inlineStr"/>
+      <c r="S6" t="n">
+        <v>839</v>
+      </c>
       <c r="T6" t="inlineStr"/>
       <c r="U6" t="inlineStr"/>
       <c r="V6" t="inlineStr"/>
@@ -1001,7 +1045,11 @@
       </c>
       <c r="AA6" t="inlineStr"/>
       <c r="AB6" t="inlineStr"/>
-      <c r="AC6" t="inlineStr"/>
+      <c r="AC6" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr"/>
@@ -1052,7 +1100,11 @@
           <t>España</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr"/>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>BS.AS.(CAPITAL)</t>
+        </is>
+      </c>
       <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr">
         <is>
@@ -1064,7 +1116,9 @@
         <v>7853.38</v>
       </c>
       <c r="R7" t="inlineStr"/>
-      <c r="S7" t="inlineStr"/>
+      <c r="S7" t="n">
+        <v>604.11</v>
+      </c>
       <c r="T7" t="inlineStr"/>
       <c r="U7" t="inlineStr"/>
       <c r="V7" t="inlineStr"/>
@@ -1086,7 +1140,11 @@
       </c>
       <c r="AA7" t="inlineStr"/>
       <c r="AB7" t="inlineStr"/>
-      <c r="AC7" t="inlineStr"/>
+      <c r="AC7" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
@@ -1137,7 +1195,11 @@
           <t>China</t>
         </is>
       </c>
-      <c r="M8" t="inlineStr"/>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>BS.AS.(CAPITAL)</t>
+        </is>
+      </c>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr">
         <is>
@@ -1169,7 +1231,11 @@
       </c>
       <c r="AA8" t="inlineStr"/>
       <c r="AB8" t="inlineStr"/>
-      <c r="AC8" t="inlineStr"/>
+      <c r="AC8" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr"/>
@@ -1220,7 +1286,11 @@
           <t>China</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr"/>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>BS.AS.(CAPITAL)</t>
+        </is>
+      </c>
       <c r="N9" t="inlineStr"/>
       <c r="O9" t="inlineStr">
         <is>
@@ -1232,7 +1302,9 @@
         <v>14700</v>
       </c>
       <c r="R9" t="inlineStr"/>
-      <c r="S9" t="inlineStr"/>
+      <c r="S9" t="n">
+        <v>565.38</v>
+      </c>
       <c r="T9" t="inlineStr"/>
       <c r="U9" t="inlineStr"/>
       <c r="V9" t="inlineStr"/>
@@ -1254,7 +1326,11 @@
       </c>
       <c r="AA9" t="inlineStr"/>
       <c r="AB9" t="inlineStr"/>
-      <c r="AC9" t="inlineStr"/>
+      <c r="AC9" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr"/>
@@ -1305,7 +1381,11 @@
           <t>Brasil</t>
         </is>
       </c>
-      <c r="M10" t="inlineStr"/>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>BS.AS.(CAPITAL)</t>
+        </is>
+      </c>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr">
         <is>
@@ -1317,7 +1397,9 @@
         <v>5044</v>
       </c>
       <c r="R10" t="inlineStr"/>
-      <c r="S10" t="inlineStr"/>
+      <c r="S10" t="n">
+        <v>970</v>
+      </c>
       <c r="T10" t="inlineStr"/>
       <c r="U10" t="inlineStr"/>
       <c r="V10" t="inlineStr"/>
@@ -1339,7 +1421,11 @@
       </c>
       <c r="AA10" t="inlineStr"/>
       <c r="AB10" t="inlineStr"/>
-      <c r="AC10" t="inlineStr"/>
+      <c r="AC10" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr"/>
@@ -1390,7 +1476,11 @@
           <t>España</t>
         </is>
       </c>
-      <c r="M11" t="inlineStr"/>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>BS.AS.(CAPITAL)</t>
+        </is>
+      </c>
       <c r="N11" t="inlineStr"/>
       <c r="O11" t="inlineStr">
         <is>
@@ -1402,7 +1492,9 @@
         <v>3625.4</v>
       </c>
       <c r="R11" t="inlineStr"/>
-      <c r="S11" t="inlineStr"/>
+      <c r="S11" t="n">
+        <v>604.23</v>
+      </c>
       <c r="T11" t="inlineStr"/>
       <c r="U11" t="inlineStr"/>
       <c r="V11" t="inlineStr"/>
@@ -1424,7 +1516,11 @@
       </c>
       <c r="AA11" t="inlineStr"/>
       <c r="AB11" t="inlineStr"/>
-      <c r="AC11" t="inlineStr"/>
+      <c r="AC11" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr"/>
@@ -1475,7 +1571,11 @@
           <t>España</t>
         </is>
       </c>
-      <c r="M12" t="inlineStr"/>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>BS.AS.(CAPITAL)</t>
+        </is>
+      </c>
       <c r="N12" t="inlineStr"/>
       <c r="O12" t="inlineStr">
         <is>
@@ -1487,7 +1587,9 @@
         <v>1812.7</v>
       </c>
       <c r="R12" t="inlineStr"/>
-      <c r="S12" t="inlineStr"/>
+      <c r="S12" t="n">
+        <v>604.23</v>
+      </c>
       <c r="T12" t="inlineStr"/>
       <c r="U12" t="inlineStr"/>
       <c r="V12" t="inlineStr"/>
@@ -1509,7 +1611,11 @@
       </c>
       <c r="AA12" t="inlineStr"/>
       <c r="AB12" t="inlineStr"/>
-      <c r="AC12" t="inlineStr"/>
+      <c r="AC12" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr"/>
@@ -1560,7 +1666,11 @@
           <t>España</t>
         </is>
       </c>
-      <c r="M13" t="inlineStr"/>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>BS.AS.(CAPITAL)</t>
+        </is>
+      </c>
       <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr">
         <is>
@@ -1572,7 +1682,9 @@
         <v>3625.4</v>
       </c>
       <c r="R13" t="inlineStr"/>
-      <c r="S13" t="inlineStr"/>
+      <c r="S13" t="n">
+        <v>604.23</v>
+      </c>
       <c r="T13" t="inlineStr"/>
       <c r="U13" t="inlineStr"/>
       <c r="V13" t="inlineStr"/>
@@ -1594,7 +1706,11 @@
       </c>
       <c r="AA13" t="inlineStr"/>
       <c r="AB13" t="inlineStr"/>
-      <c r="AC13" t="inlineStr"/>
+      <c r="AC13" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr"/>
@@ -1645,7 +1761,11 @@
           <t>China</t>
         </is>
       </c>
-      <c r="M14" t="inlineStr"/>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>BS.AS.(CAPITAL)</t>
+        </is>
+      </c>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="inlineStr">
         <is>
@@ -1657,7 +1777,9 @@
         <v>23492</v>
       </c>
       <c r="R14" t="inlineStr"/>
-      <c r="S14" t="inlineStr"/>
+      <c r="S14" t="n">
+        <v>839</v>
+      </c>
       <c r="T14" t="inlineStr"/>
       <c r="U14" t="inlineStr"/>
       <c r="V14" t="inlineStr"/>
@@ -1679,7 +1801,11 @@
       </c>
       <c r="AA14" t="inlineStr"/>
       <c r="AB14" t="inlineStr"/>
-      <c r="AC14" t="inlineStr"/>
+      <c r="AC14" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr"/>
@@ -1730,7 +1856,11 @@
           <t>China</t>
         </is>
       </c>
-      <c r="M15" t="inlineStr"/>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>BS.AS.(CAPITAL)</t>
+        </is>
+      </c>
       <c r="N15" t="inlineStr"/>
       <c r="O15" t="inlineStr">
         <is>
@@ -1742,7 +1872,9 @@
         <v>14725.8</v>
       </c>
       <c r="R15" t="inlineStr"/>
-      <c r="S15" t="inlineStr"/>
+      <c r="S15" t="n">
+        <v>545.4</v>
+      </c>
       <c r="T15" t="inlineStr"/>
       <c r="U15" t="inlineStr"/>
       <c r="V15" t="inlineStr"/>
@@ -1764,7 +1896,11 @@
       </c>
       <c r="AA15" t="inlineStr"/>
       <c r="AB15" t="inlineStr"/>
-      <c r="AC15" t="inlineStr"/>
+      <c r="AC15" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr"/>
@@ -1815,7 +1951,11 @@
           <t>Chile</t>
         </is>
       </c>
-      <c r="M16" t="inlineStr"/>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>BS.AS.(CAPITAL)</t>
+        </is>
+      </c>
       <c r="N16" t="inlineStr"/>
       <c r="O16" t="inlineStr">
         <is>
@@ -1827,7 +1967,9 @@
         <v>2010</v>
       </c>
       <c r="R16" t="inlineStr"/>
-      <c r="S16" t="inlineStr"/>
+      <c r="S16" t="n">
+        <v>670</v>
+      </c>
       <c r="T16" t="inlineStr"/>
       <c r="U16" t="inlineStr"/>
       <c r="V16" t="inlineStr"/>
@@ -1849,7 +1991,11 @@
       </c>
       <c r="AA16" t="inlineStr"/>
       <c r="AB16" t="inlineStr"/>
-      <c r="AC16" t="inlineStr"/>
+      <c r="AC16" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr"/>
@@ -1900,7 +2046,11 @@
           <t>China</t>
         </is>
       </c>
-      <c r="M17" t="inlineStr"/>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>BS.AS.(CAPITAL)</t>
+        </is>
+      </c>
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="inlineStr">
         <is>
@@ -1912,7 +2062,9 @@
         <v>23492</v>
       </c>
       <c r="R17" t="inlineStr"/>
-      <c r="S17" t="inlineStr"/>
+      <c r="S17" t="n">
+        <v>839</v>
+      </c>
       <c r="T17" t="inlineStr"/>
       <c r="U17" t="inlineStr"/>
       <c r="V17" t="inlineStr"/>
@@ -1934,7 +2086,11 @@
       </c>
       <c r="AA17" t="inlineStr"/>
       <c r="AB17" t="inlineStr"/>
-      <c r="AC17" t="inlineStr"/>
+      <c r="AC17" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr"/>
@@ -1985,7 +2141,11 @@
           <t>China</t>
         </is>
       </c>
-      <c r="M18" t="inlineStr"/>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>BS.AS.(CAPITAL)</t>
+        </is>
+      </c>
       <c r="N18" t="inlineStr"/>
       <c r="O18" t="inlineStr">
         <is>
@@ -1997,7 +2157,9 @@
         <v>14040</v>
       </c>
       <c r="R18" t="inlineStr"/>
-      <c r="S18" t="inlineStr"/>
+      <c r="S18" t="n">
+        <v>540</v>
+      </c>
       <c r="T18" t="inlineStr"/>
       <c r="U18" t="inlineStr"/>
       <c r="V18" t="inlineStr"/>
@@ -2019,7 +2181,11 @@
       </c>
       <c r="AA18" t="inlineStr"/>
       <c r="AB18" t="inlineStr"/>
-      <c r="AC18" t="inlineStr"/>
+      <c r="AC18" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr"/>
@@ -2070,7 +2236,11 @@
           <t>España</t>
         </is>
       </c>
-      <c r="M19" t="inlineStr"/>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>BS.AS.(CAPITAL)</t>
+        </is>
+      </c>
       <c r="N19" t="inlineStr"/>
       <c r="O19" t="inlineStr">
         <is>
@@ -2082,7 +2252,9 @@
         <v>2848.89</v>
       </c>
       <c r="R19" t="inlineStr"/>
-      <c r="S19" t="inlineStr"/>
+      <c r="S19" t="n">
+        <v>712.22</v>
+      </c>
       <c r="T19" t="inlineStr"/>
       <c r="U19" t="inlineStr"/>
       <c r="V19" t="inlineStr"/>
@@ -2104,7 +2276,11 @@
       </c>
       <c r="AA19" t="inlineStr"/>
       <c r="AB19" t="inlineStr"/>
-      <c r="AC19" t="inlineStr"/>
+      <c r="AC19" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr"/>
@@ -2155,7 +2331,11 @@
           <t>España</t>
         </is>
       </c>
-      <c r="M20" t="inlineStr"/>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>BS.AS.(CAPITAL)</t>
+        </is>
+      </c>
       <c r="N20" t="inlineStr"/>
       <c r="O20" t="inlineStr">
         <is>
@@ -2167,7 +2347,9 @@
         <v>2848.89</v>
       </c>
       <c r="R20" t="inlineStr"/>
-      <c r="S20" t="inlineStr"/>
+      <c r="S20" t="n">
+        <v>712.22</v>
+      </c>
       <c r="T20" t="inlineStr"/>
       <c r="U20" t="inlineStr"/>
       <c r="V20" t="inlineStr"/>
@@ -2189,7 +2371,11 @@
       </c>
       <c r="AA20" t="inlineStr"/>
       <c r="AB20" t="inlineStr"/>
-      <c r="AC20" t="inlineStr"/>
+      <c r="AC20" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr"/>
@@ -2240,7 +2426,11 @@
           <t>Brasil</t>
         </is>
       </c>
-      <c r="M21" t="inlineStr"/>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>BS.AS.(CAPITAL)</t>
+        </is>
+      </c>
       <c r="N21" t="inlineStr"/>
       <c r="O21" t="inlineStr">
         <is>
@@ -2252,7 +2442,9 @@
         <v>5044</v>
       </c>
       <c r="R21" t="inlineStr"/>
-      <c r="S21" t="inlineStr"/>
+      <c r="S21" t="n">
+        <v>970</v>
+      </c>
       <c r="T21" t="inlineStr"/>
       <c r="U21" t="inlineStr"/>
       <c r="V21" t="inlineStr"/>
@@ -2274,7 +2466,11 @@
       </c>
       <c r="AA21" t="inlineStr"/>
       <c r="AB21" t="inlineStr"/>
-      <c r="AC21" t="inlineStr"/>
+      <c r="AC21" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr"/>
@@ -2325,7 +2521,11 @@
           <t>Brasil</t>
         </is>
       </c>
-      <c r="M22" t="inlineStr"/>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>BS.AS.(CAPITAL)</t>
+        </is>
+      </c>
       <c r="N22" t="inlineStr"/>
       <c r="O22" t="inlineStr">
         <is>
@@ -2337,7 +2537,9 @@
         <v>6258</v>
       </c>
       <c r="R22" t="inlineStr"/>
-      <c r="S22" t="inlineStr"/>
+      <c r="S22" t="n">
+        <v>625.8</v>
+      </c>
       <c r="T22" t="inlineStr"/>
       <c r="U22" t="inlineStr"/>
       <c r="V22" t="inlineStr"/>
@@ -2359,7 +2561,11 @@
       </c>
       <c r="AA22" t="inlineStr"/>
       <c r="AB22" t="inlineStr"/>
-      <c r="AC22" t="inlineStr"/>
+      <c r="AC22" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr"/>
@@ -2410,7 +2616,11 @@
           <t>China</t>
         </is>
       </c>
-      <c r="M23" t="inlineStr"/>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>BS.AS.(CAPITAL)</t>
+        </is>
+      </c>
       <c r="N23" t="inlineStr"/>
       <c r="O23" t="inlineStr">
         <is>
@@ -2422,7 +2632,9 @@
         <v>13780</v>
       </c>
       <c r="R23" t="inlineStr"/>
-      <c r="S23" t="inlineStr"/>
+      <c r="S23" t="n">
+        <v>530</v>
+      </c>
       <c r="T23" t="inlineStr"/>
       <c r="U23" t="inlineStr"/>
       <c r="V23" t="inlineStr"/>
@@ -2444,7 +2656,11 @@
       </c>
       <c r="AA23" t="inlineStr"/>
       <c r="AB23" t="inlineStr"/>
-      <c r="AC23" t="inlineStr"/>
+      <c r="AC23" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr"/>
@@ -2495,7 +2711,11 @@
           <t>Suiza</t>
         </is>
       </c>
-      <c r="M24" t="inlineStr"/>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>BS.AS.(CAPITAL)</t>
+        </is>
+      </c>
       <c r="N24" t="inlineStr"/>
       <c r="O24" t="inlineStr">
         <is>
@@ -2527,7 +2747,11 @@
       </c>
       <c r="AA24" t="inlineStr"/>
       <c r="AB24" t="inlineStr"/>
-      <c r="AC24" t="inlineStr"/>
+      <c r="AC24" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr"/>
@@ -2578,7 +2802,11 @@
           <t>Brasil</t>
         </is>
       </c>
-      <c r="M25" t="inlineStr"/>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>BS.AS.(CAPITAL)</t>
+        </is>
+      </c>
       <c r="N25" t="inlineStr"/>
       <c r="O25" t="inlineStr">
         <is>
@@ -2590,7 +2818,9 @@
         <v>8827</v>
       </c>
       <c r="R25" t="inlineStr"/>
-      <c r="S25" t="inlineStr"/>
+      <c r="S25" t="n">
+        <v>970</v>
+      </c>
       <c r="T25" t="inlineStr"/>
       <c r="U25" t="inlineStr"/>
       <c r="V25" t="inlineStr"/>
@@ -2612,7 +2842,11 @@
       </c>
       <c r="AA25" t="inlineStr"/>
       <c r="AB25" t="inlineStr"/>
-      <c r="AC25" t="inlineStr"/>
+      <c r="AC25" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr"/>
@@ -2663,7 +2897,11 @@
           <t>China</t>
         </is>
       </c>
-      <c r="M26" t="inlineStr"/>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>BS.AS.(CAPITAL)</t>
+        </is>
+      </c>
       <c r="N26" t="inlineStr"/>
       <c r="O26" t="inlineStr">
         <is>
@@ -2675,7 +2913,9 @@
         <v>23492</v>
       </c>
       <c r="R26" t="inlineStr"/>
-      <c r="S26" t="inlineStr"/>
+      <c r="S26" t="n">
+        <v>839</v>
+      </c>
       <c r="T26" t="inlineStr"/>
       <c r="U26" t="inlineStr"/>
       <c r="V26" t="inlineStr"/>
@@ -2697,7 +2937,11 @@
       </c>
       <c r="AA26" t="inlineStr"/>
       <c r="AB26" t="inlineStr"/>
-      <c r="AC26" t="inlineStr"/>
+      <c r="AC26" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr"/>
@@ -2748,7 +2992,11 @@
           <t>España</t>
         </is>
       </c>
-      <c r="M27" t="inlineStr"/>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>BS.AS.(CAPITAL)</t>
+        </is>
+      </c>
       <c r="N27" t="inlineStr"/>
       <c r="O27" t="inlineStr">
         <is>
@@ -2760,7 +3008,9 @@
         <v>3311.53</v>
       </c>
       <c r="R27" t="inlineStr"/>
-      <c r="S27" t="inlineStr"/>
+      <c r="S27" t="n">
+        <v>551.92</v>
+      </c>
       <c r="T27" t="inlineStr"/>
       <c r="U27" t="inlineStr"/>
       <c r="V27" t="inlineStr"/>
@@ -2782,7 +3032,11 @@
       </c>
       <c r="AA27" t="inlineStr"/>
       <c r="AB27" t="inlineStr"/>
-      <c r="AC27" t="inlineStr"/>
+      <c r="AC27" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr"/>
@@ -2833,7 +3087,11 @@
           <t>España</t>
         </is>
       </c>
-      <c r="M28" t="inlineStr"/>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>BS.AS.(CAPITAL)</t>
+        </is>
+      </c>
       <c r="N28" t="inlineStr"/>
       <c r="O28" t="inlineStr">
         <is>
@@ -2845,7 +3103,9 @@
         <v>3438.9</v>
       </c>
       <c r="R28" t="inlineStr"/>
-      <c r="S28" t="inlineStr"/>
+      <c r="S28" t="n">
+        <v>573.15</v>
+      </c>
       <c r="T28" t="inlineStr"/>
       <c r="U28" t="inlineStr"/>
       <c r="V28" t="inlineStr"/>
@@ -2867,7 +3127,11 @@
       </c>
       <c r="AA28" t="inlineStr"/>
       <c r="AB28" t="inlineStr"/>
-      <c r="AC28" t="inlineStr"/>
+      <c r="AC28" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr"/>
@@ -2918,7 +3182,11 @@
           <t>España</t>
         </is>
       </c>
-      <c r="M29" t="inlineStr"/>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>BS.AS.(CAPITAL)</t>
+        </is>
+      </c>
       <c r="N29" t="inlineStr"/>
       <c r="O29" t="inlineStr">
         <is>
@@ -2930,7 +3198,9 @@
         <v>3329.05</v>
       </c>
       <c r="R29" t="inlineStr"/>
-      <c r="S29" t="inlineStr"/>
+      <c r="S29" t="n">
+        <v>554.84</v>
+      </c>
       <c r="T29" t="inlineStr"/>
       <c r="U29" t="inlineStr"/>
       <c r="V29" t="inlineStr"/>
@@ -2952,7 +3222,11 @@
       </c>
       <c r="AA29" t="inlineStr"/>
       <c r="AB29" t="inlineStr"/>
-      <c r="AC29" t="inlineStr"/>
+      <c r="AC29" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr"/>
@@ -3003,7 +3277,11 @@
           <t>España</t>
         </is>
       </c>
-      <c r="M30" t="inlineStr"/>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>BS.AS.(CAPITAL)</t>
+        </is>
+      </c>
       <c r="N30" t="inlineStr"/>
       <c r="O30" t="inlineStr">
         <is>
@@ -3015,7 +3293,9 @@
         <v>3456.17</v>
       </c>
       <c r="R30" t="inlineStr"/>
-      <c r="S30" t="inlineStr"/>
+      <c r="S30" t="n">
+        <v>576.03</v>
+      </c>
       <c r="T30" t="inlineStr"/>
       <c r="U30" t="inlineStr"/>
       <c r="V30" t="inlineStr"/>
@@ -3037,7 +3317,11 @@
       </c>
       <c r="AA30" t="inlineStr"/>
       <c r="AB30" t="inlineStr"/>
-      <c r="AC30" t="inlineStr"/>
+      <c r="AC30" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr"/>
@@ -3088,7 +3372,11 @@
           <t>España</t>
         </is>
       </c>
-      <c r="M31" t="inlineStr"/>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>BS.AS.(CAPITAL)</t>
+        </is>
+      </c>
       <c r="N31" t="inlineStr"/>
       <c r="O31" t="inlineStr">
         <is>
@@ -3100,7 +3388,9 @@
         <v>3580.73</v>
       </c>
       <c r="R31" t="inlineStr"/>
-      <c r="S31" t="inlineStr"/>
+      <c r="S31" t="n">
+        <v>596.79</v>
+      </c>
       <c r="T31" t="inlineStr"/>
       <c r="U31" t="inlineStr"/>
       <c r="V31" t="inlineStr"/>
@@ -3122,7 +3412,11 @@
       </c>
       <c r="AA31" t="inlineStr"/>
       <c r="AB31" t="inlineStr"/>
-      <c r="AC31" t="inlineStr"/>
+      <c r="AC31" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr"/>
@@ -3173,7 +3467,11 @@
           <t>España</t>
         </is>
       </c>
-      <c r="M32" t="inlineStr"/>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>BS.AS.(CAPITAL)</t>
+        </is>
+      </c>
       <c r="N32" t="inlineStr"/>
       <c r="O32" t="inlineStr">
         <is>
@@ -3185,7 +3483,9 @@
         <v>3531.3</v>
       </c>
       <c r="R32" t="inlineStr"/>
-      <c r="S32" t="inlineStr"/>
+      <c r="S32" t="n">
+        <v>588.55</v>
+      </c>
       <c r="T32" t="inlineStr"/>
       <c r="U32" t="inlineStr"/>
       <c r="V32" t="inlineStr"/>
@@ -3207,7 +3507,11 @@
       </c>
       <c r="AA32" t="inlineStr"/>
       <c r="AB32" t="inlineStr"/>
-      <c r="AC32" t="inlineStr"/>
+      <c r="AC32" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr"/>
@@ -3258,7 +3562,11 @@
           <t>España</t>
         </is>
       </c>
-      <c r="M33" t="inlineStr"/>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>BS.AS.(CAPITAL)</t>
+        </is>
+      </c>
       <c r="N33" t="inlineStr"/>
       <c r="O33" t="inlineStr">
         <is>
@@ -3270,7 +3578,9 @@
         <v>3560.4</v>
       </c>
       <c r="R33" t="inlineStr"/>
-      <c r="S33" t="inlineStr"/>
+      <c r="S33" t="n">
+        <v>593.4</v>
+      </c>
       <c r="T33" t="inlineStr"/>
       <c r="U33" t="inlineStr"/>
       <c r="V33" t="inlineStr"/>
@@ -3292,7 +3602,11 @@
       </c>
       <c r="AA33" t="inlineStr"/>
       <c r="AB33" t="inlineStr"/>
-      <c r="AC33" t="inlineStr"/>
+      <c r="AC33" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr"/>
@@ -3343,7 +3657,11 @@
           <t>China</t>
         </is>
       </c>
-      <c r="M34" t="inlineStr"/>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>CORDOBA</t>
+        </is>
+      </c>
       <c r="N34" t="inlineStr"/>
       <c r="O34" t="inlineStr">
         <is>
@@ -3355,7 +3673,9 @@
         <v>60</v>
       </c>
       <c r="R34" t="inlineStr"/>
-      <c r="S34" t="inlineStr"/>
+      <c r="S34" t="n">
+        <v>300</v>
+      </c>
       <c r="T34" t="inlineStr"/>
       <c r="U34" t="inlineStr"/>
       <c r="V34" t="inlineStr"/>
@@ -3377,7 +3697,11 @@
       </c>
       <c r="AA34" t="inlineStr"/>
       <c r="AB34" t="inlineStr"/>
-      <c r="AC34" t="inlineStr"/>
+      <c r="AC34" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr"/>
@@ -3428,7 +3752,11 @@
           <t>Brasil</t>
         </is>
       </c>
-      <c r="M35" t="inlineStr"/>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>PASO DE LOS LIBRES</t>
+        </is>
+      </c>
       <c r="N35" t="inlineStr"/>
       <c r="O35" t="inlineStr">
         <is>
@@ -3440,7 +3768,9 @@
         <v>12750</v>
       </c>
       <c r="R35" t="inlineStr"/>
-      <c r="S35" t="inlineStr"/>
+      <c r="S35" t="n">
+        <v>250</v>
+      </c>
       <c r="T35" t="inlineStr"/>
       <c r="U35" t="inlineStr"/>
       <c r="V35" t="inlineStr"/>
@@ -3462,7 +3792,11 @@
       </c>
       <c r="AA35" t="inlineStr"/>
       <c r="AB35" t="inlineStr"/>
-      <c r="AC35" t="inlineStr"/>
+      <c r="AC35" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr"/>
@@ -3513,7 +3847,11 @@
           <t>Brasil</t>
         </is>
       </c>
-      <c r="M36" t="inlineStr"/>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>PASO DE LOS LIBRES</t>
+        </is>
+      </c>
       <c r="N36" t="inlineStr"/>
       <c r="O36" t="inlineStr">
         <is>
@@ -3525,7 +3863,9 @@
         <v>12750</v>
       </c>
       <c r="R36" t="inlineStr"/>
-      <c r="S36" t="inlineStr"/>
+      <c r="S36" t="n">
+        <v>250</v>
+      </c>
       <c r="T36" t="inlineStr"/>
       <c r="U36" t="inlineStr"/>
       <c r="V36" t="inlineStr"/>
@@ -3547,7 +3887,11 @@
       </c>
       <c r="AA36" t="inlineStr"/>
       <c r="AB36" t="inlineStr"/>
-      <c r="AC36" t="inlineStr"/>
+      <c r="AC36" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr"/>
@@ -3598,7 +3942,11 @@
           <t>Brasil</t>
         </is>
       </c>
-      <c r="M37" t="inlineStr"/>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>PASO DE LOS LIBRES</t>
+        </is>
+      </c>
       <c r="N37" t="inlineStr"/>
       <c r="O37" t="inlineStr">
         <is>
@@ -3610,7 +3958,9 @@
         <v>15228</v>
       </c>
       <c r="R37" t="inlineStr"/>
-      <c r="S37" t="inlineStr"/>
+      <c r="S37" t="n">
+        <v>282</v>
+      </c>
       <c r="T37" t="inlineStr"/>
       <c r="U37" t="inlineStr"/>
       <c r="V37" t="inlineStr"/>
@@ -3632,7 +3982,11 @@
       </c>
       <c r="AA37" t="inlineStr"/>
       <c r="AB37" t="inlineStr"/>
-      <c r="AC37" t="inlineStr"/>
+      <c r="AC37" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr"/>
@@ -3683,7 +4037,11 @@
           <t>Brasil</t>
         </is>
       </c>
-      <c r="M38" t="inlineStr"/>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>PASO DE LOS LIBRES</t>
+        </is>
+      </c>
       <c r="N38" t="inlineStr"/>
       <c r="O38" t="inlineStr">
         <is>
@@ -3695,7 +4053,9 @@
         <v>10710</v>
       </c>
       <c r="R38" t="inlineStr"/>
-      <c r="S38" t="inlineStr"/>
+      <c r="S38" t="n">
+        <v>210</v>
+      </c>
       <c r="T38" t="inlineStr"/>
       <c r="U38" t="inlineStr"/>
       <c r="V38" t="inlineStr"/>
@@ -3717,7 +4077,11 @@
       </c>
       <c r="AA38" t="inlineStr"/>
       <c r="AB38" t="inlineStr"/>
-      <c r="AC38" t="inlineStr"/>
+      <c r="AC38" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr"/>
@@ -3768,7 +4132,11 @@
           <t>Brasil</t>
         </is>
       </c>
-      <c r="M39" t="inlineStr"/>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>PASO DE LOS LIBRES</t>
+        </is>
+      </c>
       <c r="N39" t="inlineStr"/>
       <c r="O39" t="inlineStr">
         <is>
@@ -3780,7 +4148,9 @@
         <v>10710</v>
       </c>
       <c r="R39" t="inlineStr"/>
-      <c r="S39" t="inlineStr"/>
+      <c r="S39" t="n">
+        <v>210</v>
+      </c>
       <c r="T39" t="inlineStr"/>
       <c r="U39" t="inlineStr"/>
       <c r="V39" t="inlineStr"/>
@@ -3802,7 +4172,11 @@
       </c>
       <c r="AA39" t="inlineStr"/>
       <c r="AB39" t="inlineStr"/>
-      <c r="AC39" t="inlineStr"/>
+      <c r="AC39" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr"/>
@@ -3853,7 +4227,11 @@
           <t>Brasil</t>
         </is>
       </c>
-      <c r="M40" t="inlineStr"/>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>PASO DE LOS LIBRES</t>
+        </is>
+      </c>
       <c r="N40" t="inlineStr"/>
       <c r="O40" t="inlineStr">
         <is>
@@ -3865,7 +4243,9 @@
         <v>13608</v>
       </c>
       <c r="R40" t="inlineStr"/>
-      <c r="S40" t="inlineStr"/>
+      <c r="S40" t="n">
+        <v>270</v>
+      </c>
       <c r="T40" t="inlineStr"/>
       <c r="U40" t="inlineStr"/>
       <c r="V40" t="inlineStr"/>
@@ -3887,7 +4267,11 @@
       </c>
       <c r="AA40" t="inlineStr"/>
       <c r="AB40" t="inlineStr"/>
-      <c r="AC40" t="inlineStr"/>
+      <c r="AC40" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr"/>
@@ -3938,7 +4322,11 @@
           <t>Brasil</t>
         </is>
       </c>
-      <c r="M41" t="inlineStr"/>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>PASO DE LOS LIBRES</t>
+        </is>
+      </c>
       <c r="N41" t="inlineStr"/>
       <c r="O41" t="inlineStr">
         <is>
@@ -3950,7 +4338,9 @@
         <v>339.6</v>
       </c>
       <c r="R41" t="inlineStr"/>
-      <c r="S41" t="inlineStr"/>
+      <c r="S41" t="n">
+        <v>1698</v>
+      </c>
       <c r="T41" t="inlineStr"/>
       <c r="U41" t="inlineStr"/>
       <c r="V41" t="inlineStr"/>
@@ -3972,7 +4362,11 @@
       </c>
       <c r="AA41" t="inlineStr"/>
       <c r="AB41" t="inlineStr"/>
-      <c r="AC41" t="inlineStr"/>
+      <c r="AC41" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr"/>
@@ -4023,7 +4417,11 @@
           <t>Brasil</t>
         </is>
       </c>
-      <c r="M42" t="inlineStr"/>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>PASO DE LOS LIBRES</t>
+        </is>
+      </c>
       <c r="N42" t="inlineStr"/>
       <c r="O42" t="inlineStr">
         <is>
@@ -4035,7 +4433,9 @@
         <v>8600</v>
       </c>
       <c r="R42" t="inlineStr"/>
-      <c r="S42" t="inlineStr"/>
+      <c r="S42" t="n">
+        <v>2500</v>
+      </c>
       <c r="T42" t="inlineStr"/>
       <c r="U42" t="inlineStr"/>
       <c r="V42" t="inlineStr"/>
@@ -4057,7 +4457,11 @@
       </c>
       <c r="AA42" t="inlineStr"/>
       <c r="AB42" t="inlineStr"/>
-      <c r="AC42" t="inlineStr"/>
+      <c r="AC42" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr"/>
@@ -4108,7 +4512,11 @@
           <t>Brasil</t>
         </is>
       </c>
-      <c r="M43" t="inlineStr"/>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>PASO DE LOS LIBRES</t>
+        </is>
+      </c>
       <c r="N43" t="inlineStr"/>
       <c r="O43" t="inlineStr">
         <is>
@@ -4120,7 +4528,9 @@
         <v>7308</v>
       </c>
       <c r="R43" t="inlineStr"/>
-      <c r="S43" t="inlineStr"/>
+      <c r="S43" t="n">
+        <v>290</v>
+      </c>
       <c r="T43" t="inlineStr"/>
       <c r="U43" t="inlineStr"/>
       <c r="V43" t="inlineStr"/>
@@ -4142,7 +4552,11 @@
       </c>
       <c r="AA43" t="inlineStr"/>
       <c r="AB43" t="inlineStr"/>
-      <c r="AC43" t="inlineStr"/>
+      <c r="AC43" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr"/>
@@ -4193,7 +4607,11 @@
           <t>Brasil</t>
         </is>
       </c>
-      <c r="M44" t="inlineStr"/>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>PASO DE LOS LIBRES</t>
+        </is>
+      </c>
       <c r="N44" t="inlineStr"/>
       <c r="O44" t="inlineStr">
         <is>
@@ -4205,7 +4623,9 @@
         <v>339.6</v>
       </c>
       <c r="R44" t="inlineStr"/>
-      <c r="S44" t="inlineStr"/>
+      <c r="S44" t="n">
+        <v>1698</v>
+      </c>
       <c r="T44" t="inlineStr"/>
       <c r="U44" t="inlineStr"/>
       <c r="V44" t="inlineStr"/>
@@ -4227,7 +4647,11 @@
       </c>
       <c r="AA44" t="inlineStr"/>
       <c r="AB44" t="inlineStr"/>
-      <c r="AC44" t="inlineStr"/>
+      <c r="AC44" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr"/>
@@ -4278,7 +4702,11 @@
           <t>Brasil</t>
         </is>
       </c>
-      <c r="M45" t="inlineStr"/>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>PASO DE LOS LIBRES</t>
+        </is>
+      </c>
       <c r="N45" t="inlineStr"/>
       <c r="O45" t="inlineStr">
         <is>
@@ -4290,7 +4718,9 @@
         <v>100</v>
       </c>
       <c r="R45" t="inlineStr"/>
-      <c r="S45" t="inlineStr"/>
+      <c r="S45" t="n">
+        <v>1250</v>
+      </c>
       <c r="T45" t="inlineStr"/>
       <c r="U45" t="inlineStr"/>
       <c r="V45" t="inlineStr"/>
@@ -4312,7 +4742,11 @@
       </c>
       <c r="AA45" t="inlineStr"/>
       <c r="AB45" t="inlineStr"/>
-      <c r="AC45" t="inlineStr"/>
+      <c r="AC45" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr"/>
@@ -4363,7 +4797,11 @@
           <t>Brasil</t>
         </is>
       </c>
-      <c r="M46" t="inlineStr"/>
+      <c r="M46" t="inlineStr">
+        <is>
+          <t>PASO DE LOS LIBRES</t>
+        </is>
+      </c>
       <c r="N46" t="inlineStr"/>
       <c r="O46" t="inlineStr">
         <is>
@@ -4375,7 +4813,9 @@
         <v>9600</v>
       </c>
       <c r="R46" t="inlineStr"/>
-      <c r="S46" t="inlineStr"/>
+      <c r="S46" t="n">
+        <v>2500</v>
+      </c>
       <c r="T46" t="inlineStr"/>
       <c r="U46" t="inlineStr"/>
       <c r="V46" t="inlineStr"/>
@@ -4397,7 +4837,11 @@
       </c>
       <c r="AA46" t="inlineStr"/>
       <c r="AB46" t="inlineStr"/>
-      <c r="AC46" t="inlineStr"/>
+      <c r="AC46" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr"/>
@@ -4448,7 +4892,11 @@
           <t>Brasil</t>
         </is>
       </c>
-      <c r="M47" t="inlineStr"/>
+      <c r="M47" t="inlineStr">
+        <is>
+          <t>ROSARIO</t>
+        </is>
+      </c>
       <c r="N47" t="inlineStr"/>
       <c r="O47" t="inlineStr">
         <is>
@@ -4460,7 +4908,9 @@
         <v>2682</v>
       </c>
       <c r="R47" t="inlineStr"/>
-      <c r="S47" t="inlineStr"/>
+      <c r="S47" t="n">
+        <v>670.5</v>
+      </c>
       <c r="T47" t="inlineStr"/>
       <c r="U47" t="inlineStr"/>
       <c r="V47" t="inlineStr"/>
@@ -4482,7 +4932,11 @@
       </c>
       <c r="AA47" t="inlineStr"/>
       <c r="AB47" t="inlineStr"/>
-      <c r="AC47" t="inlineStr"/>
+      <c r="AC47" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr"/>
@@ -4533,7 +4987,11 @@
           <t>Estados Unidos</t>
         </is>
       </c>
-      <c r="M48" t="inlineStr"/>
+      <c r="M48" t="inlineStr">
+        <is>
+          <t>EZEIZA</t>
+        </is>
+      </c>
       <c r="N48" t="inlineStr"/>
       <c r="O48" t="inlineStr">
         <is>
@@ -4565,7 +5023,11 @@
       </c>
       <c r="AA48" t="inlineStr"/>
       <c r="AB48" t="inlineStr"/>
-      <c r="AC48" t="inlineStr"/>
+      <c r="AC48" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr"/>
@@ -4616,7 +5078,11 @@
           <t>España</t>
         </is>
       </c>
-      <c r="M49" t="inlineStr"/>
+      <c r="M49" t="inlineStr">
+        <is>
+          <t>EZEIZA</t>
+        </is>
+      </c>
       <c r="N49" t="inlineStr"/>
       <c r="O49" t="inlineStr">
         <is>
@@ -4628,7 +5094,9 @@
         <v>11.34</v>
       </c>
       <c r="R49" t="inlineStr"/>
-      <c r="S49" t="inlineStr"/>
+      <c r="S49" t="n">
+        <v>11340</v>
+      </c>
       <c r="T49" t="inlineStr"/>
       <c r="U49" t="inlineStr"/>
       <c r="V49" t="inlineStr"/>
@@ -4650,7 +5118,11 @@
       </c>
       <c r="AA49" t="inlineStr"/>
       <c r="AB49" t="inlineStr"/>
-      <c r="AC49" t="inlineStr"/>
+      <c r="AC49" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr"/>
@@ -4701,7 +5173,11 @@
           <t>Australia</t>
         </is>
       </c>
-      <c r="M50" t="inlineStr"/>
+      <c r="M50" t="inlineStr">
+        <is>
+          <t>EZEIZA</t>
+        </is>
+      </c>
       <c r="N50" t="inlineStr"/>
       <c r="O50" t="inlineStr">
         <is>
@@ -4713,7 +5189,9 @@
         <v>1</v>
       </c>
       <c r="R50" t="inlineStr"/>
-      <c r="S50" t="inlineStr"/>
+      <c r="S50" t="n">
+        <v>1000</v>
+      </c>
       <c r="T50" t="inlineStr"/>
       <c r="U50" t="inlineStr"/>
       <c r="V50" t="inlineStr"/>
@@ -4735,7 +5213,11 @@
       </c>
       <c r="AA50" t="inlineStr"/>
       <c r="AB50" t="inlineStr"/>
-      <c r="AC50" t="inlineStr"/>
+      <c r="AC50" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr"/>
@@ -4786,7 +5268,11 @@
           <t>Estados Unidos</t>
         </is>
       </c>
-      <c r="M51" t="inlineStr"/>
+      <c r="M51" t="inlineStr">
+        <is>
+          <t>EZEIZA</t>
+        </is>
+      </c>
       <c r="N51" t="inlineStr"/>
       <c r="O51" t="inlineStr">
         <is>
@@ -4818,7 +5304,11 @@
       </c>
       <c r="AA51" t="inlineStr"/>
       <c r="AB51" t="inlineStr"/>
-      <c r="AC51" t="inlineStr"/>
+      <c r="AC51" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr"/>
@@ -4869,7 +5359,11 @@
           <t>Estados Unidos</t>
         </is>
       </c>
-      <c r="M52" t="inlineStr"/>
+      <c r="M52" t="inlineStr">
+        <is>
+          <t>EZEIZA</t>
+        </is>
+      </c>
       <c r="N52" t="inlineStr"/>
       <c r="O52" t="inlineStr">
         <is>
@@ -4903,7 +5397,11 @@
       </c>
       <c r="AA52" t="inlineStr"/>
       <c r="AB52" t="inlineStr"/>
-      <c r="AC52" t="inlineStr"/>
+      <c r="AC52" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr"/>
@@ -4954,7 +5452,11 @@
           <t>Brasil</t>
         </is>
       </c>
-      <c r="M53" t="inlineStr"/>
+      <c r="M53" t="inlineStr">
+        <is>
+          <t>SANTO TOME</t>
+        </is>
+      </c>
       <c r="N53" t="inlineStr"/>
       <c r="O53" t="inlineStr">
         <is>
@@ -4966,7 +5468,9 @@
         <v>734.4</v>
       </c>
       <c r="R53" t="inlineStr"/>
-      <c r="S53" t="inlineStr"/>
+      <c r="S53" t="n">
+        <v>1360</v>
+      </c>
       <c r="T53" t="inlineStr"/>
       <c r="U53" t="inlineStr"/>
       <c r="V53" t="inlineStr"/>
@@ -4988,7 +5492,11 @@
       </c>
       <c r="AA53" t="inlineStr"/>
       <c r="AB53" t="inlineStr"/>
-      <c r="AC53" t="inlineStr"/>
+      <c r="AC53" t="inlineStr">
+        <is>
+          <t>De sodio:  Los dem?s</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr"/>

</xml_diff>

<commit_message>
Bolivia completo y funcionando
</commit_message>
<xml_diff>
--- a/importaciones_unificadas.xlsx
+++ b/importaciones_unificadas.xlsx
@@ -5542,8 +5542,16 @@
           <t>Brasil</t>
         </is>
       </c>
-      <c r="L54" t="inlineStr"/>
-      <c r="M54" t="inlineStr"/>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
+      <c r="M54" t="inlineStr">
+        <is>
+          <t>I. Santa Cruz</t>
+        </is>
+      </c>
       <c r="N54" t="inlineStr"/>
       <c r="O54" t="inlineStr">
         <is>
@@ -5568,8 +5576,14 @@
       <c r="W54" t="n">
         <v>1260</v>
       </c>
-      <c r="X54" t="inlineStr"/>
-      <c r="Y54" t="inlineStr"/>
+      <c r="X54" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y54" t="n">
+        <v>1.26</v>
+      </c>
       <c r="Z54" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -5581,7 +5595,11 @@
         </is>
       </c>
       <c r="AB54" t="inlineStr"/>
-      <c r="AC54" t="inlineStr"/>
+      <c r="AC54" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr"/>
@@ -5627,8 +5645,16 @@
           <t>Perú</t>
         </is>
       </c>
-      <c r="L55" t="inlineStr"/>
-      <c r="M55" t="inlineStr"/>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>Perú</t>
+        </is>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
+          <t>F. Desaguadero</t>
+        </is>
+      </c>
       <c r="N55" t="inlineStr"/>
       <c r="O55" t="inlineStr">
         <is>
@@ -5653,8 +5679,14 @@
       <c r="W55" t="n">
         <v>23200</v>
       </c>
-      <c r="X55" t="inlineStr"/>
-      <c r="Y55" t="inlineStr"/>
+      <c r="X55" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y55" t="n">
+        <v>23.2</v>
+      </c>
       <c r="Z55" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -5666,7 +5698,11 @@
         </is>
       </c>
       <c r="AB55" t="inlineStr"/>
-      <c r="AC55" t="inlineStr"/>
+      <c r="AC55" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr"/>
@@ -5712,8 +5748,16 @@
           <t>Brasil</t>
         </is>
       </c>
-      <c r="L56" t="inlineStr"/>
-      <c r="M56" t="inlineStr"/>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
+      <c r="M56" t="inlineStr">
+        <is>
+          <t>I. Santa Cruz</t>
+        </is>
+      </c>
       <c r="N56" t="inlineStr"/>
       <c r="O56" t="inlineStr">
         <is>
@@ -5738,8 +5782,14 @@
       <c r="W56" t="n">
         <v>22400</v>
       </c>
-      <c r="X56" t="inlineStr"/>
-      <c r="Y56" t="inlineStr"/>
+      <c r="X56" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y56" t="n">
+        <v>22.4</v>
+      </c>
       <c r="Z56" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -5751,7 +5801,11 @@
         </is>
       </c>
       <c r="AB56" t="inlineStr"/>
-      <c r="AC56" t="inlineStr"/>
+      <c r="AC56" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr"/>
@@ -5797,8 +5851,16 @@
           <t>Argentina</t>
         </is>
       </c>
-      <c r="L57" t="inlineStr"/>
-      <c r="M57" t="inlineStr"/>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>Argentina</t>
+        </is>
+      </c>
+      <c r="M57" t="inlineStr">
+        <is>
+          <t>I. Cochabamba</t>
+        </is>
+      </c>
       <c r="N57" t="inlineStr"/>
       <c r="O57" t="inlineStr">
         <is>
@@ -5823,8 +5885,14 @@
       <c r="W57" t="n">
         <v>28000</v>
       </c>
-      <c r="X57" t="inlineStr"/>
-      <c r="Y57" t="inlineStr"/>
+      <c r="X57" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y57" t="n">
+        <v>28</v>
+      </c>
       <c r="Z57" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -5836,7 +5904,11 @@
         </is>
       </c>
       <c r="AB57" t="inlineStr"/>
-      <c r="AC57" t="inlineStr"/>
+      <c r="AC57" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr"/>
@@ -5882,8 +5954,16 @@
           <t>Brasil</t>
         </is>
       </c>
-      <c r="L58" t="inlineStr"/>
-      <c r="M58" t="inlineStr"/>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
+      <c r="M58" t="inlineStr">
+        <is>
+          <t>F. Bermejo</t>
+        </is>
+      </c>
       <c r="N58" t="inlineStr"/>
       <c r="O58" t="inlineStr">
         <is>
@@ -5908,8 +5988,14 @@
       <c r="W58" t="n">
         <v>25600</v>
       </c>
-      <c r="X58" t="inlineStr"/>
-      <c r="Y58" t="inlineStr"/>
+      <c r="X58" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y58" t="n">
+        <v>25.6</v>
+      </c>
       <c r="Z58" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -5921,7 +6007,11 @@
         </is>
       </c>
       <c r="AB58" t="inlineStr"/>
-      <c r="AC58" t="inlineStr"/>
+      <c r="AC58" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr"/>
@@ -5967,8 +6057,16 @@
           <t>Brasil</t>
         </is>
       </c>
-      <c r="L59" t="inlineStr"/>
-      <c r="M59" t="inlineStr"/>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
+      <c r="M59" t="inlineStr">
+        <is>
+          <t>I. Santa Cruz</t>
+        </is>
+      </c>
       <c r="N59" t="inlineStr"/>
       <c r="O59" t="inlineStr">
         <is>
@@ -5993,8 +6091,14 @@
       <c r="W59" t="n">
         <v>2000</v>
       </c>
-      <c r="X59" t="inlineStr"/>
-      <c r="Y59" t="inlineStr"/>
+      <c r="X59" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y59" t="n">
+        <v>2</v>
+      </c>
       <c r="Z59" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -6006,7 +6110,11 @@
         </is>
       </c>
       <c r="AB59" t="inlineStr"/>
-      <c r="AC59" t="inlineStr"/>
+      <c r="AC59" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr"/>
@@ -6052,8 +6160,16 @@
           <t>Brasil</t>
         </is>
       </c>
-      <c r="L60" t="inlineStr"/>
-      <c r="M60" t="inlineStr"/>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
+      <c r="M60" t="inlineStr">
+        <is>
+          <t>F. Puerto Suarez</t>
+        </is>
+      </c>
       <c r="N60" t="inlineStr"/>
       <c r="O60" t="inlineStr">
         <is>
@@ -6078,8 +6194,14 @@
       <c r="W60" t="n">
         <v>25200</v>
       </c>
-      <c r="X60" t="inlineStr"/>
-      <c r="Y60" t="inlineStr"/>
+      <c r="X60" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y60" t="n">
+        <v>25.2</v>
+      </c>
       <c r="Z60" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -6091,7 +6213,11 @@
         </is>
       </c>
       <c r="AB60" t="inlineStr"/>
-      <c r="AC60" t="inlineStr"/>
+      <c r="AC60" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr"/>
@@ -6137,8 +6263,16 @@
           <t>Brasil</t>
         </is>
       </c>
-      <c r="L61" t="inlineStr"/>
-      <c r="M61" t="inlineStr"/>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
+      <c r="M61" t="inlineStr">
+        <is>
+          <t>F. Puerto Suarez</t>
+        </is>
+      </c>
       <c r="N61" t="inlineStr"/>
       <c r="O61" t="inlineStr">
         <is>
@@ -6163,8 +6297,14 @@
       <c r="W61" t="n">
         <v>660</v>
       </c>
-      <c r="X61" t="inlineStr"/>
-      <c r="Y61" t="inlineStr"/>
+      <c r="X61" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y61" t="n">
+        <v>0.66</v>
+      </c>
       <c r="Z61" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -6176,7 +6316,11 @@
         </is>
       </c>
       <c r="AB61" t="inlineStr"/>
-      <c r="AC61" t="inlineStr"/>
+      <c r="AC61" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr"/>
@@ -6222,8 +6366,16 @@
           <t>Brasil</t>
         </is>
       </c>
-      <c r="L62" t="inlineStr"/>
-      <c r="M62" t="inlineStr"/>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
+      <c r="M62" t="inlineStr">
+        <is>
+          <t>I. Santa Cruz</t>
+        </is>
+      </c>
       <c r="N62" t="inlineStr"/>
       <c r="O62" t="inlineStr">
         <is>
@@ -6248,8 +6400,14 @@
       <c r="W62" t="n">
         <v>350</v>
       </c>
-      <c r="X62" t="inlineStr"/>
-      <c r="Y62" t="inlineStr"/>
+      <c r="X62" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y62" t="n">
+        <v>0.35</v>
+      </c>
       <c r="Z62" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -6261,7 +6419,11 @@
         </is>
       </c>
       <c r="AB62" t="inlineStr"/>
-      <c r="AC62" t="inlineStr"/>
+      <c r="AC62" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr"/>
@@ -6307,8 +6469,16 @@
           <t>Argentina</t>
         </is>
       </c>
-      <c r="L63" t="inlineStr"/>
-      <c r="M63" t="inlineStr"/>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>Argentina</t>
+        </is>
+      </c>
+      <c r="M63" t="inlineStr">
+        <is>
+          <t>I. Cochabamba</t>
+        </is>
+      </c>
       <c r="N63" t="inlineStr"/>
       <c r="O63" t="inlineStr">
         <is>
@@ -6333,8 +6503,14 @@
       <c r="W63" t="n">
         <v>28000</v>
       </c>
-      <c r="X63" t="inlineStr"/>
-      <c r="Y63" t="inlineStr"/>
+      <c r="X63" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y63" t="n">
+        <v>28</v>
+      </c>
       <c r="Z63" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -6346,7 +6522,11 @@
         </is>
       </c>
       <c r="AB63" t="inlineStr"/>
-      <c r="AC63" t="inlineStr"/>
+      <c r="AC63" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr"/>
@@ -6392,8 +6572,16 @@
           <t>Argentina</t>
         </is>
       </c>
-      <c r="L64" t="inlineStr"/>
-      <c r="M64" t="inlineStr"/>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>Argentina</t>
+        </is>
+      </c>
+      <c r="M64" t="inlineStr">
+        <is>
+          <t>I. Cochabamba</t>
+        </is>
+      </c>
       <c r="N64" t="inlineStr"/>
       <c r="O64" t="inlineStr">
         <is>
@@ -6418,8 +6606,14 @@
       <c r="W64" t="n">
         <v>28000</v>
       </c>
-      <c r="X64" t="inlineStr"/>
-      <c r="Y64" t="inlineStr"/>
+      <c r="X64" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y64" t="n">
+        <v>28</v>
+      </c>
       <c r="Z64" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -6431,7 +6625,11 @@
         </is>
       </c>
       <c r="AB64" t="inlineStr"/>
-      <c r="AC64" t="inlineStr"/>
+      <c r="AC64" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr"/>
@@ -6477,8 +6675,16 @@
           <t>Brasil</t>
         </is>
       </c>
-      <c r="L65" t="inlineStr"/>
-      <c r="M65" t="inlineStr"/>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
+      <c r="M65" t="inlineStr">
+        <is>
+          <t>F. Bermejo</t>
+        </is>
+      </c>
       <c r="N65" t="inlineStr"/>
       <c r="O65" t="inlineStr">
         <is>
@@ -6503,8 +6709,14 @@
       <c r="W65" t="n">
         <v>25600</v>
       </c>
-      <c r="X65" t="inlineStr"/>
-      <c r="Y65" t="inlineStr"/>
+      <c r="X65" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y65" t="n">
+        <v>25.6</v>
+      </c>
       <c r="Z65" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -6516,7 +6728,11 @@
         </is>
       </c>
       <c r="AB65" t="inlineStr"/>
-      <c r="AC65" t="inlineStr"/>
+      <c r="AC65" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr"/>
@@ -6562,8 +6778,16 @@
           <t>Brasil</t>
         </is>
       </c>
-      <c r="L66" t="inlineStr"/>
-      <c r="M66" t="inlineStr"/>
+      <c r="L66" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
+      <c r="M66" t="inlineStr">
+        <is>
+          <t>F. Puerto Suarez</t>
+        </is>
+      </c>
       <c r="N66" t="inlineStr"/>
       <c r="O66" t="inlineStr">
         <is>
@@ -6588,8 +6812,14 @@
       <c r="W66" t="n">
         <v>2080</v>
       </c>
-      <c r="X66" t="inlineStr"/>
-      <c r="Y66" t="inlineStr"/>
+      <c r="X66" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y66" t="n">
+        <v>2.08</v>
+      </c>
       <c r="Z66" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -6601,7 +6831,11 @@
         </is>
       </c>
       <c r="AB66" t="inlineStr"/>
-      <c r="AC66" t="inlineStr"/>
+      <c r="AC66" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr"/>
@@ -6647,8 +6881,16 @@
           <t>Argentina</t>
         </is>
       </c>
-      <c r="L67" t="inlineStr"/>
-      <c r="M67" t="inlineStr"/>
+      <c r="L67" t="inlineStr">
+        <is>
+          <t>Argentina</t>
+        </is>
+      </c>
+      <c r="M67" t="inlineStr">
+        <is>
+          <t>I. Cochabamba</t>
+        </is>
+      </c>
       <c r="N67" t="inlineStr"/>
       <c r="O67" t="inlineStr">
         <is>
@@ -6673,8 +6915,14 @@
       <c r="W67" t="n">
         <v>28000</v>
       </c>
-      <c r="X67" t="inlineStr"/>
-      <c r="Y67" t="inlineStr"/>
+      <c r="X67" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y67" t="n">
+        <v>28</v>
+      </c>
       <c r="Z67" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -6686,7 +6934,11 @@
         </is>
       </c>
       <c r="AB67" t="inlineStr"/>
-      <c r="AC67" t="inlineStr"/>
+      <c r="AC67" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr"/>
@@ -6732,8 +6984,16 @@
           <t>Brasil</t>
         </is>
       </c>
-      <c r="L68" t="inlineStr"/>
-      <c r="M68" t="inlineStr"/>
+      <c r="L68" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
+      <c r="M68" t="inlineStr">
+        <is>
+          <t>I. Santa Cruz</t>
+        </is>
+      </c>
       <c r="N68" t="inlineStr"/>
       <c r="O68" t="inlineStr">
         <is>
@@ -6758,8 +7018,14 @@
       <c r="W68" t="n">
         <v>1260</v>
       </c>
-      <c r="X68" t="inlineStr"/>
-      <c r="Y68" t="inlineStr"/>
+      <c r="X68" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y68" t="n">
+        <v>1.26</v>
+      </c>
       <c r="Z68" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -6771,7 +7037,11 @@
         </is>
       </c>
       <c r="AB68" t="inlineStr"/>
-      <c r="AC68" t="inlineStr"/>
+      <c r="AC68" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr"/>
@@ -6817,8 +7087,16 @@
           <t>Brasil</t>
         </is>
       </c>
-      <c r="L69" t="inlineStr"/>
-      <c r="M69" t="inlineStr"/>
+      <c r="L69" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
+      <c r="M69" t="inlineStr">
+        <is>
+          <t>I. Santa Cruz</t>
+        </is>
+      </c>
       <c r="N69" t="inlineStr"/>
       <c r="O69" t="inlineStr">
         <is>
@@ -6843,8 +7121,14 @@
       <c r="W69" t="n">
         <v>500</v>
       </c>
-      <c r="X69" t="inlineStr"/>
-      <c r="Y69" t="inlineStr"/>
+      <c r="X69" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y69" t="n">
+        <v>0.5</v>
+      </c>
       <c r="Z69" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -6856,7 +7140,11 @@
         </is>
       </c>
       <c r="AB69" t="inlineStr"/>
-      <c r="AC69" t="inlineStr"/>
+      <c r="AC69" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr"/>
@@ -6902,8 +7190,16 @@
           <t>Perú</t>
         </is>
       </c>
-      <c r="L70" t="inlineStr"/>
-      <c r="M70" t="inlineStr"/>
+      <c r="L70" t="inlineStr">
+        <is>
+          <t>Perú</t>
+        </is>
+      </c>
+      <c r="M70" t="inlineStr">
+        <is>
+          <t>I. Santa Cruz</t>
+        </is>
+      </c>
       <c r="N70" t="inlineStr"/>
       <c r="O70" t="inlineStr">
         <is>
@@ -6928,8 +7224,14 @@
       <c r="W70" t="n">
         <v>23200</v>
       </c>
-      <c r="X70" t="inlineStr"/>
-      <c r="Y70" t="inlineStr"/>
+      <c r="X70" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y70" t="n">
+        <v>23.2</v>
+      </c>
       <c r="Z70" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -6941,7 +7243,11 @@
         </is>
       </c>
       <c r="AB70" t="inlineStr"/>
-      <c r="AC70" t="inlineStr"/>
+      <c r="AC70" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr"/>
@@ -6987,8 +7293,16 @@
           <t>Brasil</t>
         </is>
       </c>
-      <c r="L71" t="inlineStr"/>
-      <c r="M71" t="inlineStr"/>
+      <c r="L71" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
+      <c r="M71" t="inlineStr">
+        <is>
+          <t>I. Santa Cruz</t>
+        </is>
+      </c>
       <c r="N71" t="inlineStr"/>
       <c r="O71" t="inlineStr">
         <is>
@@ -7013,8 +7327,14 @@
       <c r="W71" t="n">
         <v>1260</v>
       </c>
-      <c r="X71" t="inlineStr"/>
-      <c r="Y71" t="inlineStr"/>
+      <c r="X71" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y71" t="n">
+        <v>1.26</v>
+      </c>
       <c r="Z71" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -7026,7 +7346,11 @@
         </is>
       </c>
       <c r="AB71" t="inlineStr"/>
-      <c r="AC71" t="inlineStr"/>
+      <c r="AC71" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr"/>
@@ -7072,8 +7396,16 @@
           <t>Argentina</t>
         </is>
       </c>
-      <c r="L72" t="inlineStr"/>
-      <c r="M72" t="inlineStr"/>
+      <c r="L72" t="inlineStr">
+        <is>
+          <t>Argentina</t>
+        </is>
+      </c>
+      <c r="M72" t="inlineStr">
+        <is>
+          <t>I. Cochabamba</t>
+        </is>
+      </c>
       <c r="N72" t="inlineStr"/>
       <c r="O72" t="inlineStr">
         <is>
@@ -7098,8 +7430,14 @@
       <c r="W72" t="n">
         <v>28000</v>
       </c>
-      <c r="X72" t="inlineStr"/>
-      <c r="Y72" t="inlineStr"/>
+      <c r="X72" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y72" t="n">
+        <v>28</v>
+      </c>
       <c r="Z72" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -7111,7 +7449,11 @@
         </is>
       </c>
       <c r="AB72" t="inlineStr"/>
-      <c r="AC72" t="inlineStr"/>
+      <c r="AC72" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr"/>
@@ -7157,8 +7499,16 @@
           <t>Argentina</t>
         </is>
       </c>
-      <c r="L73" t="inlineStr"/>
-      <c r="M73" t="inlineStr"/>
+      <c r="L73" t="inlineStr">
+        <is>
+          <t>Argentina</t>
+        </is>
+      </c>
+      <c r="M73" t="inlineStr">
+        <is>
+          <t>I. Cochabamba</t>
+        </is>
+      </c>
       <c r="N73" t="inlineStr"/>
       <c r="O73" t="inlineStr">
         <is>
@@ -7183,8 +7533,14 @@
       <c r="W73" t="n">
         <v>28000</v>
       </c>
-      <c r="X73" t="inlineStr"/>
-      <c r="Y73" t="inlineStr"/>
+      <c r="X73" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y73" t="n">
+        <v>28</v>
+      </c>
       <c r="Z73" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -7196,7 +7552,11 @@
         </is>
       </c>
       <c r="AB73" t="inlineStr"/>
-      <c r="AC73" t="inlineStr"/>
+      <c r="AC73" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr"/>
@@ -7242,8 +7602,16 @@
           <t>Brasil</t>
         </is>
       </c>
-      <c r="L74" t="inlineStr"/>
-      <c r="M74" t="inlineStr"/>
+      <c r="L74" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
+      <c r="M74" t="inlineStr">
+        <is>
+          <t>I. Santa Cruz</t>
+        </is>
+      </c>
       <c r="N74" t="inlineStr"/>
       <c r="O74" t="inlineStr">
         <is>
@@ -7268,8 +7636,14 @@
       <c r="W74" t="n">
         <v>1000</v>
       </c>
-      <c r="X74" t="inlineStr"/>
-      <c r="Y74" t="inlineStr"/>
+      <c r="X74" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y74" t="n">
+        <v>1</v>
+      </c>
       <c r="Z74" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -7281,7 +7655,11 @@
         </is>
       </c>
       <c r="AB74" t="inlineStr"/>
-      <c r="AC74" t="inlineStr"/>
+      <c r="AC74" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr"/>
@@ -7327,8 +7705,16 @@
           <t>Argentina</t>
         </is>
       </c>
-      <c r="L75" t="inlineStr"/>
-      <c r="M75" t="inlineStr"/>
+      <c r="L75" t="inlineStr">
+        <is>
+          <t>Argentina</t>
+        </is>
+      </c>
+      <c r="M75" t="inlineStr">
+        <is>
+          <t>I. Cochabamba</t>
+        </is>
+      </c>
       <c r="N75" t="inlineStr"/>
       <c r="O75" t="inlineStr">
         <is>
@@ -7353,8 +7739,14 @@
       <c r="W75" t="n">
         <v>28000</v>
       </c>
-      <c r="X75" t="inlineStr"/>
-      <c r="Y75" t="inlineStr"/>
+      <c r="X75" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y75" t="n">
+        <v>28</v>
+      </c>
       <c r="Z75" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -7366,7 +7758,11 @@
         </is>
       </c>
       <c r="AB75" t="inlineStr"/>
-      <c r="AC75" t="inlineStr"/>
+      <c r="AC75" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr"/>
@@ -7412,8 +7808,16 @@
           <t>Brasil</t>
         </is>
       </c>
-      <c r="L76" t="inlineStr"/>
-      <c r="M76" t="inlineStr"/>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
+      <c r="M76" t="inlineStr">
+        <is>
+          <t>I. Santa Cruz</t>
+        </is>
+      </c>
       <c r="N76" t="inlineStr"/>
       <c r="O76" t="inlineStr">
         <is>
@@ -7438,8 +7842,14 @@
       <c r="W76" t="n">
         <v>1260</v>
       </c>
-      <c r="X76" t="inlineStr"/>
-      <c r="Y76" t="inlineStr"/>
+      <c r="X76" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y76" t="n">
+        <v>1.26</v>
+      </c>
       <c r="Z76" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -7451,7 +7861,11 @@
         </is>
       </c>
       <c r="AB76" t="inlineStr"/>
-      <c r="AC76" t="inlineStr"/>
+      <c r="AC76" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr"/>
@@ -7497,8 +7911,16 @@
           <t>Brasil</t>
         </is>
       </c>
-      <c r="L77" t="inlineStr"/>
-      <c r="M77" t="inlineStr"/>
+      <c r="L77" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
+      <c r="M77" t="inlineStr">
+        <is>
+          <t>I. Santa Cruz</t>
+        </is>
+      </c>
       <c r="N77" t="inlineStr"/>
       <c r="O77" t="inlineStr">
         <is>
@@ -7523,8 +7945,14 @@
       <c r="W77" t="n">
         <v>7840</v>
       </c>
-      <c r="X77" t="inlineStr"/>
-      <c r="Y77" t="inlineStr"/>
+      <c r="X77" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y77" t="n">
+        <v>7.84</v>
+      </c>
       <c r="Z77" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -7536,7 +7964,11 @@
         </is>
       </c>
       <c r="AB77" t="inlineStr"/>
-      <c r="AC77" t="inlineStr"/>
+      <c r="AC77" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr"/>
@@ -7582,8 +8014,16 @@
           <t>Argentina</t>
         </is>
       </c>
-      <c r="L78" t="inlineStr"/>
-      <c r="M78" t="inlineStr"/>
+      <c r="L78" t="inlineStr">
+        <is>
+          <t>Argentina</t>
+        </is>
+      </c>
+      <c r="M78" t="inlineStr">
+        <is>
+          <t>I. Cochabamba</t>
+        </is>
+      </c>
       <c r="N78" t="inlineStr"/>
       <c r="O78" t="inlineStr">
         <is>
@@ -7608,8 +8048,14 @@
       <c r="W78" t="n">
         <v>28000</v>
       </c>
-      <c r="X78" t="inlineStr"/>
-      <c r="Y78" t="inlineStr"/>
+      <c r="X78" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y78" t="n">
+        <v>28</v>
+      </c>
       <c r="Z78" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -7621,7 +8067,11 @@
         </is>
       </c>
       <c r="AB78" t="inlineStr"/>
-      <c r="AC78" t="inlineStr"/>
+      <c r="AC78" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr"/>
@@ -7667,8 +8117,16 @@
           <t>Argentina</t>
         </is>
       </c>
-      <c r="L79" t="inlineStr"/>
-      <c r="M79" t="inlineStr"/>
+      <c r="L79" t="inlineStr">
+        <is>
+          <t>Argentina</t>
+        </is>
+      </c>
+      <c r="M79" t="inlineStr">
+        <is>
+          <t>I. Cochabamba</t>
+        </is>
+      </c>
       <c r="N79" t="inlineStr"/>
       <c r="O79" t="inlineStr">
         <is>
@@ -7693,8 +8151,14 @@
       <c r="W79" t="n">
         <v>28000</v>
       </c>
-      <c r="X79" t="inlineStr"/>
-      <c r="Y79" t="inlineStr"/>
+      <c r="X79" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y79" t="n">
+        <v>28</v>
+      </c>
       <c r="Z79" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -7706,7 +8170,11 @@
         </is>
       </c>
       <c r="AB79" t="inlineStr"/>
-      <c r="AC79" t="inlineStr"/>
+      <c r="AC79" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr"/>
@@ -7752,8 +8220,16 @@
           <t>Perú</t>
         </is>
       </c>
-      <c r="L80" t="inlineStr"/>
-      <c r="M80" t="inlineStr"/>
+      <c r="L80" t="inlineStr">
+        <is>
+          <t>Perú</t>
+        </is>
+      </c>
+      <c r="M80" t="inlineStr">
+        <is>
+          <t>A. Viru-Viru</t>
+        </is>
+      </c>
       <c r="N80" t="inlineStr"/>
       <c r="O80" t="inlineStr">
         <is>
@@ -7778,8 +8254,14 @@
       <c r="W80" t="n">
         <v>0</v>
       </c>
-      <c r="X80" t="inlineStr"/>
-      <c r="Y80" t="inlineStr"/>
+      <c r="X80" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y80" t="n">
+        <v>0</v>
+      </c>
       <c r="Z80" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -7791,7 +8273,11 @@
         </is>
       </c>
       <c r="AB80" t="inlineStr"/>
-      <c r="AC80" t="inlineStr"/>
+      <c r="AC80" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr"/>
@@ -7837,8 +8323,16 @@
           <t>Perú</t>
         </is>
       </c>
-      <c r="L81" t="inlineStr"/>
-      <c r="M81" t="inlineStr"/>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>Perú</t>
+        </is>
+      </c>
+      <c r="M81" t="inlineStr">
+        <is>
+          <t>A. Viru-Viru</t>
+        </is>
+      </c>
       <c r="N81" t="inlineStr"/>
       <c r="O81" t="inlineStr">
         <is>
@@ -7863,8 +8357,14 @@
       <c r="W81" t="n">
         <v>0</v>
       </c>
-      <c r="X81" t="inlineStr"/>
-      <c r="Y81" t="inlineStr"/>
+      <c r="X81" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y81" t="n">
+        <v>0</v>
+      </c>
       <c r="Z81" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -7876,7 +8376,11 @@
         </is>
       </c>
       <c r="AB81" t="inlineStr"/>
-      <c r="AC81" t="inlineStr"/>
+      <c r="AC81" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr"/>
@@ -7922,8 +8426,16 @@
           <t>Perú</t>
         </is>
       </c>
-      <c r="L82" t="inlineStr"/>
-      <c r="M82" t="inlineStr"/>
+      <c r="L82" t="inlineStr">
+        <is>
+          <t>Perú</t>
+        </is>
+      </c>
+      <c r="M82" t="inlineStr">
+        <is>
+          <t>A. Viru-Viru</t>
+        </is>
+      </c>
       <c r="N82" t="inlineStr"/>
       <c r="O82" t="inlineStr">
         <is>
@@ -7948,8 +8460,14 @@
       <c r="W82" t="n">
         <v>0</v>
       </c>
-      <c r="X82" t="inlineStr"/>
-      <c r="Y82" t="inlineStr"/>
+      <c r="X82" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y82" t="n">
+        <v>0</v>
+      </c>
       <c r="Z82" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -7961,7 +8479,11 @@
         </is>
       </c>
       <c r="AB82" t="inlineStr"/>
-      <c r="AC82" t="inlineStr"/>
+      <c r="AC82" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr"/>
@@ -8007,8 +8529,16 @@
           <t>Brasil</t>
         </is>
       </c>
-      <c r="L83" t="inlineStr"/>
-      <c r="M83" t="inlineStr"/>
+      <c r="L83" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
+      <c r="M83" t="inlineStr">
+        <is>
+          <t>I. Santa Cruz</t>
+        </is>
+      </c>
       <c r="N83" t="inlineStr"/>
       <c r="O83" t="inlineStr">
         <is>
@@ -8033,8 +8563,14 @@
       <c r="W83" t="n">
         <v>22400</v>
       </c>
-      <c r="X83" t="inlineStr"/>
-      <c r="Y83" t="inlineStr"/>
+      <c r="X83" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y83" t="n">
+        <v>22.4</v>
+      </c>
       <c r="Z83" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -8046,7 +8582,11 @@
         </is>
       </c>
       <c r="AB83" t="inlineStr"/>
-      <c r="AC83" t="inlineStr"/>
+      <c r="AC83" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr"/>
@@ -8092,8 +8632,16 @@
           <t>Brasil</t>
         </is>
       </c>
-      <c r="L84" t="inlineStr"/>
-      <c r="M84" t="inlineStr"/>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
+      <c r="M84" t="inlineStr">
+        <is>
+          <t>I. Santa Cruz</t>
+        </is>
+      </c>
       <c r="N84" t="inlineStr"/>
       <c r="O84" t="inlineStr">
         <is>
@@ -8118,8 +8666,14 @@
       <c r="W84" t="n">
         <v>1000</v>
       </c>
-      <c r="X84" t="inlineStr"/>
-      <c r="Y84" t="inlineStr"/>
+      <c r="X84" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y84" t="n">
+        <v>1</v>
+      </c>
       <c r="Z84" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -8131,7 +8685,11 @@
         </is>
       </c>
       <c r="AB84" t="inlineStr"/>
-      <c r="AC84" t="inlineStr"/>
+      <c r="AC84" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr"/>
@@ -8177,8 +8735,16 @@
           <t>Argentina</t>
         </is>
       </c>
-      <c r="L85" t="inlineStr"/>
-      <c r="M85" t="inlineStr"/>
+      <c r="L85" t="inlineStr">
+        <is>
+          <t>Argentina</t>
+        </is>
+      </c>
+      <c r="M85" t="inlineStr">
+        <is>
+          <t>I. Cochabamba</t>
+        </is>
+      </c>
       <c r="N85" t="inlineStr"/>
       <c r="O85" t="inlineStr">
         <is>
@@ -8203,8 +8769,14 @@
       <c r="W85" t="n">
         <v>28000</v>
       </c>
-      <c r="X85" t="inlineStr"/>
-      <c r="Y85" t="inlineStr"/>
+      <c r="X85" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y85" t="n">
+        <v>28</v>
+      </c>
       <c r="Z85" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -8216,7 +8788,11 @@
         </is>
       </c>
       <c r="AB85" t="inlineStr"/>
-      <c r="AC85" t="inlineStr"/>
+      <c r="AC85" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr"/>
@@ -8262,8 +8838,16 @@
           <t>Argentina</t>
         </is>
       </c>
-      <c r="L86" t="inlineStr"/>
-      <c r="M86" t="inlineStr"/>
+      <c r="L86" t="inlineStr">
+        <is>
+          <t>Argentina</t>
+        </is>
+      </c>
+      <c r="M86" t="inlineStr">
+        <is>
+          <t>I. Cochabamba</t>
+        </is>
+      </c>
       <c r="N86" t="inlineStr"/>
       <c r="O86" t="inlineStr">
         <is>
@@ -8288,8 +8872,14 @@
       <c r="W86" t="n">
         <v>28000</v>
       </c>
-      <c r="X86" t="inlineStr"/>
-      <c r="Y86" t="inlineStr"/>
+      <c r="X86" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y86" t="n">
+        <v>28</v>
+      </c>
       <c r="Z86" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -8301,7 +8891,11 @@
         </is>
       </c>
       <c r="AB86" t="inlineStr"/>
-      <c r="AC86" t="inlineStr"/>
+      <c r="AC86" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr"/>
@@ -8347,8 +8941,16 @@
           <t>Argentina</t>
         </is>
       </c>
-      <c r="L87" t="inlineStr"/>
-      <c r="M87" t="inlineStr"/>
+      <c r="L87" t="inlineStr">
+        <is>
+          <t>Argentina</t>
+        </is>
+      </c>
+      <c r="M87" t="inlineStr">
+        <is>
+          <t>I. Cochabamba</t>
+        </is>
+      </c>
       <c r="N87" t="inlineStr"/>
       <c r="O87" t="inlineStr">
         <is>
@@ -8373,8 +8975,14 @@
       <c r="W87" t="n">
         <v>28000</v>
       </c>
-      <c r="X87" t="inlineStr"/>
-      <c r="Y87" t="inlineStr"/>
+      <c r="X87" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y87" t="n">
+        <v>28</v>
+      </c>
       <c r="Z87" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -8386,7 +8994,11 @@
         </is>
       </c>
       <c r="AB87" t="inlineStr"/>
-      <c r="AC87" t="inlineStr"/>
+      <c r="AC87" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr"/>
@@ -8432,8 +9044,16 @@
           <t>Argentina</t>
         </is>
       </c>
-      <c r="L88" t="inlineStr"/>
-      <c r="M88" t="inlineStr"/>
+      <c r="L88" t="inlineStr">
+        <is>
+          <t>Argentina</t>
+        </is>
+      </c>
+      <c r="M88" t="inlineStr">
+        <is>
+          <t>I. Santa Cruz</t>
+        </is>
+      </c>
       <c r="N88" t="inlineStr"/>
       <c r="O88" t="inlineStr">
         <is>
@@ -8458,8 +9078,14 @@
       <c r="W88" t="n">
         <v>400</v>
       </c>
-      <c r="X88" t="inlineStr"/>
-      <c r="Y88" t="inlineStr"/>
+      <c r="X88" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y88" t="n">
+        <v>0.4</v>
+      </c>
       <c r="Z88" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -8471,7 +9097,11 @@
         </is>
       </c>
       <c r="AB88" t="inlineStr"/>
-      <c r="AC88" t="inlineStr"/>
+      <c r="AC88" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr"/>
@@ -8517,8 +9147,16 @@
           <t>Argentina</t>
         </is>
       </c>
-      <c r="L89" t="inlineStr"/>
-      <c r="M89" t="inlineStr"/>
+      <c r="L89" t="inlineStr">
+        <is>
+          <t>Argentina</t>
+        </is>
+      </c>
+      <c r="M89" t="inlineStr">
+        <is>
+          <t>I. Cochabamba</t>
+        </is>
+      </c>
       <c r="N89" t="inlineStr"/>
       <c r="O89" t="inlineStr">
         <is>
@@ -8543,8 +9181,14 @@
       <c r="W89" t="n">
         <v>28000</v>
       </c>
-      <c r="X89" t="inlineStr"/>
-      <c r="Y89" t="inlineStr"/>
+      <c r="X89" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y89" t="n">
+        <v>28</v>
+      </c>
       <c r="Z89" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -8556,7 +9200,11 @@
         </is>
       </c>
       <c r="AB89" t="inlineStr"/>
-      <c r="AC89" t="inlineStr"/>
+      <c r="AC89" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr"/>
@@ -8602,8 +9250,16 @@
           <t>Argentina</t>
         </is>
       </c>
-      <c r="L90" t="inlineStr"/>
-      <c r="M90" t="inlineStr"/>
+      <c r="L90" t="inlineStr">
+        <is>
+          <t>Argentina</t>
+        </is>
+      </c>
+      <c r="M90" t="inlineStr">
+        <is>
+          <t>I. Cochabamba</t>
+        </is>
+      </c>
       <c r="N90" t="inlineStr"/>
       <c r="O90" t="inlineStr">
         <is>
@@ -8628,8 +9284,14 @@
       <c r="W90" t="n">
         <v>28000</v>
       </c>
-      <c r="X90" t="inlineStr"/>
-      <c r="Y90" t="inlineStr"/>
+      <c r="X90" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y90" t="n">
+        <v>28</v>
+      </c>
       <c r="Z90" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -8641,7 +9303,11 @@
         </is>
       </c>
       <c r="AB90" t="inlineStr"/>
-      <c r="AC90" t="inlineStr"/>
+      <c r="AC90" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr"/>
@@ -8687,8 +9353,16 @@
           <t>Argentina</t>
         </is>
       </c>
-      <c r="L91" t="inlineStr"/>
-      <c r="M91" t="inlineStr"/>
+      <c r="L91" t="inlineStr">
+        <is>
+          <t>Argentina</t>
+        </is>
+      </c>
+      <c r="M91" t="inlineStr">
+        <is>
+          <t>I. Cochabamba</t>
+        </is>
+      </c>
       <c r="N91" t="inlineStr"/>
       <c r="O91" t="inlineStr">
         <is>
@@ -8713,8 +9387,14 @@
       <c r="W91" t="n">
         <v>28000</v>
       </c>
-      <c r="X91" t="inlineStr"/>
-      <c r="Y91" t="inlineStr"/>
+      <c r="X91" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y91" t="n">
+        <v>28</v>
+      </c>
       <c r="Z91" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -8726,7 +9406,11 @@
         </is>
       </c>
       <c r="AB91" t="inlineStr"/>
-      <c r="AC91" t="inlineStr"/>
+      <c r="AC91" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr"/>
@@ -8772,8 +9456,16 @@
           <t>Perú</t>
         </is>
       </c>
-      <c r="L92" t="inlineStr"/>
-      <c r="M92" t="inlineStr"/>
+      <c r="L92" t="inlineStr">
+        <is>
+          <t>Perú</t>
+        </is>
+      </c>
+      <c r="M92" t="inlineStr">
+        <is>
+          <t>F. Desaguadero</t>
+        </is>
+      </c>
       <c r="N92" t="inlineStr"/>
       <c r="O92" t="inlineStr">
         <is>
@@ -8798,8 +9490,14 @@
       <c r="W92" t="n">
         <v>23200</v>
       </c>
-      <c r="X92" t="inlineStr"/>
-      <c r="Y92" t="inlineStr"/>
+      <c r="X92" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y92" t="n">
+        <v>23.2</v>
+      </c>
       <c r="Z92" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -8811,7 +9509,11 @@
         </is>
       </c>
       <c r="AB92" t="inlineStr"/>
-      <c r="AC92" t="inlineStr"/>
+      <c r="AC92" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr"/>
@@ -8857,8 +9559,16 @@
           <t>China</t>
         </is>
       </c>
-      <c r="L93" t="inlineStr"/>
-      <c r="M93" t="inlineStr"/>
+      <c r="L93" t="inlineStr">
+        <is>
+          <t>China</t>
+        </is>
+      </c>
+      <c r="M93" t="inlineStr">
+        <is>
+          <t>A. Viru-Viru</t>
+        </is>
+      </c>
       <c r="N93" t="inlineStr"/>
       <c r="O93" t="inlineStr">
         <is>
@@ -8883,8 +9593,14 @@
       <c r="W93" t="n">
         <v>6</v>
       </c>
-      <c r="X93" t="inlineStr"/>
-      <c r="Y93" t="inlineStr"/>
+      <c r="X93" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y93" t="n">
+        <v>0.006</v>
+      </c>
       <c r="Z93" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -8896,7 +9612,11 @@
         </is>
       </c>
       <c r="AB93" t="inlineStr"/>
-      <c r="AC93" t="inlineStr"/>
+      <c r="AC93" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr"/>
@@ -8942,8 +9662,16 @@
           <t>España</t>
         </is>
       </c>
-      <c r="L94" t="inlineStr"/>
-      <c r="M94" t="inlineStr"/>
+      <c r="L94" t="inlineStr">
+        <is>
+          <t>España</t>
+        </is>
+      </c>
+      <c r="M94" t="inlineStr">
+        <is>
+          <t>A. Viru-Viru</t>
+        </is>
+      </c>
       <c r="N94" t="inlineStr"/>
       <c r="O94" t="inlineStr">
         <is>
@@ -8968,8 +9696,14 @@
       <c r="W94" t="n">
         <v>0</v>
       </c>
-      <c r="X94" t="inlineStr"/>
-      <c r="Y94" t="inlineStr"/>
+      <c r="X94" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y94" t="n">
+        <v>0</v>
+      </c>
       <c r="Z94" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -8981,7 +9715,11 @@
         </is>
       </c>
       <c r="AB94" t="inlineStr"/>
-      <c r="AC94" t="inlineStr"/>
+      <c r="AC94" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr"/>
@@ -9027,8 +9765,16 @@
           <t>China</t>
         </is>
       </c>
-      <c r="L95" t="inlineStr"/>
-      <c r="M95" t="inlineStr"/>
+      <c r="L95" t="inlineStr">
+        <is>
+          <t>China</t>
+        </is>
+      </c>
+      <c r="M95" t="inlineStr">
+        <is>
+          <t>I. La Paz</t>
+        </is>
+      </c>
       <c r="N95" t="inlineStr"/>
       <c r="O95" t="inlineStr">
         <is>
@@ -9053,8 +9799,14 @@
       <c r="W95" t="n">
         <v>8650</v>
       </c>
-      <c r="X95" t="inlineStr"/>
-      <c r="Y95" t="inlineStr"/>
+      <c r="X95" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y95" t="n">
+        <v>8.65</v>
+      </c>
       <c r="Z95" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -9066,7 +9818,11 @@
         </is>
       </c>
       <c r="AB95" t="inlineStr"/>
-      <c r="AC95" t="inlineStr"/>
+      <c r="AC95" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr"/>
@@ -9112,8 +9868,16 @@
           <t>Argentina</t>
         </is>
       </c>
-      <c r="L96" t="inlineStr"/>
-      <c r="M96" t="inlineStr"/>
+      <c r="L96" t="inlineStr">
+        <is>
+          <t>Argentina</t>
+        </is>
+      </c>
+      <c r="M96" t="inlineStr">
+        <is>
+          <t>I. Santa Cruz</t>
+        </is>
+      </c>
       <c r="N96" t="inlineStr"/>
       <c r="O96" t="inlineStr">
         <is>
@@ -9138,8 +9902,14 @@
       <c r="W96" t="n">
         <v>800</v>
       </c>
-      <c r="X96" t="inlineStr"/>
-      <c r="Y96" t="inlineStr"/>
+      <c r="X96" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y96" t="n">
+        <v>0.8</v>
+      </c>
       <c r="Z96" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -9151,7 +9921,11 @@
         </is>
       </c>
       <c r="AB96" t="inlineStr"/>
-      <c r="AC96" t="inlineStr"/>
+      <c r="AC96" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr"/>
@@ -9197,8 +9971,16 @@
           <t>Perú</t>
         </is>
       </c>
-      <c r="L97" t="inlineStr"/>
-      <c r="M97" t="inlineStr"/>
+      <c r="L97" t="inlineStr">
+        <is>
+          <t>Perú</t>
+        </is>
+      </c>
+      <c r="M97" t="inlineStr">
+        <is>
+          <t>I. Santa Cruz</t>
+        </is>
+      </c>
       <c r="N97" t="inlineStr"/>
       <c r="O97" t="inlineStr">
         <is>
@@ -9223,8 +10005,14 @@
       <c r="W97" t="n">
         <v>16800</v>
       </c>
-      <c r="X97" t="inlineStr"/>
-      <c r="Y97" t="inlineStr"/>
+      <c r="X97" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y97" t="n">
+        <v>16.8</v>
+      </c>
       <c r="Z97" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -9236,7 +10024,11 @@
         </is>
       </c>
       <c r="AB97" t="inlineStr"/>
-      <c r="AC97" t="inlineStr"/>
+      <c r="AC97" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr"/>
@@ -9282,8 +10074,16 @@
           <t>Brasil</t>
         </is>
       </c>
-      <c r="L98" t="inlineStr"/>
-      <c r="M98" t="inlineStr"/>
+      <c r="L98" t="inlineStr">
+        <is>
+          <t>Brasil</t>
+        </is>
+      </c>
+      <c r="M98" t="inlineStr">
+        <is>
+          <t>I. Santa Cruz</t>
+        </is>
+      </c>
       <c r="N98" t="inlineStr"/>
       <c r="O98" t="inlineStr">
         <is>
@@ -9308,8 +10108,14 @@
       <c r="W98" t="n">
         <v>9100</v>
       </c>
-      <c r="X98" t="inlineStr"/>
-      <c r="Y98" t="inlineStr"/>
+      <c r="X98" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y98" t="n">
+        <v>9.1</v>
+      </c>
       <c r="Z98" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -9321,7 +10127,11 @@
         </is>
       </c>
       <c r="AB98" t="inlineStr"/>
-      <c r="AC98" t="inlineStr"/>
+      <c r="AC98" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr"/>
@@ -9367,8 +10177,16 @@
           <t>Egipto</t>
         </is>
       </c>
-      <c r="L99" t="inlineStr"/>
-      <c r="M99" t="inlineStr"/>
+      <c r="L99" t="inlineStr">
+        <is>
+          <t>Estados Unidos</t>
+        </is>
+      </c>
+      <c r="M99" t="inlineStr">
+        <is>
+          <t>A. Viru-Viru</t>
+        </is>
+      </c>
       <c r="N99" t="inlineStr"/>
       <c r="O99" t="inlineStr">
         <is>
@@ -9393,8 +10211,14 @@
       <c r="W99" t="n">
         <v>4</v>
       </c>
-      <c r="X99" t="inlineStr"/>
-      <c r="Y99" t="inlineStr"/>
+      <c r="X99" t="inlineStr">
+        <is>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y99" t="n">
+        <v>0.004</v>
+      </c>
       <c r="Z99" t="inlineStr">
         <is>
           <t>No disponible</t>
@@ -9406,7 +10230,11 @@
         </is>
       </c>
       <c r="AB99" t="inlineStr"/>
-      <c r="AC99" t="inlineStr"/>
+      <c r="AC99" t="inlineStr">
+        <is>
+          <t>Silicatos; silicatos comerciales de los metales alcalinos  Los demás</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr"/>

</xml_diff>

<commit_message>
version final funcionando aplica SI-NO
</commit_message>
<xml_diff>
--- a/importaciones_unificadas.xlsx
+++ b/importaciones_unificadas.xlsx
@@ -581,7 +581,11 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr"/>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B2" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -676,7 +680,11 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr"/>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B3" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -771,7 +779,11 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr"/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B4" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -862,7 +874,11 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr"/>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B5" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -957,7 +973,11 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr"/>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B6" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -1052,7 +1072,11 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr"/>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B7" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -1147,7 +1171,11 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr"/>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B8" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -1238,7 +1266,11 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B9" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -1333,7 +1365,11 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr"/>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B10" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -1428,7 +1464,11 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr"/>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B11" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -1523,7 +1563,11 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr"/>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B12" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -1618,7 +1662,11 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr"/>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B13" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -1713,7 +1761,11 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr"/>
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B14" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -1808,7 +1860,11 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr"/>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B15" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -1903,7 +1959,11 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr"/>
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B16" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -1998,7 +2058,11 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr"/>
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B17" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -2093,7 +2157,11 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr"/>
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B18" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -2188,7 +2256,11 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr"/>
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B19" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -2283,7 +2355,11 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr"/>
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B20" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -2378,7 +2454,11 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr"/>
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B21" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -2473,7 +2553,11 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr"/>
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B22" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -2568,7 +2652,11 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr"/>
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B23" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -2663,7 +2751,11 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr"/>
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B24" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -2754,7 +2846,11 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr"/>
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B25" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -2849,7 +2945,11 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr"/>
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B26" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -2944,7 +3044,11 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr"/>
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B27" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -3039,7 +3143,11 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr"/>
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B28" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -3134,7 +3242,11 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr"/>
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B29" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -3229,7 +3341,11 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr"/>
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B30" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -3324,7 +3440,11 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr"/>
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B31" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -3419,7 +3539,11 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr"/>
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B32" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -3514,7 +3638,11 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr"/>
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B33" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -3609,7 +3737,11 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr"/>
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B34" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -3704,7 +3836,11 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr"/>
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B35" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -3799,7 +3935,11 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr"/>
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B36" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -3894,7 +4034,11 @@
       </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr"/>
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B37" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -3989,7 +4133,11 @@
       </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr"/>
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B38" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -4084,7 +4232,11 @@
       </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr"/>
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B39" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -4179,7 +4331,11 @@
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr"/>
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B40" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -4274,7 +4430,11 @@
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr"/>
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B41" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -4369,7 +4529,11 @@
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr"/>
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B42" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -4464,7 +4628,11 @@
       </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr"/>
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B43" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -4559,7 +4727,11 @@
       </c>
     </row>
     <row r="44">
-      <c r="A44" t="inlineStr"/>
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B44" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -4654,7 +4826,11 @@
       </c>
     </row>
     <row r="45">
-      <c r="A45" t="inlineStr"/>
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B45" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -4749,7 +4925,11 @@
       </c>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr"/>
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B46" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -4844,7 +5024,11 @@
       </c>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr"/>
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B47" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -4939,7 +5123,11 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr"/>
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B48" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -5030,7 +5218,11 @@
       </c>
     </row>
     <row r="49">
-      <c r="A49" t="inlineStr"/>
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B49" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -5125,7 +5317,11 @@
       </c>
     </row>
     <row r="50">
-      <c r="A50" t="inlineStr"/>
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B50" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -5220,7 +5416,11 @@
       </c>
     </row>
     <row r="51">
-      <c r="A51" t="inlineStr"/>
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B51" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -5311,7 +5511,11 @@
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="inlineStr"/>
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B52" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -5404,7 +5608,11 @@
       </c>
     </row>
     <row r="53">
-      <c r="A53" t="inlineStr"/>
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B53" t="inlineStr">
         <is>
           <t>Argentina</t>
@@ -5499,7 +5707,11 @@
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="inlineStr"/>
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B54" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -5602,7 +5814,11 @@
       </c>
     </row>
     <row r="55">
-      <c r="A55" t="inlineStr"/>
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B55" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -5705,7 +5921,11 @@
       </c>
     </row>
     <row r="56">
-      <c r="A56" t="inlineStr"/>
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B56" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -5808,7 +6028,11 @@
       </c>
     </row>
     <row r="57">
-      <c r="A57" t="inlineStr"/>
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B57" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -5911,7 +6135,11 @@
       </c>
     </row>
     <row r="58">
-      <c r="A58" t="inlineStr"/>
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B58" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -6014,7 +6242,11 @@
       </c>
     </row>
     <row r="59">
-      <c r="A59" t="inlineStr"/>
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B59" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -6117,7 +6349,11 @@
       </c>
     </row>
     <row r="60">
-      <c r="A60" t="inlineStr"/>
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B60" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -6220,7 +6456,11 @@
       </c>
     </row>
     <row r="61">
-      <c r="A61" t="inlineStr"/>
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B61" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -6323,7 +6563,11 @@
       </c>
     </row>
     <row r="62">
-      <c r="A62" t="inlineStr"/>
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B62" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -6426,7 +6670,11 @@
       </c>
     </row>
     <row r="63">
-      <c r="A63" t="inlineStr"/>
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B63" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -6529,7 +6777,11 @@
       </c>
     </row>
     <row r="64">
-      <c r="A64" t="inlineStr"/>
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B64" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -6632,7 +6884,11 @@
       </c>
     </row>
     <row r="65">
-      <c r="A65" t="inlineStr"/>
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B65" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -6735,7 +6991,11 @@
       </c>
     </row>
     <row r="66">
-      <c r="A66" t="inlineStr"/>
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B66" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -6838,7 +7098,11 @@
       </c>
     </row>
     <row r="67">
-      <c r="A67" t="inlineStr"/>
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B67" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -6941,7 +7205,11 @@
       </c>
     </row>
     <row r="68">
-      <c r="A68" t="inlineStr"/>
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B68" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -7044,7 +7312,11 @@
       </c>
     </row>
     <row r="69">
-      <c r="A69" t="inlineStr"/>
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B69" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -7147,7 +7419,11 @@
       </c>
     </row>
     <row r="70">
-      <c r="A70" t="inlineStr"/>
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B70" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -7250,7 +7526,11 @@
       </c>
     </row>
     <row r="71">
-      <c r="A71" t="inlineStr"/>
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B71" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -7353,7 +7633,11 @@
       </c>
     </row>
     <row r="72">
-      <c r="A72" t="inlineStr"/>
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B72" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -7456,7 +7740,11 @@
       </c>
     </row>
     <row r="73">
-      <c r="A73" t="inlineStr"/>
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B73" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -7559,7 +7847,11 @@
       </c>
     </row>
     <row r="74">
-      <c r="A74" t="inlineStr"/>
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B74" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -7662,7 +7954,11 @@
       </c>
     </row>
     <row r="75">
-      <c r="A75" t="inlineStr"/>
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B75" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -7765,7 +8061,11 @@
       </c>
     </row>
     <row r="76">
-      <c r="A76" t="inlineStr"/>
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B76" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -7868,7 +8168,11 @@
       </c>
     </row>
     <row r="77">
-      <c r="A77" t="inlineStr"/>
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B77" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -7971,7 +8275,11 @@
       </c>
     </row>
     <row r="78">
-      <c r="A78" t="inlineStr"/>
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B78" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -8074,7 +8382,11 @@
       </c>
     </row>
     <row r="79">
-      <c r="A79" t="inlineStr"/>
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B79" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -8177,7 +8489,11 @@
       </c>
     </row>
     <row r="80">
-      <c r="A80" t="inlineStr"/>
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B80" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -8280,7 +8596,11 @@
       </c>
     </row>
     <row r="81">
-      <c r="A81" t="inlineStr"/>
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B81" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -8383,7 +8703,11 @@
       </c>
     </row>
     <row r="82">
-      <c r="A82" t="inlineStr"/>
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B82" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -8486,7 +8810,11 @@
       </c>
     </row>
     <row r="83">
-      <c r="A83" t="inlineStr"/>
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B83" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -8589,7 +8917,11 @@
       </c>
     </row>
     <row r="84">
-      <c r="A84" t="inlineStr"/>
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B84" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -8692,7 +9024,11 @@
       </c>
     </row>
     <row r="85">
-      <c r="A85" t="inlineStr"/>
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B85" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -8795,7 +9131,11 @@
       </c>
     </row>
     <row r="86">
-      <c r="A86" t="inlineStr"/>
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B86" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -8898,7 +9238,11 @@
       </c>
     </row>
     <row r="87">
-      <c r="A87" t="inlineStr"/>
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B87" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -9001,7 +9345,11 @@
       </c>
     </row>
     <row r="88">
-      <c r="A88" t="inlineStr"/>
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B88" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -9104,7 +9452,11 @@
       </c>
     </row>
     <row r="89">
-      <c r="A89" t="inlineStr"/>
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B89" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -9207,7 +9559,11 @@
       </c>
     </row>
     <row r="90">
-      <c r="A90" t="inlineStr"/>
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B90" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -9310,7 +9666,11 @@
       </c>
     </row>
     <row r="91">
-      <c r="A91" t="inlineStr"/>
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B91" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -9413,7 +9773,11 @@
       </c>
     </row>
     <row r="92">
-      <c r="A92" t="inlineStr"/>
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B92" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -9516,7 +9880,11 @@
       </c>
     </row>
     <row r="93">
-      <c r="A93" t="inlineStr"/>
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B93" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -9619,7 +9987,11 @@
       </c>
     </row>
     <row r="94">
-      <c r="A94" t="inlineStr"/>
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B94" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -9722,7 +10094,11 @@
       </c>
     </row>
     <row r="95">
-      <c r="A95" t="inlineStr"/>
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B95" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -9825,7 +10201,11 @@
       </c>
     </row>
     <row r="96">
-      <c r="A96" t="inlineStr"/>
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B96" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -9928,7 +10308,11 @@
       </c>
     </row>
     <row r="97">
-      <c r="A97" t="inlineStr"/>
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B97" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -10031,7 +10415,11 @@
       </c>
     </row>
     <row r="98">
-      <c r="A98" t="inlineStr"/>
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B98" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -10134,7 +10522,11 @@
       </c>
     </row>
     <row r="99">
-      <c r="A99" t="inlineStr"/>
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B99" t="inlineStr">
         <is>
           <t>Bolivia</t>
@@ -10237,7 +10629,11 @@
       </c>
     </row>
     <row r="100">
-      <c r="A100" t="inlineStr"/>
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B100" t="inlineStr">
         <is>
           <t>Brasil</t>
@@ -10318,7 +10714,11 @@
       </c>
     </row>
     <row r="101">
-      <c r="A101" t="inlineStr"/>
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B101" t="inlineStr">
         <is>
           <t>Brasil</t>
@@ -10399,7 +10799,11 @@
       </c>
     </row>
     <row r="102">
-      <c r="A102" t="inlineStr"/>
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B102" t="inlineStr">
         <is>
           <t>Brasil</t>
@@ -10480,7 +10884,11 @@
       </c>
     </row>
     <row r="103">
-      <c r="A103" t="inlineStr"/>
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B103" t="inlineStr">
         <is>
           <t>Brasil</t>
@@ -10561,7 +10969,11 @@
       </c>
     </row>
     <row r="104">
-      <c r="A104" t="inlineStr"/>
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B104" t="inlineStr">
         <is>
           <t>Brasil</t>
@@ -10642,7 +11054,11 @@
       </c>
     </row>
     <row r="105">
-      <c r="A105" t="inlineStr"/>
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B105" t="inlineStr">
         <is>
           <t>Brasil</t>
@@ -10723,7 +11139,11 @@
       </c>
     </row>
     <row r="106">
-      <c r="A106" t="inlineStr"/>
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B106" t="inlineStr">
         <is>
           <t>Brasil</t>
@@ -10804,7 +11224,11 @@
       </c>
     </row>
     <row r="107">
-      <c r="A107" t="inlineStr"/>
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B107" t="inlineStr">
         <is>
           <t>Brasil</t>
@@ -10885,7 +11309,11 @@
       </c>
     </row>
     <row r="108">
-      <c r="A108" t="inlineStr"/>
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B108" t="inlineStr">
         <is>
           <t>Brasil</t>
@@ -10966,7 +11394,11 @@
       </c>
     </row>
     <row r="109">
-      <c r="A109" t="inlineStr"/>
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B109" t="inlineStr">
         <is>
           <t>Brasil</t>
@@ -11047,7 +11479,11 @@
       </c>
     </row>
     <row r="110">
-      <c r="A110" t="inlineStr"/>
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B110" t="inlineStr">
         <is>
           <t>Brasil</t>
@@ -11128,7 +11564,11 @@
       </c>
     </row>
     <row r="111">
-      <c r="A111" t="inlineStr"/>
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B111" t="inlineStr">
         <is>
           <t>Brasil</t>
@@ -11209,7 +11649,11 @@
       </c>
     </row>
     <row r="112">
-      <c r="A112" t="inlineStr"/>
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B112" t="inlineStr">
         <is>
           <t>Brasil</t>
@@ -11290,7 +11734,11 @@
       </c>
     </row>
     <row r="113">
-      <c r="A113" t="inlineStr"/>
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B113" t="inlineStr">
         <is>
           <t>Brasil</t>
@@ -11371,7 +11819,11 @@
       </c>
     </row>
     <row r="114">
-      <c r="A114" t="inlineStr"/>
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B114" t="inlineStr">
         <is>
           <t>Brasil</t>
@@ -11452,7 +11904,11 @@
       </c>
     </row>
     <row r="115">
-      <c r="A115" t="inlineStr"/>
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B115" t="inlineStr">
         <is>
           <t>Brasil</t>
@@ -11533,7 +11989,11 @@
       </c>
     </row>
     <row r="116">
-      <c r="A116" t="inlineStr"/>
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B116" t="inlineStr">
         <is>
           <t>Brasil</t>
@@ -11614,7 +12074,11 @@
       </c>
     </row>
     <row r="117">
-      <c r="A117" t="inlineStr"/>
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B117" t="inlineStr">
         <is>
           <t>Brasil</t>
@@ -11695,7 +12159,11 @@
       </c>
     </row>
     <row r="118">
-      <c r="A118" t="inlineStr"/>
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B118" t="inlineStr">
         <is>
           <t>Brasil</t>
@@ -11776,7 +12244,11 @@
       </c>
     </row>
     <row r="119">
-      <c r="A119" t="inlineStr"/>
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B119" t="inlineStr">
         <is>
           <t>Brasil</t>
@@ -11857,7 +12329,11 @@
       </c>
     </row>
     <row r="120">
-      <c r="A120" t="inlineStr"/>
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B120" t="inlineStr">
         <is>
           <t>Brasil</t>
@@ -11938,7 +12414,11 @@
       </c>
     </row>
     <row r="121">
-      <c r="A121" t="inlineStr"/>
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B121" t="inlineStr">
         <is>
           <t>Brasil</t>
@@ -12019,7 +12499,11 @@
       </c>
     </row>
     <row r="122">
-      <c r="A122" t="inlineStr"/>
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B122" t="inlineStr">
         <is>
           <t>Brasil</t>
@@ -12100,7 +12584,11 @@
       </c>
     </row>
     <row r="123">
-      <c r="A123" t="inlineStr"/>
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B123" t="inlineStr">
         <is>
           <t>Brasil</t>
@@ -12181,7 +12669,11 @@
       </c>
     </row>
     <row r="124">
-      <c r="A124" t="inlineStr"/>
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B124" t="inlineStr">
         <is>
           <t>Brasil</t>
@@ -12262,7 +12754,11 @@
       </c>
     </row>
     <row r="125">
-      <c r="A125" t="inlineStr"/>
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B125" t="inlineStr">
         <is>
           <t>Brasil</t>
@@ -12343,7 +12839,11 @@
       </c>
     </row>
     <row r="126">
-      <c r="A126" t="inlineStr"/>
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B126" t="inlineStr">
         <is>
           <t>Brasil</t>
@@ -12424,7 +12924,11 @@
       </c>
     </row>
     <row r="127">
-      <c r="A127" t="inlineStr"/>
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B127" t="inlineStr">
         <is>
           <t>Brasil</t>
@@ -12505,7 +13009,11 @@
       </c>
     </row>
     <row r="128">
-      <c r="A128" t="inlineStr"/>
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B128" t="inlineStr">
         <is>
           <t>Brasil</t>
@@ -12586,7 +13094,11 @@
       </c>
     </row>
     <row r="129">
-      <c r="A129" t="inlineStr"/>
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B129" t="inlineStr">
         <is>
           <t>Brasil</t>
@@ -12667,7 +13179,11 @@
       </c>
     </row>
     <row r="130">
-      <c r="A130" t="inlineStr"/>
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B130" t="inlineStr">
         <is>
           <t>Brasil</t>
@@ -12748,7 +13264,11 @@
       </c>
     </row>
     <row r="131">
-      <c r="A131" t="inlineStr"/>
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B131" t="inlineStr">
         <is>
           <t>Brasil</t>
@@ -12829,7 +13349,11 @@
       </c>
     </row>
     <row r="132">
-      <c r="A132" t="inlineStr"/>
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B132" t="inlineStr">
         <is>
           <t>Brasil</t>
@@ -12910,7 +13434,11 @@
       </c>
     </row>
     <row r="133">
-      <c r="A133" t="inlineStr"/>
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B133" t="inlineStr">
         <is>
           <t>Brasil</t>
@@ -12991,7 +13519,11 @@
       </c>
     </row>
     <row r="134">
-      <c r="A134" t="inlineStr"/>
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B134" t="inlineStr">
         <is>
           <t>Brasil</t>
@@ -13072,7 +13604,11 @@
       </c>
     </row>
     <row r="135">
-      <c r="A135" t="inlineStr"/>
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B135" t="inlineStr">
         <is>
           <t>Brasil</t>
@@ -13153,7 +13689,11 @@
       </c>
     </row>
     <row r="136">
-      <c r="A136" t="inlineStr"/>
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B136" t="inlineStr">
         <is>
           <t>Brasil</t>
@@ -13234,7 +13774,11 @@
       </c>
     </row>
     <row r="137">
-      <c r="A137" t="inlineStr"/>
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B137" t="inlineStr">
         <is>
           <t>Brasil</t>
@@ -13315,7 +13859,11 @@
       </c>
     </row>
     <row r="138">
-      <c r="A138" t="inlineStr"/>
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B138" t="inlineStr">
         <is>
           <t>Chile</t>
@@ -13432,7 +13980,11 @@
       </c>
     </row>
     <row r="139">
-      <c r="A139" t="inlineStr"/>
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B139" t="inlineStr">
         <is>
           <t>Chile</t>
@@ -13549,7 +14101,11 @@
       </c>
     </row>
     <row r="140">
-      <c r="A140" t="inlineStr"/>
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B140" t="inlineStr">
         <is>
           <t>Chile</t>
@@ -13666,7 +14222,11 @@
       </c>
     </row>
     <row r="141">
-      <c r="A141" t="inlineStr"/>
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B141" t="inlineStr">
         <is>
           <t>Chile</t>
@@ -13783,7 +14343,11 @@
       </c>
     </row>
     <row r="142">
-      <c r="A142" t="inlineStr"/>
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B142" t="inlineStr">
         <is>
           <t>Chile</t>
@@ -13900,7 +14464,11 @@
       </c>
     </row>
     <row r="143">
-      <c r="A143" t="inlineStr"/>
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B143" t="inlineStr">
         <is>
           <t>Chile</t>
@@ -14017,7 +14585,11 @@
       </c>
     </row>
     <row r="144">
-      <c r="A144" t="inlineStr"/>
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B144" t="inlineStr">
         <is>
           <t>Chile</t>
@@ -14134,7 +14706,11 @@
       </c>
     </row>
     <row r="145">
-      <c r="A145" t="inlineStr"/>
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B145" t="inlineStr">
         <is>
           <t>Chile</t>
@@ -14251,7 +14827,11 @@
       </c>
     </row>
     <row r="146">
-      <c r="A146" t="inlineStr"/>
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B146" t="inlineStr">
         <is>
           <t>Chile</t>
@@ -14368,7 +14948,11 @@
       </c>
     </row>
     <row r="147">
-      <c r="A147" t="inlineStr"/>
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B147" t="inlineStr">
         <is>
           <t>Chile</t>
@@ -14485,7 +15069,11 @@
       </c>
     </row>
     <row r="148">
-      <c r="A148" t="inlineStr"/>
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B148" t="inlineStr">
         <is>
           <t>Chile</t>
@@ -14602,7 +15190,11 @@
       </c>
     </row>
     <row r="149">
-      <c r="A149" t="inlineStr"/>
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B149" t="inlineStr">
         <is>
           <t>Chile</t>
@@ -14719,7 +15311,11 @@
       </c>
     </row>
     <row r="150">
-      <c r="A150" t="inlineStr"/>
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B150" t="inlineStr">
         <is>
           <t>Chile</t>
@@ -14836,7 +15432,11 @@
       </c>
     </row>
     <row r="151">
-      <c r="A151" t="inlineStr"/>
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B151" t="inlineStr">
         <is>
           <t>Chile</t>
@@ -14953,7 +15553,11 @@
       </c>
     </row>
     <row r="152">
-      <c r="A152" t="inlineStr"/>
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B152" t="inlineStr">
         <is>
           <t>Chile</t>
@@ -15070,7 +15674,11 @@
       </c>
     </row>
     <row r="153">
-      <c r="A153" t="inlineStr"/>
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B153" t="inlineStr">
         <is>
           <t>Chile</t>
@@ -15187,7 +15795,11 @@
       </c>
     </row>
     <row r="154">
-      <c r="A154" t="inlineStr"/>
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B154" t="inlineStr">
         <is>
           <t>Chile</t>
@@ -15304,7 +15916,11 @@
       </c>
     </row>
     <row r="155">
-      <c r="A155" t="inlineStr"/>
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B155" t="inlineStr">
         <is>
           <t>Chile</t>
@@ -15421,7 +16037,11 @@
       </c>
     </row>
     <row r="156">
-      <c r="A156" t="inlineStr"/>
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B156" t="inlineStr">
         <is>
           <t>Chile</t>
@@ -15538,7 +16158,11 @@
       </c>
     </row>
     <row r="157">
-      <c r="A157" t="inlineStr"/>
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B157" t="inlineStr">
         <is>
           <t>Chile</t>
@@ -15655,7 +16279,11 @@
       </c>
     </row>
     <row r="158">
-      <c r="A158" t="inlineStr"/>
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B158" t="inlineStr">
         <is>
           <t>Colombia</t>
@@ -15766,7 +16394,11 @@
       </c>
     </row>
     <row r="159">
-      <c r="A159" t="inlineStr"/>
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B159" t="inlineStr">
         <is>
           <t>Colombia</t>
@@ -15877,7 +16509,11 @@
       </c>
     </row>
     <row r="160">
-      <c r="A160" t="inlineStr"/>
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B160" t="inlineStr">
         <is>
           <t>Colombia</t>
@@ -15988,7 +16624,11 @@
       </c>
     </row>
     <row r="161">
-      <c r="A161" t="inlineStr"/>
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B161" t="inlineStr">
         <is>
           <t>Colombia</t>
@@ -16099,7 +16739,11 @@
       </c>
     </row>
     <row r="162">
-      <c r="A162" t="inlineStr"/>
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B162" t="inlineStr">
         <is>
           <t>Colombia</t>
@@ -16210,7 +16854,11 @@
       </c>
     </row>
     <row r="163">
-      <c r="A163" t="inlineStr"/>
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B163" t="inlineStr">
         <is>
           <t>Colombia</t>
@@ -16321,7 +16969,11 @@
       </c>
     </row>
     <row r="164">
-      <c r="A164" t="inlineStr"/>
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B164" t="inlineStr">
         <is>
           <t>Colombia</t>
@@ -16432,7 +17084,11 @@
       </c>
     </row>
     <row r="165">
-      <c r="A165" t="inlineStr"/>
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B165" t="inlineStr">
         <is>
           <t>Colombia</t>
@@ -16543,7 +17199,11 @@
       </c>
     </row>
     <row r="166">
-      <c r="A166" t="inlineStr"/>
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B166" t="inlineStr">
         <is>
           <t>Colombia</t>
@@ -16654,7 +17314,11 @@
       </c>
     </row>
     <row r="167">
-      <c r="A167" t="inlineStr"/>
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B167" t="inlineStr">
         <is>
           <t>Colombia</t>
@@ -16765,7 +17429,11 @@
       </c>
     </row>
     <row r="168">
-      <c r="A168" t="inlineStr"/>
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B168" t="inlineStr">
         <is>
           <t>Colombia</t>
@@ -16876,7 +17544,11 @@
       </c>
     </row>
     <row r="169">
-      <c r="A169" t="inlineStr"/>
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B169" t="inlineStr">
         <is>
           <t>Colombia</t>
@@ -16987,7 +17659,11 @@
       </c>
     </row>
     <row r="170">
-      <c r="A170" t="inlineStr"/>
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B170" t="inlineStr">
         <is>
           <t>Ecuador</t>
@@ -17106,7 +17782,11 @@
       </c>
     </row>
     <row r="171">
-      <c r="A171" t="inlineStr"/>
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B171" t="inlineStr">
         <is>
           <t>Ecuador</t>
@@ -17225,7 +17905,11 @@
       </c>
     </row>
     <row r="172">
-      <c r="A172" t="inlineStr"/>
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B172" t="inlineStr">
         <is>
           <t>Ecuador</t>
@@ -17344,7 +18028,11 @@
       </c>
     </row>
     <row r="173">
-      <c r="A173" t="inlineStr"/>
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B173" t="inlineStr">
         <is>
           <t>Ecuador</t>
@@ -17463,7 +18151,11 @@
       </c>
     </row>
     <row r="174">
-      <c r="A174" t="inlineStr"/>
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B174" t="inlineStr">
         <is>
           <t>Ecuador</t>
@@ -17582,7 +18274,11 @@
       </c>
     </row>
     <row r="175">
-      <c r="A175" t="inlineStr"/>
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B175" t="inlineStr">
         <is>
           <t>Ecuador</t>
@@ -17701,7 +18397,11 @@
       </c>
     </row>
     <row r="176">
-      <c r="A176" t="inlineStr"/>
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B176" t="inlineStr">
         <is>
           <t>Ecuador</t>
@@ -17820,7 +18520,11 @@
       </c>
     </row>
     <row r="177">
-      <c r="A177" t="inlineStr"/>
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B177" t="inlineStr">
         <is>
           <t>Ecuador</t>
@@ -17939,7 +18643,11 @@
       </c>
     </row>
     <row r="178">
-      <c r="A178" t="inlineStr"/>
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B178" t="inlineStr">
         <is>
           <t>Ecuador</t>
@@ -18058,7 +18766,11 @@
       </c>
     </row>
     <row r="179">
-      <c r="A179" t="inlineStr"/>
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B179" t="inlineStr">
         <is>
           <t>Ecuador</t>
@@ -18177,7 +18889,11 @@
       </c>
     </row>
     <row r="180">
-      <c r="A180" t="inlineStr"/>
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B180" t="inlineStr">
         <is>
           <t>Ecuador</t>
@@ -18296,7 +19012,11 @@
       </c>
     </row>
     <row r="181">
-      <c r="A181" t="inlineStr"/>
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B181" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -18417,7 +19137,11 @@
       </c>
     </row>
     <row r="182">
-      <c r="A182" t="inlineStr"/>
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B182" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -18538,7 +19262,11 @@
       </c>
     </row>
     <row r="183">
-      <c r="A183" t="inlineStr"/>
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B183" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -18659,7 +19387,11 @@
       </c>
     </row>
     <row r="184">
-      <c r="A184" t="inlineStr"/>
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B184" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -18778,7 +19510,11 @@
       </c>
     </row>
     <row r="185">
-      <c r="A185" t="inlineStr"/>
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B185" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -18897,7 +19633,11 @@
       </c>
     </row>
     <row r="186">
-      <c r="A186" t="inlineStr"/>
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B186" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -19018,7 +19758,11 @@
       </c>
     </row>
     <row r="187">
-      <c r="A187" t="inlineStr"/>
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B187" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -19137,7 +19881,11 @@
       </c>
     </row>
     <row r="188">
-      <c r="A188" t="inlineStr"/>
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B188" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -19256,7 +20004,11 @@
       </c>
     </row>
     <row r="189">
-      <c r="A189" t="inlineStr"/>
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B189" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -19375,7 +20127,11 @@
       </c>
     </row>
     <row r="190">
-      <c r="A190" t="inlineStr"/>
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B190" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -19494,7 +20250,11 @@
       </c>
     </row>
     <row r="191">
-      <c r="A191" t="inlineStr"/>
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B191" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -19613,7 +20373,11 @@
       </c>
     </row>
     <row r="192">
-      <c r="A192" t="inlineStr"/>
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B192" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -19732,7 +20496,11 @@
       </c>
     </row>
     <row r="193">
-      <c r="A193" t="inlineStr"/>
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B193" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -19853,7 +20621,11 @@
       </c>
     </row>
     <row r="194">
-      <c r="A194" t="inlineStr"/>
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B194" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -19974,7 +20746,11 @@
       </c>
     </row>
     <row r="195">
-      <c r="A195" t="inlineStr"/>
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B195" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -20093,7 +20869,11 @@
       </c>
     </row>
     <row r="196">
-      <c r="A196" t="inlineStr"/>
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B196" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -20212,7 +20992,11 @@
       </c>
     </row>
     <row r="197">
-      <c r="A197" t="inlineStr"/>
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B197" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -20333,7 +21117,11 @@
       </c>
     </row>
     <row r="198">
-      <c r="A198" t="inlineStr"/>
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B198" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -20454,7 +21242,11 @@
       </c>
     </row>
     <row r="199">
-      <c r="A199" t="inlineStr"/>
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B199" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -20573,7 +21365,11 @@
       </c>
     </row>
     <row r="200">
-      <c r="A200" t="inlineStr"/>
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B200" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -20694,7 +21490,11 @@
       </c>
     </row>
     <row r="201">
-      <c r="A201" t="inlineStr"/>
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B201" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -20813,7 +21613,11 @@
       </c>
     </row>
     <row r="202">
-      <c r="A202" t="inlineStr"/>
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B202" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -20932,7 +21736,11 @@
       </c>
     </row>
     <row r="203">
-      <c r="A203" t="inlineStr"/>
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B203" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -21051,7 +21859,11 @@
       </c>
     </row>
     <row r="204">
-      <c r="A204" t="inlineStr"/>
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B204" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -21172,7 +21984,11 @@
       </c>
     </row>
     <row r="205">
-      <c r="A205" t="inlineStr"/>
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B205" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -21293,7 +22109,11 @@
       </c>
     </row>
     <row r="206">
-      <c r="A206" t="inlineStr"/>
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B206" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -21414,7 +22234,11 @@
       </c>
     </row>
     <row r="207">
-      <c r="A207" t="inlineStr"/>
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B207" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -21533,7 +22357,11 @@
       </c>
     </row>
     <row r="208">
-      <c r="A208" t="inlineStr"/>
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B208" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -21652,7 +22480,11 @@
       </c>
     </row>
     <row r="209">
-      <c r="A209" t="inlineStr"/>
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B209" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -21771,7 +22603,11 @@
       </c>
     </row>
     <row r="210">
-      <c r="A210" t="inlineStr"/>
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B210" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -21890,7 +22726,11 @@
       </c>
     </row>
     <row r="211">
-      <c r="A211" t="inlineStr"/>
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B211" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -22009,7 +22849,11 @@
       </c>
     </row>
     <row r="212">
-      <c r="A212" t="inlineStr"/>
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B212" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -22128,7 +22972,11 @@
       </c>
     </row>
     <row r="213">
-      <c r="A213" t="inlineStr"/>
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B213" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -22247,7 +23095,11 @@
       </c>
     </row>
     <row r="214">
-      <c r="A214" t="inlineStr"/>
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B214" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -22366,7 +23218,11 @@
       </c>
     </row>
     <row r="215">
-      <c r="A215" t="inlineStr"/>
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B215" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -22485,7 +23341,11 @@
       </c>
     </row>
     <row r="216">
-      <c r="A216" t="inlineStr"/>
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B216" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -22604,7 +23464,11 @@
       </c>
     </row>
     <row r="217">
-      <c r="A217" t="inlineStr"/>
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B217" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -22723,7 +23587,11 @@
       </c>
     </row>
     <row r="218">
-      <c r="A218" t="inlineStr"/>
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B218" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -22842,7 +23710,11 @@
       </c>
     </row>
     <row r="219">
-      <c r="A219" t="inlineStr"/>
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B219" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -22961,7 +23833,11 @@
       </c>
     </row>
     <row r="220">
-      <c r="A220" t="inlineStr"/>
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B220" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -23080,7 +23956,11 @@
       </c>
     </row>
     <row r="221">
-      <c r="A221" t="inlineStr"/>
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B221" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -23199,7 +24079,11 @@
       </c>
     </row>
     <row r="222">
-      <c r="A222" t="inlineStr"/>
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B222" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -23318,7 +24202,11 @@
       </c>
     </row>
     <row r="223">
-      <c r="A223" t="inlineStr"/>
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B223" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -23437,7 +24325,11 @@
       </c>
     </row>
     <row r="224">
-      <c r="A224" t="inlineStr"/>
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B224" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -23556,7 +24448,11 @@
       </c>
     </row>
     <row r="225">
-      <c r="A225" t="inlineStr"/>
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B225" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -23677,7 +24573,11 @@
       </c>
     </row>
     <row r="226">
-      <c r="A226" t="inlineStr"/>
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B226" t="inlineStr">
         <is>
           <t>Perú</t>
@@ -23796,7 +24696,11 @@
       </c>
     </row>
     <row r="227">
-      <c r="A227" t="inlineStr"/>
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B227" t="inlineStr">
         <is>
           <t>Paraguay</t>
@@ -23899,7 +24803,11 @@
       </c>
     </row>
     <row r="228">
-      <c r="A228" t="inlineStr"/>
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B228" t="inlineStr">
         <is>
           <t>Paraguay</t>
@@ -24002,7 +24910,11 @@
       </c>
     </row>
     <row r="229">
-      <c r="A229" t="inlineStr"/>
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B229" t="inlineStr">
         <is>
           <t>Paraguay</t>
@@ -24105,7 +25017,11 @@
       </c>
     </row>
     <row r="230">
-      <c r="A230" t="inlineStr"/>
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B230" t="inlineStr">
         <is>
           <t>Paraguay</t>
@@ -24208,7 +25124,11 @@
       </c>
     </row>
     <row r="231">
-      <c r="A231" t="inlineStr"/>
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B231" t="inlineStr">
         <is>
           <t>Paraguay</t>
@@ -24311,7 +25231,11 @@
       </c>
     </row>
     <row r="232">
-      <c r="A232" t="inlineStr"/>
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B232" t="inlineStr">
         <is>
           <t>Paraguay</t>
@@ -24414,7 +25338,11 @@
       </c>
     </row>
     <row r="233">
-      <c r="A233" t="inlineStr"/>
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B233" t="inlineStr">
         <is>
           <t>Paraguay</t>
@@ -24517,7 +25445,11 @@
       </c>
     </row>
     <row r="234">
-      <c r="A234" t="inlineStr"/>
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B234" t="inlineStr">
         <is>
           <t>Paraguay</t>
@@ -24620,7 +25552,11 @@
       </c>
     </row>
     <row r="235">
-      <c r="A235" t="inlineStr"/>
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B235" t="inlineStr">
         <is>
           <t>Paraguay</t>
@@ -24723,7 +25659,11 @@
       </c>
     </row>
     <row r="236">
-      <c r="A236" t="inlineStr"/>
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B236" t="inlineStr">
         <is>
           <t>Paraguay</t>
@@ -24826,7 +25766,11 @@
       </c>
     </row>
     <row r="237">
-      <c r="A237" t="inlineStr"/>
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B237" t="inlineStr">
         <is>
           <t>Paraguay</t>
@@ -24929,7 +25873,11 @@
       </c>
     </row>
     <row r="238">
-      <c r="A238" t="inlineStr"/>
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B238" t="inlineStr">
         <is>
           <t>Paraguay</t>
@@ -25032,7 +25980,11 @@
       </c>
     </row>
     <row r="239">
-      <c r="A239" t="inlineStr"/>
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B239" t="inlineStr">
         <is>
           <t>Paraguay</t>
@@ -25135,7 +26087,11 @@
       </c>
     </row>
     <row r="240">
-      <c r="A240" t="inlineStr"/>
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B240" t="inlineStr">
         <is>
           <t>Paraguay</t>
@@ -25238,7 +26194,11 @@
       </c>
     </row>
     <row r="241">
-      <c r="A241" t="inlineStr"/>
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B241" t="inlineStr">
         <is>
           <t>Paraguay</t>
@@ -25341,7 +26301,11 @@
       </c>
     </row>
     <row r="242">
-      <c r="A242" t="inlineStr"/>
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B242" t="inlineStr">
         <is>
           <t>Paraguay</t>
@@ -25444,7 +26408,11 @@
       </c>
     </row>
     <row r="243">
-      <c r="A243" t="inlineStr"/>
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B243" t="inlineStr">
         <is>
           <t>Paraguay</t>
@@ -25547,7 +26515,11 @@
       </c>
     </row>
     <row r="244">
-      <c r="A244" t="inlineStr"/>
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B244" t="inlineStr">
         <is>
           <t>Paraguay</t>
@@ -25650,7 +26622,11 @@
       </c>
     </row>
     <row r="245">
-      <c r="A245" t="inlineStr"/>
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B245" t="inlineStr">
         <is>
           <t>Paraguay</t>
@@ -25753,7 +26729,11 @@
       </c>
     </row>
     <row r="246">
-      <c r="A246" t="inlineStr"/>
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B246" t="inlineStr">
         <is>
           <t>Uruguay</t>
@@ -25848,7 +26828,11 @@
       </c>
     </row>
     <row r="247">
-      <c r="A247" t="inlineStr"/>
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B247" t="inlineStr">
         <is>
           <t>Uruguay</t>
@@ -25943,7 +26927,11 @@
       </c>
     </row>
     <row r="248">
-      <c r="A248" t="inlineStr"/>
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B248" t="inlineStr">
         <is>
           <t>Uruguay</t>
@@ -26038,7 +27026,11 @@
       </c>
     </row>
     <row r="249">
-      <c r="A249" t="inlineStr"/>
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B249" t="inlineStr">
         <is>
           <t>Uruguay</t>
@@ -26135,7 +27127,11 @@
       </c>
     </row>
     <row r="250">
-      <c r="A250" t="inlineStr"/>
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B250" t="inlineStr">
         <is>
           <t>Uruguay</t>
@@ -26230,7 +27226,11 @@
       </c>
     </row>
     <row r="251">
-      <c r="A251" t="inlineStr"/>
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B251" t="inlineStr">
         <is>
           <t>Uruguay</t>
@@ -26325,7 +27325,11 @@
       </c>
     </row>
     <row r="252">
-      <c r="A252" t="inlineStr"/>
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>SI</t>
+        </is>
+      </c>
       <c r="B252" t="inlineStr">
         <is>
           <t>Uruguay</t>
@@ -26422,7 +27426,11 @@
       </c>
     </row>
     <row r="253">
-      <c r="A253" t="inlineStr"/>
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
       <c r="B253" t="inlineStr">
         <is>
           <t>Uruguay</t>

</xml_diff>

<commit_message>
Agregado soporte para Brasil (QUILOGRAMA LIQUIDO) y cálculo de Toneladas Finales
</commit_message>
<xml_diff>
--- a/importaciones_unificadas.xlsx
+++ b/importaciones_unificadas.xlsx
@@ -10631,7 +10631,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SI</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -10700,10 +10700,12 @@
       </c>
       <c r="X100" t="inlineStr">
         <is>
-          <t>QUILOGRAMA LIQUIDO</t>
-        </is>
-      </c>
-      <c r="Y100" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y100" t="n">
+        <v>1.451</v>
+      </c>
       <c r="Z100" t="inlineStr"/>
       <c r="AA100" t="inlineStr"/>
       <c r="AB100" t="inlineStr"/>
@@ -10785,10 +10787,12 @@
       </c>
       <c r="X101" t="inlineStr">
         <is>
-          <t>QUILOGRAMA LIQUIDO</t>
-        </is>
-      </c>
-      <c r="Y101" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y101" t="n">
+        <v>0.425</v>
+      </c>
       <c r="Z101" t="inlineStr"/>
       <c r="AA101" t="inlineStr"/>
       <c r="AB101" t="inlineStr"/>
@@ -10801,7 +10805,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SI</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -10870,10 +10874,12 @@
       </c>
       <c r="X102" t="inlineStr">
         <is>
-          <t>QUILOGRAMA LIQUIDO</t>
-        </is>
-      </c>
-      <c r="Y102" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y102" t="n">
+        <v>19.84</v>
+      </c>
       <c r="Z102" t="inlineStr"/>
       <c r="AA102" t="inlineStr"/>
       <c r="AB102" t="inlineStr"/>
@@ -10955,10 +10961,12 @@
       </c>
       <c r="X103" t="inlineStr">
         <is>
-          <t>QUILOGRAMA LIQUIDO</t>
-        </is>
-      </c>
-      <c r="Y103" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y103" t="n">
+        <v>0.067</v>
+      </c>
       <c r="Z103" t="inlineStr"/>
       <c r="AA103" t="inlineStr"/>
       <c r="AB103" t="inlineStr"/>
@@ -11040,10 +11048,12 @@
       </c>
       <c r="X104" t="inlineStr">
         <is>
-          <t>QUILOGRAMA LIQUIDO</t>
-        </is>
-      </c>
-      <c r="Y104" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y104" t="n">
+        <v>0.01</v>
+      </c>
       <c r="Z104" t="inlineStr"/>
       <c r="AA104" t="inlineStr"/>
       <c r="AB104" t="inlineStr"/>
@@ -11056,7 +11066,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SI</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -11125,10 +11135,12 @@
       </c>
       <c r="X105" t="inlineStr">
         <is>
-          <t>QUILOGRAMA LIQUIDO</t>
-        </is>
-      </c>
-      <c r="Y105" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y105" t="n">
+        <v>12</v>
+      </c>
       <c r="Z105" t="inlineStr"/>
       <c r="AA105" t="inlineStr"/>
       <c r="AB105" t="inlineStr"/>
@@ -11141,7 +11153,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SI</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -11210,10 +11222,12 @@
       </c>
       <c r="X106" t="inlineStr">
         <is>
-          <t>QUILOGRAMA LIQUIDO</t>
-        </is>
-      </c>
-      <c r="Y106" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y106" t="n">
+        <v>11.596</v>
+      </c>
       <c r="Z106" t="inlineStr"/>
       <c r="AA106" t="inlineStr"/>
       <c r="AB106" t="inlineStr"/>
@@ -11226,7 +11240,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SI</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -11295,10 +11309,12 @@
       </c>
       <c r="X107" t="inlineStr">
         <is>
-          <t>QUILOGRAMA LIQUIDO</t>
-        </is>
-      </c>
-      <c r="Y107" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y107" t="n">
+        <v>1.44</v>
+      </c>
       <c r="Z107" t="inlineStr"/>
       <c r="AA107" t="inlineStr"/>
       <c r="AB107" t="inlineStr"/>
@@ -11380,10 +11396,12 @@
       </c>
       <c r="X108" t="inlineStr">
         <is>
-          <t>QUILOGRAMA LIQUIDO</t>
-        </is>
-      </c>
-      <c r="Y108" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y108" t="n">
+        <v>0.249</v>
+      </c>
       <c r="Z108" t="inlineStr"/>
       <c r="AA108" t="inlineStr"/>
       <c r="AB108" t="inlineStr"/>
@@ -11396,7 +11414,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SI</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -11465,10 +11483,12 @@
       </c>
       <c r="X109" t="inlineStr">
         <is>
-          <t>QUILOGRAMA LIQUIDO</t>
-        </is>
-      </c>
-      <c r="Y109" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y109" t="n">
+        <v>3.096</v>
+      </c>
       <c r="Z109" t="inlineStr"/>
       <c r="AA109" t="inlineStr"/>
       <c r="AB109" t="inlineStr"/>
@@ -11481,7 +11501,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SI</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -11550,10 +11570,12 @@
       </c>
       <c r="X110" t="inlineStr">
         <is>
-          <t>QUILOGRAMA LIQUIDO</t>
-        </is>
-      </c>
-      <c r="Y110" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y110" t="n">
+        <v>53.04</v>
+      </c>
       <c r="Z110" t="inlineStr"/>
       <c r="AA110" t="inlineStr"/>
       <c r="AB110" t="inlineStr"/>
@@ -11635,10 +11657,12 @@
       </c>
       <c r="X111" t="inlineStr">
         <is>
-          <t>QUILOGRAMA LIQUIDO</t>
-        </is>
-      </c>
-      <c r="Y111" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y111" t="n">
+        <v>0.041</v>
+      </c>
       <c r="Z111" t="inlineStr"/>
       <c r="AA111" t="inlineStr"/>
       <c r="AB111" t="inlineStr"/>
@@ -11720,10 +11744,12 @@
       </c>
       <c r="X112" t="inlineStr">
         <is>
-          <t>QUILOGRAMA LIQUIDO</t>
-        </is>
-      </c>
-      <c r="Y112" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y112" t="n">
+        <v>0.59</v>
+      </c>
       <c r="Z112" t="inlineStr"/>
       <c r="AA112" t="inlineStr"/>
       <c r="AB112" t="inlineStr"/>
@@ -11805,10 +11831,12 @@
       </c>
       <c r="X113" t="inlineStr">
         <is>
-          <t>QUILOGRAMA LIQUIDO</t>
-        </is>
-      </c>
-      <c r="Y113" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y113" t="n">
+        <v>0.011</v>
+      </c>
       <c r="Z113" t="inlineStr"/>
       <c r="AA113" t="inlineStr"/>
       <c r="AB113" t="inlineStr"/>
@@ -11890,10 +11918,12 @@
       </c>
       <c r="X114" t="inlineStr">
         <is>
-          <t>QUILOGRAMA LIQUIDO</t>
-        </is>
-      </c>
-      <c r="Y114" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y114" t="n">
+        <v>0.1</v>
+      </c>
       <c r="Z114" t="inlineStr"/>
       <c r="AA114" t="inlineStr"/>
       <c r="AB114" t="inlineStr"/>
@@ -11906,7 +11936,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SI</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -11975,10 +12005,12 @@
       </c>
       <c r="X115" t="inlineStr">
         <is>
-          <t>QUILOGRAMA LIQUIDO</t>
-        </is>
-      </c>
-      <c r="Y115" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y115" t="n">
+        <v>2.061</v>
+      </c>
       <c r="Z115" t="inlineStr"/>
       <c r="AA115" t="inlineStr"/>
       <c r="AB115" t="inlineStr"/>
@@ -11991,7 +12023,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SI</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -12060,10 +12092,12 @@
       </c>
       <c r="X116" t="inlineStr">
         <is>
-          <t>QUILOGRAMA LIQUIDO</t>
-        </is>
-      </c>
-      <c r="Y116" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y116" t="n">
+        <v>2.275</v>
+      </c>
       <c r="Z116" t="inlineStr"/>
       <c r="AA116" t="inlineStr"/>
       <c r="AB116" t="inlineStr"/>
@@ -12145,10 +12179,12 @@
       </c>
       <c r="X117" t="inlineStr">
         <is>
-          <t>QUILOGRAMA LIQUIDO</t>
-        </is>
-      </c>
-      <c r="Y117" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y117" t="n">
+        <v>0.325</v>
+      </c>
       <c r="Z117" t="inlineStr"/>
       <c r="AA117" t="inlineStr"/>
       <c r="AB117" t="inlineStr"/>
@@ -12230,10 +12266,12 @@
       </c>
       <c r="X118" t="inlineStr">
         <is>
-          <t>QUILOGRAMA LIQUIDO</t>
-        </is>
-      </c>
-      <c r="Y118" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y118" t="n">
+        <v>0.067</v>
+      </c>
       <c r="Z118" t="inlineStr"/>
       <c r="AA118" t="inlineStr"/>
       <c r="AB118" t="inlineStr"/>
@@ -12315,10 +12353,12 @@
       </c>
       <c r="X119" t="inlineStr">
         <is>
-          <t>QUILOGRAMA LIQUIDO</t>
-        </is>
-      </c>
-      <c r="Y119" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y119" t="n">
+        <v>0.011</v>
+      </c>
       <c r="Z119" t="inlineStr"/>
       <c r="AA119" t="inlineStr"/>
       <c r="AB119" t="inlineStr"/>
@@ -12400,10 +12440,12 @@
       </c>
       <c r="X120" t="inlineStr">
         <is>
-          <t>QUILOGRAMA LIQUIDO</t>
-        </is>
-      </c>
-      <c r="Y120" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y120" t="n">
+        <v>0.15</v>
+      </c>
       <c r="Z120" t="inlineStr"/>
       <c r="AA120" t="inlineStr"/>
       <c r="AB120" t="inlineStr"/>
@@ -12416,7 +12458,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SI</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -12485,10 +12527,12 @@
       </c>
       <c r="X121" t="inlineStr">
         <is>
-          <t>QUILOGRAMA LIQUIDO</t>
-        </is>
-      </c>
-      <c r="Y121" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y121" t="n">
+        <v>1.95</v>
+      </c>
       <c r="Z121" t="inlineStr"/>
       <c r="AA121" t="inlineStr"/>
       <c r="AB121" t="inlineStr"/>
@@ -12570,10 +12614,12 @@
       </c>
       <c r="X122" t="inlineStr">
         <is>
-          <t>QUILOGRAMA LIQUIDO</t>
-        </is>
-      </c>
-      <c r="Y122" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y122" t="n">
+        <v>0.104</v>
+      </c>
       <c r="Z122" t="inlineStr"/>
       <c r="AA122" t="inlineStr"/>
       <c r="AB122" t="inlineStr"/>
@@ -12586,7 +12632,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SI</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -12655,10 +12701,12 @@
       </c>
       <c r="X123" t="inlineStr">
         <is>
-          <t>QUILOGRAMA LIQUIDO</t>
-        </is>
-      </c>
-      <c r="Y123" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y123" t="n">
+        <v>2.704</v>
+      </c>
       <c r="Z123" t="inlineStr"/>
       <c r="AA123" t="inlineStr"/>
       <c r="AB123" t="inlineStr"/>
@@ -12740,10 +12788,12 @@
       </c>
       <c r="X124" t="inlineStr">
         <is>
-          <t>QUILOGRAMA LIQUIDO</t>
-        </is>
-      </c>
-      <c r="Y124" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y124" t="n">
+        <v>0.05</v>
+      </c>
       <c r="Z124" t="inlineStr"/>
       <c r="AA124" t="inlineStr"/>
       <c r="AB124" t="inlineStr"/>
@@ -12756,7 +12806,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SI</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -12825,10 +12875,12 @@
       </c>
       <c r="X125" t="inlineStr">
         <is>
-          <t>QUILOGRAMA LIQUIDO</t>
-        </is>
-      </c>
-      <c r="Y125" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y125" t="n">
+        <v>1.44</v>
+      </c>
       <c r="Z125" t="inlineStr"/>
       <c r="AA125" t="inlineStr"/>
       <c r="AB125" t="inlineStr"/>
@@ -12841,7 +12893,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SI</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -12910,10 +12962,12 @@
       </c>
       <c r="X126" t="inlineStr">
         <is>
-          <t>QUILOGRAMA LIQUIDO</t>
-        </is>
-      </c>
-      <c r="Y126" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y126" t="n">
+        <v>12</v>
+      </c>
       <c r="Z126" t="inlineStr"/>
       <c r="AA126" t="inlineStr"/>
       <c r="AB126" t="inlineStr"/>
@@ -12926,7 +12980,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SI</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -12995,10 +13049,12 @@
       </c>
       <c r="X127" t="inlineStr">
         <is>
-          <t>QUILOGRAMA LIQUIDO</t>
-        </is>
-      </c>
-      <c r="Y127" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y127" t="n">
+        <v>1.625</v>
+      </c>
       <c r="Z127" t="inlineStr"/>
       <c r="AA127" t="inlineStr"/>
       <c r="AB127" t="inlineStr"/>
@@ -13011,7 +13067,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SI</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -13080,10 +13136,12 @@
       </c>
       <c r="X128" t="inlineStr">
         <is>
-          <t>QUILOGRAMA LIQUIDO</t>
-        </is>
-      </c>
-      <c r="Y128" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y128" t="n">
+        <v>1.626</v>
+      </c>
       <c r="Z128" t="inlineStr"/>
       <c r="AA128" t="inlineStr"/>
       <c r="AB128" t="inlineStr"/>
@@ -13165,10 +13223,12 @@
       </c>
       <c r="X129" t="inlineStr">
         <is>
-          <t>QUILOGRAMA LIQUIDO</t>
-        </is>
-      </c>
-      <c r="Y129" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y129" t="n">
+        <v>0.3</v>
+      </c>
       <c r="Z129" t="inlineStr"/>
       <c r="AA129" t="inlineStr"/>
       <c r="AB129" t="inlineStr"/>
@@ -13181,7 +13241,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SI</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -13250,10 +13310,12 @@
       </c>
       <c r="X130" t="inlineStr">
         <is>
-          <t>QUILOGRAMA LIQUIDO</t>
-        </is>
-      </c>
-      <c r="Y130" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y130" t="n">
+        <v>12</v>
+      </c>
       <c r="Z130" t="inlineStr"/>
       <c r="AA130" t="inlineStr"/>
       <c r="AB130" t="inlineStr"/>
@@ -13266,7 +13328,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SI</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -13335,10 +13397,12 @@
       </c>
       <c r="X131" t="inlineStr">
         <is>
-          <t>QUILOGRAMA LIQUIDO</t>
-        </is>
-      </c>
-      <c r="Y131" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y131" t="n">
+        <v>2.673</v>
+      </c>
       <c r="Z131" t="inlineStr"/>
       <c r="AA131" t="inlineStr"/>
       <c r="AB131" t="inlineStr"/>
@@ -13351,7 +13415,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SI</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -13420,10 +13484,12 @@
       </c>
       <c r="X132" t="inlineStr">
         <is>
-          <t>QUILOGRAMA LIQUIDO</t>
-        </is>
-      </c>
-      <c r="Y132" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y132" t="n">
+        <v>3.594</v>
+      </c>
       <c r="Z132" t="inlineStr"/>
       <c r="AA132" t="inlineStr"/>
       <c r="AB132" t="inlineStr"/>
@@ -13436,7 +13502,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SI</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -13505,10 +13571,12 @@
       </c>
       <c r="X133" t="inlineStr">
         <is>
-          <t>QUILOGRAMA LIQUIDO</t>
-        </is>
-      </c>
-      <c r="Y133" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y133" t="n">
+        <v>1.2</v>
+      </c>
       <c r="Z133" t="inlineStr"/>
       <c r="AA133" t="inlineStr"/>
       <c r="AB133" t="inlineStr"/>
@@ -13590,10 +13658,12 @@
       </c>
       <c r="X134" t="inlineStr">
         <is>
-          <t>QUILOGRAMA LIQUIDO</t>
-        </is>
-      </c>
-      <c r="Y134" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y134" t="n">
+        <v>0.01</v>
+      </c>
       <c r="Z134" t="inlineStr"/>
       <c r="AA134" t="inlineStr"/>
       <c r="AB134" t="inlineStr"/>
@@ -13606,7 +13676,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SI</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -13675,10 +13745,12 @@
       </c>
       <c r="X135" t="inlineStr">
         <is>
-          <t>QUILOGRAMA LIQUIDO</t>
-        </is>
-      </c>
-      <c r="Y135" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y135" t="n">
+        <v>1</v>
+      </c>
       <c r="Z135" t="inlineStr"/>
       <c r="AA135" t="inlineStr"/>
       <c r="AB135" t="inlineStr"/>
@@ -13760,10 +13832,12 @@
       </c>
       <c r="X136" t="inlineStr">
         <is>
-          <t>QUILOGRAMA LIQUIDO</t>
-        </is>
-      </c>
-      <c r="Y136" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y136" t="n">
+        <v>0.096</v>
+      </c>
       <c r="Z136" t="inlineStr"/>
       <c r="AA136" t="inlineStr"/>
       <c r="AB136" t="inlineStr"/>
@@ -13776,7 +13850,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>SI</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -13845,10 +13919,12 @@
       </c>
       <c r="X137" t="inlineStr">
         <is>
-          <t>QUILOGRAMA LIQUIDO</t>
-        </is>
-      </c>
-      <c r="Y137" t="inlineStr"/>
+          <t>KILOGRAMOS</t>
+        </is>
+      </c>
+      <c r="Y137" t="n">
+        <v>19.8</v>
+      </c>
       <c r="Z137" t="inlineStr"/>
       <c r="AA137" t="inlineStr"/>
       <c r="AB137" t="inlineStr"/>

</xml_diff>

<commit_message>
se modifica pais Bolivia para que aparezca valores cif unitarios
</commit_message>
<xml_diff>
--- a/importaciones_unificadas.xlsx
+++ b/importaciones_unificadas.xlsx
@@ -5778,7 +5778,9 @@
         <v>1160.2</v>
       </c>
       <c r="S54" t="inlineStr"/>
-      <c r="T54" t="inlineStr"/>
+      <c r="T54" t="n">
+        <v>0.92</v>
+      </c>
       <c r="U54" t="n">
         <v>114.08</v>
       </c>
@@ -5885,7 +5887,9 @@
         <v>10499.14</v>
       </c>
       <c r="S55" t="inlineStr"/>
-      <c r="T55" t="inlineStr"/>
+      <c r="T55" t="n">
+        <v>0.45</v>
+      </c>
       <c r="U55" t="n">
         <v>1980</v>
       </c>
@@ -5992,7 +5996,9 @@
         <v>8787.5</v>
       </c>
       <c r="S56" t="inlineStr"/>
-      <c r="T56" t="inlineStr"/>
+      <c r="T56" t="n">
+        <v>0.39</v>
+      </c>
       <c r="U56" t="n">
         <v>1597.4</v>
       </c>
@@ -6099,7 +6105,9 @@
         <v>14483.76</v>
       </c>
       <c r="S57" t="inlineStr"/>
-      <c r="T57" t="inlineStr"/>
+      <c r="T57" t="n">
+        <v>0.52</v>
+      </c>
       <c r="U57" t="n">
         <v>3000</v>
       </c>
@@ -6206,7 +6214,9 @@
         <v>18885.06</v>
       </c>
       <c r="S58" t="inlineStr"/>
-      <c r="T58" t="inlineStr"/>
+      <c r="T58" t="n">
+        <v>0.74</v>
+      </c>
       <c r="U58" t="n">
         <v>2459.84</v>
       </c>
@@ -6313,7 +6323,9 @@
         <v>693.25</v>
       </c>
       <c r="S59" t="inlineStr"/>
-      <c r="T59" t="inlineStr"/>
+      <c r="T59" t="n">
+        <v>0.35</v>
+      </c>
       <c r="U59" t="n">
         <v>111.48</v>
       </c>
@@ -6420,7 +6432,9 @@
         <v>12679.74</v>
       </c>
       <c r="S60" t="inlineStr"/>
-      <c r="T60" t="inlineStr"/>
+      <c r="T60" t="n">
+        <v>0.5</v>
+      </c>
       <c r="U60" t="n">
         <v>2825.99</v>
       </c>
@@ -6527,7 +6541,9 @@
         <v>332.18</v>
       </c>
       <c r="S61" t="inlineStr"/>
-      <c r="T61" t="inlineStr"/>
+      <c r="T61" t="n">
+        <v>0.5</v>
+      </c>
       <c r="U61" t="n">
         <v>74.01000000000001</v>
       </c>
@@ -6634,7 +6650,9 @@
         <v>1652.44</v>
       </c>
       <c r="S62" t="inlineStr"/>
-      <c r="T62" t="inlineStr"/>
+      <c r="T62" t="n">
+        <v>4.72</v>
+      </c>
       <c r="U62" t="n">
         <v>315</v>
       </c>
@@ -6741,7 +6759,9 @@
         <v>14483.76</v>
       </c>
       <c r="S63" t="inlineStr"/>
-      <c r="T63" t="inlineStr"/>
+      <c r="T63" t="n">
+        <v>0.52</v>
+      </c>
       <c r="U63" t="n">
         <v>3000</v>
       </c>
@@ -6848,7 +6868,9 @@
         <v>14483.76</v>
       </c>
       <c r="S64" t="inlineStr"/>
-      <c r="T64" t="inlineStr"/>
+      <c r="T64" t="n">
+        <v>0.52</v>
+      </c>
       <c r="U64" t="n">
         <v>3000</v>
       </c>
@@ -6955,7 +6977,9 @@
         <v>19065.23</v>
       </c>
       <c r="S65" t="inlineStr"/>
-      <c r="T65" t="inlineStr"/>
+      <c r="T65" t="n">
+        <v>0.74</v>
+      </c>
       <c r="U65" t="n">
         <v>2640</v>
       </c>
@@ -7062,7 +7086,9 @@
         <v>3176.44</v>
       </c>
       <c r="S66" t="inlineStr"/>
-      <c r="T66" t="inlineStr"/>
+      <c r="T66" t="n">
+        <v>1.53</v>
+      </c>
       <c r="U66" t="n">
         <v>256.71</v>
       </c>
@@ -7169,7 +7195,9 @@
         <v>14483.76</v>
       </c>
       <c r="S67" t="inlineStr"/>
-      <c r="T67" t="inlineStr"/>
+      <c r="T67" t="n">
+        <v>0.52</v>
+      </c>
       <c r="U67" t="n">
         <v>3000</v>
       </c>
@@ -7276,7 +7304,9 @@
         <v>1160.78</v>
       </c>
       <c r="S68" t="inlineStr"/>
-      <c r="T68" t="inlineStr"/>
+      <c r="T68" t="n">
+        <v>0.92</v>
+      </c>
       <c r="U68" t="n">
         <v>76.92</v>
       </c>
@@ -7383,7 +7413,9 @@
         <v>161.49</v>
       </c>
       <c r="S69" t="inlineStr"/>
-      <c r="T69" t="inlineStr"/>
+      <c r="T69" t="n">
+        <v>0.32</v>
+      </c>
       <c r="U69" t="n">
         <v>8.460000000000001</v>
       </c>
@@ -7490,7 +7522,9 @@
         <v>11597.99</v>
       </c>
       <c r="S70" t="inlineStr"/>
-      <c r="T70" t="inlineStr"/>
+      <c r="T70" t="n">
+        <v>0.5</v>
+      </c>
       <c r="U70" t="n">
         <v>2490</v>
       </c>
@@ -7597,7 +7631,9 @@
         <v>1515.66</v>
       </c>
       <c r="S71" t="inlineStr"/>
-      <c r="T71" t="inlineStr"/>
+      <c r="T71" t="n">
+        <v>1.2</v>
+      </c>
       <c r="U71" t="n">
         <v>418.93</v>
       </c>
@@ -7704,7 +7740,9 @@
         <v>14483.76</v>
       </c>
       <c r="S72" t="inlineStr"/>
-      <c r="T72" t="inlineStr"/>
+      <c r="T72" t="n">
+        <v>0.52</v>
+      </c>
       <c r="U72" t="n">
         <v>3000</v>
       </c>
@@ -7811,7 +7849,9 @@
         <v>14483.76</v>
       </c>
       <c r="S73" t="inlineStr"/>
-      <c r="T73" t="inlineStr"/>
+      <c r="T73" t="n">
+        <v>0.52</v>
+      </c>
       <c r="U73" t="n">
         <v>3000</v>
       </c>
@@ -7918,7 +7958,9 @@
         <v>1120.83</v>
       </c>
       <c r="S74" t="inlineStr"/>
-      <c r="T74" t="inlineStr"/>
+      <c r="T74" t="n">
+        <v>1.12</v>
+      </c>
       <c r="U74" t="n">
         <v>167.46</v>
       </c>
@@ -8025,7 +8067,9 @@
         <v>14483.76</v>
       </c>
       <c r="S75" t="inlineStr"/>
-      <c r="T75" t="inlineStr"/>
+      <c r="T75" t="n">
+        <v>0.52</v>
+      </c>
       <c r="U75" t="n">
         <v>3000</v>
       </c>
@@ -8132,7 +8176,9 @@
         <v>3360.06</v>
       </c>
       <c r="S76" t="inlineStr"/>
-      <c r="T76" t="inlineStr"/>
+      <c r="T76" t="n">
+        <v>2.67</v>
+      </c>
       <c r="U76" t="n">
         <v>2287.89</v>
       </c>
@@ -8239,7 +8285,9 @@
         <v>5717.96</v>
       </c>
       <c r="S77" t="inlineStr"/>
-      <c r="T77" t="inlineStr"/>
+      <c r="T77" t="n">
+        <v>0.73</v>
+      </c>
       <c r="U77" t="n">
         <v>2170</v>
       </c>
@@ -8346,7 +8394,9 @@
         <v>14483.76</v>
       </c>
       <c r="S78" t="inlineStr"/>
-      <c r="T78" t="inlineStr"/>
+      <c r="T78" t="n">
+        <v>0.52</v>
+      </c>
       <c r="U78" t="n">
         <v>3000</v>
       </c>
@@ -8453,7 +8503,9 @@
         <v>14483.76</v>
       </c>
       <c r="S79" t="inlineStr"/>
-      <c r="T79" t="inlineStr"/>
+      <c r="T79" t="n">
+        <v>0.52</v>
+      </c>
       <c r="U79" t="n">
         <v>3000</v>
       </c>
@@ -8560,7 +8612,9 @@
         <v>6.9</v>
       </c>
       <c r="S80" t="inlineStr"/>
-      <c r="T80" t="inlineStr"/>
+      <c r="T80" t="n">
+        <v>11.31</v>
+      </c>
       <c r="U80" t="n">
         <v>6.52</v>
       </c>
@@ -8667,7 +8721,9 @@
         <v>6.9</v>
       </c>
       <c r="S81" t="inlineStr"/>
-      <c r="T81" t="inlineStr"/>
+      <c r="T81" t="n">
+        <v>11.31</v>
+      </c>
       <c r="U81" t="n">
         <v>6.52</v>
       </c>
@@ -8774,7 +8830,9 @@
         <v>7.04</v>
       </c>
       <c r="S82" t="inlineStr"/>
-      <c r="T82" t="inlineStr"/>
+      <c r="T82" t="n">
+        <v>11.36</v>
+      </c>
       <c r="U82" t="n">
         <v>6.52</v>
       </c>
@@ -8881,7 +8939,9 @@
         <v>9075.43</v>
       </c>
       <c r="S83" t="inlineStr"/>
-      <c r="T83" t="inlineStr"/>
+      <c r="T83" t="n">
+        <v>0.41</v>
+      </c>
       <c r="U83" t="n">
         <v>1884.66</v>
       </c>
@@ -8988,7 +9048,9 @@
         <v>405.17</v>
       </c>
       <c r="S84" t="inlineStr"/>
-      <c r="T84" t="inlineStr"/>
+      <c r="T84" t="n">
+        <v>0.41</v>
+      </c>
       <c r="U84" t="n">
         <v>84.14</v>
       </c>
@@ -9095,7 +9157,9 @@
         <v>14363.79</v>
       </c>
       <c r="S85" t="inlineStr"/>
-      <c r="T85" t="inlineStr"/>
+      <c r="T85" t="n">
+        <v>0.51</v>
+      </c>
       <c r="U85" t="n">
         <v>2880</v>
       </c>
@@ -9202,7 +9266,9 @@
         <v>14363.79</v>
       </c>
       <c r="S86" t="inlineStr"/>
-      <c r="T86" t="inlineStr"/>
+      <c r="T86" t="n">
+        <v>0.51</v>
+      </c>
       <c r="U86" t="n">
         <v>2880</v>
       </c>
@@ -9309,7 +9375,9 @@
         <v>14363.79</v>
       </c>
       <c r="S87" t="inlineStr"/>
-      <c r="T87" t="inlineStr"/>
+      <c r="T87" t="n">
+        <v>0.51</v>
+      </c>
       <c r="U87" t="n">
         <v>2880</v>
       </c>
@@ -9416,7 +9484,9 @@
         <v>205.89</v>
       </c>
       <c r="S88" t="inlineStr"/>
-      <c r="T88" t="inlineStr"/>
+      <c r="T88" t="n">
+        <v>0.51</v>
+      </c>
       <c r="U88" t="n">
         <v>4.84</v>
       </c>
@@ -9523,7 +9593,9 @@
         <v>14363.79</v>
       </c>
       <c r="S89" t="inlineStr"/>
-      <c r="T89" t="inlineStr"/>
+      <c r="T89" t="n">
+        <v>0.51</v>
+      </c>
       <c r="U89" t="n">
         <v>2880</v>
       </c>
@@ -9630,7 +9702,9 @@
         <v>14363.79</v>
       </c>
       <c r="S90" t="inlineStr"/>
-      <c r="T90" t="inlineStr"/>
+      <c r="T90" t="n">
+        <v>0.51</v>
+      </c>
       <c r="U90" t="n">
         <v>2880</v>
       </c>
@@ -9737,7 +9811,9 @@
         <v>14363.79</v>
       </c>
       <c r="S91" t="inlineStr"/>
-      <c r="T91" t="inlineStr"/>
+      <c r="T91" t="n">
+        <v>0.51</v>
+      </c>
       <c r="U91" t="n">
         <v>2880</v>
       </c>
@@ -9844,7 +9920,9 @@
         <v>9639.08</v>
       </c>
       <c r="S92" t="inlineStr"/>
-      <c r="T92" t="inlineStr"/>
+      <c r="T92" t="n">
+        <v>0.42</v>
+      </c>
       <c r="U92" t="n">
         <v>1120</v>
       </c>
@@ -9951,7 +10029,9 @@
         <v>665.09</v>
       </c>
       <c r="S93" t="inlineStr"/>
-      <c r="T93" t="inlineStr"/>
+      <c r="T93" t="n">
+        <v>110.85</v>
+      </c>
       <c r="U93" t="n">
         <v>42.84</v>
       </c>
@@ -10058,7 +10138,9 @@
         <v>21.7</v>
       </c>
       <c r="S94" t="inlineStr"/>
-      <c r="T94" t="inlineStr"/>
+      <c r="T94" t="n">
+        <v>43.39</v>
+      </c>
       <c r="U94" t="n">
         <v>12.46</v>
       </c>
@@ -10165,7 +10247,9 @@
         <v>23852.44</v>
       </c>
       <c r="S95" t="inlineStr"/>
-      <c r="T95" t="inlineStr"/>
+      <c r="T95" t="n">
+        <v>2.76</v>
+      </c>
       <c r="U95" t="n">
         <v>4562</v>
       </c>
@@ -10272,7 +10356,9 @@
         <v>411.78</v>
       </c>
       <c r="S96" t="inlineStr"/>
-      <c r="T96" t="inlineStr"/>
+      <c r="T96" t="n">
+        <v>0.51</v>
+      </c>
       <c r="U96" t="n">
         <v>9.68</v>
       </c>
@@ -10379,7 +10465,9 @@
         <v>8173.42</v>
       </c>
       <c r="S97" t="inlineStr"/>
-      <c r="T97" t="inlineStr"/>
+      <c r="T97" t="n">
+        <v>0.49</v>
+      </c>
       <c r="U97" t="n">
         <v>1006.31</v>
       </c>
@@ -10486,7 +10574,9 @@
         <v>18660.06</v>
       </c>
       <c r="S98" t="inlineStr"/>
-      <c r="T98" t="inlineStr"/>
+      <c r="T98" t="n">
+        <v>2.05</v>
+      </c>
       <c r="U98" t="n">
         <v>4060</v>
       </c>
@@ -10593,7 +10683,9 @@
         <v>36.93</v>
       </c>
       <c r="S99" t="inlineStr"/>
-      <c r="T99" t="inlineStr"/>
+      <c r="T99" t="n">
+        <v>9.23</v>
+      </c>
       <c r="U99" t="n">
         <v>35.98</v>
       </c>

</xml_diff>